<commit_message>
0.0.2 : Component shall be exported with default. Implement directory will trail package directory.
</commit_message>
<xml_diff>
--- a/meta/components/BoxSample.xlsx
+++ b/meta/components/BoxSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVueComponent/meta/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9469AE5-97B1-0F4C-BA23-D26E749AA9BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72804F7E-F567-F749-9EBF-51A9BB92A9BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13200" yWindow="2260" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -610,7 +610,7 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>@/views/boxSample</t>
+    <t>@</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1367,6 +1367,24 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1380,24 +1398,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1812,7 +1812,7 @@
   </sheetPr>
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13:E13"/>
     </sheetView>
   </sheetViews>
@@ -1903,10 +1903,10 @@
       <c r="H8" s="35"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="87" t="s">
+      <c r="A9" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="88"/>
+      <c r="B9" s="94"/>
       <c r="C9" s="10" t="s">
         <v>80</v>
       </c>
@@ -1919,10 +1919,10 @@
       <c r="H9" s="35"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="87" t="s">
+      <c r="A10" s="93" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="88"/>
+      <c r="B10" s="94"/>
       <c r="C10" s="10" t="s">
         <v>81</v>
       </c>
@@ -1935,10 +1935,10 @@
       <c r="H10" s="35"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="87" t="s">
+      <c r="A11" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="88"/>
+      <c r="B11" s="94"/>
       <c r="C11" s="10" t="s">
         <v>22</v>
       </c>
@@ -1951,10 +1951,10 @@
       <c r="H11" s="35"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="87" t="s">
+      <c r="A12" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="88"/>
+      <c r="B12" s="94"/>
       <c r="C12" s="86" t="s">
         <v>82</v>
       </c>
@@ -1971,11 +1971,11 @@
         <v>1</v>
       </c>
       <c r="B13" s="6"/>
-      <c r="C13" s="89" t="s">
+      <c r="C13" s="95" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="90"/>
-      <c r="E13" s="91"/>
+      <c r="D13" s="96"/>
+      <c r="E13" s="97"/>
       <c r="F13" s="65"/>
       <c r="G13" s="65"/>
       <c r="H13" s="34"/>
@@ -2077,10 +2077,10 @@
       <c r="H19"/>
     </row>
     <row r="20" spans="1:12" s="32" customFormat="1">
-      <c r="A20" s="92" t="s">
+      <c r="A20" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="93"/>
+      <c r="B20" s="88"/>
       <c r="C20" s="64" t="s">
         <v>15</v>
       </c>
@@ -2107,10 +2107,10 @@
       <c r="H21"/>
     </row>
     <row r="22" spans="1:12" s="32" customFormat="1">
-      <c r="A22" s="92" t="s">
+      <c r="A22" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="93"/>
+      <c r="B22" s="88"/>
       <c r="C22" s="64" t="s">
         <v>15</v>
       </c>
@@ -2446,45 +2446,45 @@
       <c r="L43" s="15"/>
     </row>
     <row r="44" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A44" s="95" t="s">
+      <c r="A44" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="B44" s="95" t="s">
+      <c r="B44" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="C44" s="94" t="s">
+      <c r="C44" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="94" t="s">
+      <c r="D44" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="E44" s="94" t="s">
+      <c r="E44" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="F44" s="96" t="s">
+      <c r="F44" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="G44" s="96" t="s">
+      <c r="G44" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="H44" s="94" t="s">
+      <c r="H44" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="I44" s="94"/>
+      <c r="I44" s="89"/>
       <c r="J44" s="16"/>
       <c r="K44" s="17"/>
       <c r="L44" s="9"/>
     </row>
     <row r="45" spans="1:12">
-      <c r="A45" s="95"/>
-      <c r="B45" s="95"/>
-      <c r="C45" s="94"/>
-      <c r="D45" s="94"/>
-      <c r="E45" s="94"/>
-      <c r="F45" s="97"/>
-      <c r="G45" s="97"/>
-      <c r="H45" s="94"/>
-      <c r="I45" s="94"/>
+      <c r="A45" s="90"/>
+      <c r="B45" s="90"/>
+      <c r="C45" s="89"/>
+      <c r="D45" s="89"/>
+      <c r="E45" s="89"/>
+      <c r="F45" s="92"/>
+      <c r="G45" s="92"/>
+      <c r="H45" s="89"/>
+      <c r="I45" s="89"/>
       <c r="J45" s="18"/>
       <c r="K45" s="29"/>
       <c r="L45" s="15"/>
@@ -2829,6 +2829,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C13:E13"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H44:I45"/>
@@ -2839,11 +2844,6 @@
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="G44:G45"/>
     <mergeCell ref="F44:F45"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C13:E13"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="5">

</xml_diff>

<commit_message>
0.1.2: Implement expectConsistentAfterTransition flag.
</commit_message>
<xml_diff>
--- a/meta/components/BoxSample.xlsx
+++ b/meta/components/BoxSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVueComponent/meta/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72804F7E-F567-F749-9EBF-51A9BB92A9BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417A40FE-518D-384B-945F-BDCE9859E04E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13200" yWindow="2260" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="84">
   <si>
     <t>パッケージ</t>
   </si>
@@ -612,6 +612,16 @@
   <si>
     <t>@</t>
     <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>遷移後の参照に一貫性を期待</t>
+    <rPh sb="6" eb="7">
+      <t xml:space="preserve">ブｎ </t>
+    </rPh>
+    <rPh sb="8" eb="12">
+      <t xml:space="preserve">ジドウセイセイ </t>
+    </rPh>
+    <phoneticPr fontId="6"/>
   </si>
 </sst>
 </file>
@@ -1367,6 +1377,21 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1383,21 +1408,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1810,10 +1820,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L63"/>
+  <dimension ref="A1:L64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:E13"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1903,10 +1913,10 @@
       <c r="H8" s="35"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="93" t="s">
+      <c r="A9" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="94"/>
+      <c r="B9" s="88"/>
       <c r="C9" s="10" t="s">
         <v>80</v>
       </c>
@@ -1919,10 +1929,10 @@
       <c r="H9" s="35"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="93" t="s">
+      <c r="A10" s="87" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="94"/>
+      <c r="B10" s="88"/>
       <c r="C10" s="10" t="s">
         <v>81</v>
       </c>
@@ -1935,10 +1945,10 @@
       <c r="H10" s="35"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="93" t="s">
+      <c r="A11" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="94"/>
+      <c r="B11" s="88"/>
       <c r="C11" s="10" t="s">
         <v>22</v>
       </c>
@@ -1951,10 +1961,10 @@
       <c r="H11" s="35"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="93" t="s">
+      <c r="A12" s="87" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="94"/>
+      <c r="B12" s="88"/>
       <c r="C12" s="86" t="s">
         <v>82</v>
       </c>
@@ -1971,11 +1981,11 @@
         <v>1</v>
       </c>
       <c r="B13" s="6"/>
-      <c r="C13" s="95" t="s">
+      <c r="C13" s="89" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="96"/>
-      <c r="E13" s="97"/>
+      <c r="D13" s="90"/>
+      <c r="E13" s="91"/>
       <c r="F13" s="65"/>
       <c r="G13" s="65"/>
       <c r="H13" s="34"/>
@@ -2077,10 +2087,10 @@
       <c r="H19"/>
     </row>
     <row r="20" spans="1:12" s="32" customFormat="1">
-      <c r="A20" s="87" t="s">
+      <c r="A20" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="88"/>
+      <c r="B20" s="93"/>
       <c r="C20" s="64" t="s">
         <v>15</v>
       </c>
@@ -2107,10 +2117,10 @@
       <c r="H21"/>
     </row>
     <row r="22" spans="1:12" s="32" customFormat="1">
-      <c r="A22" s="87" t="s">
+      <c r="A22" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="88"/>
+      <c r="B22" s="93"/>
       <c r="C22" s="64" t="s">
         <v>15</v>
       </c>
@@ -2122,78 +2132,78 @@
       <c r="G22" s="66"/>
       <c r="H22"/>
     </row>
-    <row r="23" spans="1:12" s="37" customFormat="1">
-      <c r="A23" s="34"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="30" t="s">
+    <row r="23" spans="1:12" s="32" customFormat="1">
+      <c r="A23" s="92" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="93"/>
+      <c r="C23" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23" s="66"/>
+      <c r="H23"/>
+    </row>
+    <row r="24" spans="1:12" s="37" customFormat="1">
+      <c r="A24" s="34"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="81"/>
-      <c r="F24" s="44" t="s">
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="81"/>
+      <c r="F25" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="G24" s="44"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="43"/>
-      <c r="L24" s="43"/>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="47" t="s">
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="43"/>
+      <c r="L25" s="43"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="42" t="s">
+      <c r="B26" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="82"/>
-      <c r="F25" s="67"/>
-      <c r="G25" s="67"/>
-      <c r="H25" s="67"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="45"/>
-      <c r="K25" s="45"/>
-      <c r="L25" s="35"/>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="51">
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="82"/>
+      <c r="F26" s="67"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="67"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="35"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="51">
         <v>1</v>
       </c>
-      <c r="B26" s="46" t="s">
+      <c r="B27" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="68"/>
-      <c r="G26" s="68"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="36"/>
-      <c r="K26" s="36"/>
-      <c r="L26" s="35"/>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="51"/>
-      <c r="B27" s="46"/>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="41"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="39"/>
       <c r="F27" s="68"/>
       <c r="G27" s="68"/>
       <c r="H27" s="34"/>
@@ -2203,11 +2213,11 @@
       <c r="L27" s="35"/>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="52"/>
-      <c r="B28" s="48"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="50"/>
+      <c r="A28" s="51"/>
+      <c r="B28" s="46"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="41"/>
       <c r="F28" s="68"/>
       <c r="G28" s="68"/>
       <c r="H28" s="34"/>
@@ -2217,72 +2227,72 @@
       <c r="L28" s="35"/>
     </row>
     <row r="29" spans="1:12">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
+      <c r="A29" s="52"/>
+      <c r="B29" s="48"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="68"/>
+      <c r="G29" s="68"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="35"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="81"/>
-      <c r="F30" s="44" t="s">
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="81"/>
+      <c r="F31" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="43"/>
-      <c r="J30" s="43"/>
-      <c r="K30" s="43"/>
-      <c r="L30" s="43"/>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31" s="47" t="s">
+      <c r="G31" s="44"/>
+      <c r="H31" s="44"/>
+      <c r="I31" s="43"/>
+      <c r="J31" s="43"/>
+      <c r="K31" s="43"/>
+      <c r="L31" s="43"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="42" t="s">
+      <c r="B32" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="82"/>
-      <c r="F31" s="67"/>
-      <c r="G31" s="67"/>
-      <c r="H31" s="67"/>
-      <c r="I31" s="44"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="45"/>
-      <c r="L31" s="35"/>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="A32" s="51"/>
-      <c r="B32" s="46"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="68"/>
-      <c r="G32" s="68"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="36"/>
-      <c r="K32" s="36"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="82"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="67"/>
+      <c r="H32" s="67"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="45"/>
+      <c r="K32" s="45"/>
       <c r="L32" s="35"/>
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="51"/>
       <c r="B33" s="46"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="41"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="39"/>
       <c r="F33" s="68"/>
       <c r="G33" s="68"/>
       <c r="H33" s="34"/>
@@ -2292,11 +2302,11 @@
       <c r="L33" s="35"/>
     </row>
     <row r="34" spans="1:12">
-      <c r="A34" s="52"/>
-      <c r="B34" s="48"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="49"/>
-      <c r="E34" s="50"/>
+      <c r="A34" s="51"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="41"/>
       <c r="F34" s="68"/>
       <c r="G34" s="68"/>
       <c r="H34" s="34"/>
@@ -2306,80 +2316,76 @@
       <c r="L34" s="35"/>
     </row>
     <row r="35" spans="1:12">
-      <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
+      <c r="A35" s="52"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="68"/>
+      <c r="G35" s="68"/>
+      <c r="H35" s="34"/>
+      <c r="I35" s="36"/>
+      <c r="J35" s="36"/>
+      <c r="K35" s="36"/>
+      <c r="L35" s="35"/>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="30" t="s">
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="81"/>
-      <c r="F36" s="44" t="s">
+      <c r="B37" s="31"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="81"/>
+      <c r="F37" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="G36" s="44"/>
-      <c r="H36" s="44"/>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
-      <c r="K36" s="43"/>
-      <c r="L36" s="43"/>
-    </row>
-    <row r="37" spans="1:12">
-      <c r="A37" s="47" t="s">
+      <c r="G37" s="44"/>
+      <c r="H37" s="44"/>
+      <c r="I37" s="43"/>
+      <c r="J37" s="43"/>
+      <c r="K37" s="43"/>
+      <c r="L37" s="43"/>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="42" t="s">
+      <c r="B38" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="42"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="82"/>
-      <c r="F37" s="67"/>
-      <c r="G37" s="67"/>
-      <c r="H37" s="67"/>
-      <c r="I37" s="44"/>
-      <c r="J37" s="45"/>
-      <c r="K37" s="45"/>
-      <c r="L37" s="35"/>
-    </row>
-    <row r="38" spans="1:12">
-      <c r="A38" s="51">
-        <v>1</v>
-      </c>
-      <c r="B38" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="C38" s="38"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="39"/>
-      <c r="F38" s="68"/>
-      <c r="G38" s="68"/>
-      <c r="H38" s="34"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="36"/>
-      <c r="K38" s="36"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="82"/>
+      <c r="F38" s="67"/>
+      <c r="G38" s="67"/>
+      <c r="H38" s="67"/>
+      <c r="I38" s="44"/>
+      <c r="J38" s="45"/>
+      <c r="K38" s="45"/>
       <c r="L38" s="35"/>
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B39" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="C39" s="40"/>
-      <c r="D39" s="40"/>
-      <c r="E39" s="41"/>
+        <v>72</v>
+      </c>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="39"/>
       <c r="F39" s="68"/>
       <c r="G39" s="68"/>
       <c r="H39" s="34"/>
@@ -2389,11 +2395,15 @@
       <c r="L39" s="35"/>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="52"/>
-      <c r="B40" s="48"/>
-      <c r="C40" s="49"/>
-      <c r="D40" s="49"/>
-      <c r="E40" s="50"/>
+      <c r="A40" s="51">
+        <v>2</v>
+      </c>
+      <c r="B40" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="40"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="41"/>
       <c r="F40" s="68"/>
       <c r="G40" s="68"/>
       <c r="H40" s="34"/>
@@ -2403,11 +2413,11 @@
       <c r="L40" s="35"/>
     </row>
     <row r="41" spans="1:12">
-      <c r="A41" s="83"/>
-      <c r="B41" s="84"/>
-      <c r="C41" s="85"/>
-      <c r="D41" s="85"/>
-      <c r="E41" s="85"/>
+      <c r="A41" s="52"/>
+      <c r="B41" s="48"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="49"/>
+      <c r="E41" s="50"/>
       <c r="F41" s="68"/>
       <c r="G41" s="68"/>
       <c r="H41" s="34"/>
@@ -2417,123 +2427,112 @@
       <c r="L41" s="35"/>
     </row>
     <row r="42" spans="1:12">
-      <c r="A42" s="13"/>
-      <c r="B42" s="13" t="s">
+      <c r="A42" s="83"/>
+      <c r="B42" s="84"/>
+      <c r="C42" s="85"/>
+      <c r="D42" s="85"/>
+      <c r="E42" s="85"/>
+      <c r="F42" s="68"/>
+      <c r="G42" s="68"/>
+      <c r="H42" s="34"/>
+      <c r="I42" s="36"/>
+      <c r="J42" s="36"/>
+      <c r="K42" s="36"/>
+      <c r="L42" s="35"/>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="13"/>
+      <c r="B43" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-    </row>
-    <row r="43" spans="1:12">
-      <c r="A43" s="3" t="s">
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="6"/>
-      <c r="L43" s="15"/>
-    </row>
-    <row r="44" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A44" s="90" t="s">
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="14"/>
+      <c r="K44" s="6"/>
+      <c r="L44" s="15"/>
+    </row>
+    <row r="45" spans="1:12" ht="13.5" customHeight="1">
+      <c r="A45" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="B44" s="90" t="s">
+      <c r="B45" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="C44" s="89" t="s">
+      <c r="C45" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="89" t="s">
+      <c r="D45" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="E44" s="89" t="s">
+      <c r="E45" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="F44" s="91" t="s">
+      <c r="F45" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="G44" s="91" t="s">
+      <c r="G45" s="96" t="s">
         <v>17</v>
       </c>
-      <c r="H44" s="89" t="s">
+      <c r="H45" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="I44" s="89"/>
-      <c r="J44" s="16"/>
-      <c r="K44" s="17"/>
-      <c r="L44" s="9"/>
-    </row>
-    <row r="45" spans="1:12">
-      <c r="A45" s="90"/>
-      <c r="B45" s="90"/>
-      <c r="C45" s="89"/>
-      <c r="D45" s="89"/>
-      <c r="E45" s="89"/>
-      <c r="F45" s="92"/>
-      <c r="G45" s="92"/>
-      <c r="H45" s="89"/>
-      <c r="I45" s="89"/>
-      <c r="J45" s="18"/>
-      <c r="K45" s="29"/>
-      <c r="L45" s="15"/>
+      <c r="I45" s="94"/>
+      <c r="J45" s="16"/>
+      <c r="K45" s="17"/>
+      <c r="L45" s="9"/>
     </row>
     <row r="46" spans="1:12">
-      <c r="A46" s="19">
-        <v>1</v>
-      </c>
-      <c r="B46" s="71" t="s">
-        <v>57</v>
-      </c>
-      <c r="C46" s="78" t="s">
-        <v>58</v>
-      </c>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="F46" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="G46" s="69"/>
-      <c r="H46" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
-      <c r="K46" s="28"/>
+      <c r="A46" s="95"/>
+      <c r="B46" s="95"/>
+      <c r="C46" s="94"/>
+      <c r="D46" s="94"/>
+      <c r="E46" s="94"/>
+      <c r="F46" s="97"/>
+      <c r="G46" s="97"/>
+      <c r="H46" s="94"/>
+      <c r="I46" s="94"/>
+      <c r="J46" s="18"/>
+      <c r="K46" s="29"/>
       <c r="L46" s="15"/>
     </row>
     <row r="47" spans="1:12">
       <c r="A47" s="19">
-        <f>A46+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B47" s="71" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C47" s="78" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D47" s="20"/>
-      <c r="E47" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="F47" s="20"/>
+      <c r="E47" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="F47" s="20" t="s">
+        <v>15</v>
+      </c>
       <c r="G47" s="69"/>
       <c r="H47" s="20" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I47" s="21"/>
       <c r="J47" s="21"/>
@@ -2542,50 +2541,50 @@
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="19">
-        <f t="shared" ref="A48:A62" si="0">A47+1</f>
-        <v>3</v>
-      </c>
-      <c r="B48" s="72" t="s">
-        <v>63</v>
-      </c>
-      <c r="C48" s="79" t="s">
-        <v>64</v>
-      </c>
-      <c r="D48" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="E48" s="20"/>
+        <f>A47+1</f>
+        <v>2</v>
+      </c>
+      <c r="B48" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="C48" s="78" t="s">
+        <v>61</v>
+      </c>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20" t="b">
+        <v>1</v>
+      </c>
       <c r="F48" s="20"/>
-      <c r="G48" s="69" t="s">
-        <v>15</v>
-      </c>
+      <c r="G48" s="69"/>
       <c r="H48" s="20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I48" s="21"/>
       <c r="J48" s="21"/>
-      <c r="K48" s="22"/>
+      <c r="K48" s="28"/>
       <c r="L48" s="15"/>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="19">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B49" s="73" t="s">
-        <v>70</v>
-      </c>
-      <c r="C49" s="80" t="s">
+        <f t="shared" ref="A49:A63" si="0">A48+1</f>
+        <v>3</v>
+      </c>
+      <c r="B49" s="72" t="s">
+        <v>63</v>
+      </c>
+      <c r="C49" s="79" t="s">
+        <v>64</v>
+      </c>
+      <c r="D49" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="D49" s="20"/>
       <c r="E49" s="20"/>
       <c r="F49" s="20"/>
       <c r="G49" s="69" t="s">
         <v>15</v>
       </c>
       <c r="H49" s="20" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I49" s="21"/>
       <c r="J49" s="21"/>
@@ -2595,15 +2594,23 @@
     <row r="50" spans="1:12">
       <c r="A50" s="19">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B50" s="73"/>
-      <c r="C50" s="80"/>
+        <v>4</v>
+      </c>
+      <c r="B50" s="73" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="80" t="s">
+        <v>65</v>
+      </c>
       <c r="D50" s="20"/>
       <c r="E50" s="20"/>
       <c r="F50" s="20"/>
-      <c r="G50" s="69"/>
-      <c r="H50" s="20"/>
+      <c r="G50" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="H50" s="20" t="s">
+        <v>71</v>
+      </c>
       <c r="I50" s="21"/>
       <c r="J50" s="21"/>
       <c r="K50" s="22"/>
@@ -2612,58 +2619,58 @@
     <row r="51" spans="1:12">
       <c r="A51" s="19">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B51" s="73"/>
       <c r="C51" s="80"/>
-      <c r="D51" s="74"/>
-      <c r="E51" s="74"/>
-      <c r="F51" s="74"/>
-      <c r="G51" s="75"/>
-      <c r="H51" s="74"/>
-      <c r="I51" s="76"/>
-      <c r="J51" s="76"/>
-      <c r="K51" s="77"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="69"/>
+      <c r="H51" s="20"/>
+      <c r="I51" s="21"/>
+      <c r="J51" s="21"/>
+      <c r="K51" s="22"/>
       <c r="L51" s="15"/>
     </row>
     <row r="52" spans="1:12">
       <c r="A52" s="19">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B52" s="73"/>
       <c r="C52" s="80"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
-      <c r="G52" s="69"/>
-      <c r="H52" s="20"/>
-      <c r="I52" s="21"/>
-      <c r="J52" s="21"/>
-      <c r="K52" s="22"/>
+      <c r="D52" s="74"/>
+      <c r="E52" s="74"/>
+      <c r="F52" s="74"/>
+      <c r="G52" s="75"/>
+      <c r="H52" s="74"/>
+      <c r="I52" s="76"/>
+      <c r="J52" s="76"/>
+      <c r="K52" s="77"/>
       <c r="L52" s="15"/>
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="19">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B53" s="73"/>
       <c r="C53" s="80"/>
-      <c r="D53" s="74"/>
-      <c r="E53" s="74"/>
-      <c r="F53" s="74"/>
-      <c r="G53" s="75"/>
-      <c r="H53" s="74"/>
-      <c r="I53" s="76"/>
-      <c r="J53" s="76"/>
-      <c r="K53" s="77"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="69"/>
+      <c r="H53" s="20"/>
+      <c r="I53" s="21"/>
+      <c r="J53" s="21"/>
+      <c r="K53" s="22"/>
       <c r="L53" s="15"/>
     </row>
     <row r="54" spans="1:12">
       <c r="A54" s="19">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B54" s="73"/>
       <c r="C54" s="80"/>
@@ -2680,41 +2687,41 @@
     <row r="55" spans="1:12">
       <c r="A55" s="19">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B55" s="73"/>
       <c r="C55" s="80"/>
-      <c r="D55" s="20"/>
-      <c r="E55" s="20"/>
-      <c r="F55" s="20"/>
-      <c r="G55" s="69"/>
-      <c r="H55" s="20"/>
-      <c r="I55" s="21"/>
-      <c r="J55" s="21"/>
-      <c r="K55" s="22"/>
+      <c r="D55" s="74"/>
+      <c r="E55" s="74"/>
+      <c r="F55" s="74"/>
+      <c r="G55" s="75"/>
+      <c r="H55" s="74"/>
+      <c r="I55" s="76"/>
+      <c r="J55" s="76"/>
+      <c r="K55" s="77"/>
       <c r="L55" s="15"/>
     </row>
     <row r="56" spans="1:12">
       <c r="A56" s="19">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B56" s="73"/>
       <c r="C56" s="80"/>
-      <c r="D56" s="74"/>
-      <c r="E56" s="74"/>
-      <c r="F56" s="74"/>
-      <c r="G56" s="75"/>
-      <c r="H56" s="74"/>
-      <c r="I56" s="76"/>
-      <c r="J56" s="76"/>
-      <c r="K56" s="77"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="69"/>
+      <c r="H56" s="20"/>
+      <c r="I56" s="21"/>
+      <c r="J56" s="21"/>
+      <c r="K56" s="22"/>
       <c r="L56" s="15"/>
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="19">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B57" s="73"/>
       <c r="C57" s="80"/>
@@ -2731,41 +2738,41 @@
     <row r="58" spans="1:12">
       <c r="A58" s="19">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B58" s="73"/>
       <c r="C58" s="80"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="20"/>
-      <c r="F58" s="20"/>
-      <c r="G58" s="69"/>
-      <c r="H58" s="20"/>
-      <c r="I58" s="21"/>
-      <c r="J58" s="21"/>
-      <c r="K58" s="22"/>
+      <c r="D58" s="74"/>
+      <c r="E58" s="74"/>
+      <c r="F58" s="74"/>
+      <c r="G58" s="75"/>
+      <c r="H58" s="74"/>
+      <c r="I58" s="76"/>
+      <c r="J58" s="76"/>
+      <c r="K58" s="77"/>
       <c r="L58" s="15"/>
     </row>
     <row r="59" spans="1:12">
       <c r="A59" s="19">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B59" s="73"/>
       <c r="C59" s="80"/>
-      <c r="D59" s="74"/>
-      <c r="E59" s="74"/>
-      <c r="F59" s="74"/>
-      <c r="G59" s="75"/>
-      <c r="H59" s="74"/>
-      <c r="I59" s="76"/>
-      <c r="J59" s="76"/>
-      <c r="K59" s="77"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="69"/>
+      <c r="H59" s="20"/>
+      <c r="I59" s="21"/>
+      <c r="J59" s="21"/>
+      <c r="K59" s="22"/>
       <c r="L59" s="15"/>
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="19">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B60" s="73"/>
       <c r="C60" s="80"/>
@@ -2782,82 +2789,100 @@
     <row r="61" spans="1:12">
       <c r="A61" s="19">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B61" s="73"/>
       <c r="C61" s="80"/>
-      <c r="D61" s="20"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="20"/>
-      <c r="G61" s="69"/>
-      <c r="H61" s="20"/>
-      <c r="I61" s="21"/>
-      <c r="J61" s="21"/>
-      <c r="K61" s="22"/>
+      <c r="D61" s="74"/>
+      <c r="E61" s="74"/>
+      <c r="F61" s="74"/>
+      <c r="G61" s="75"/>
+      <c r="H61" s="74"/>
+      <c r="I61" s="76"/>
+      <c r="J61" s="76"/>
+      <c r="K61" s="77"/>
       <c r="L61" s="15"/>
     </row>
     <row r="62" spans="1:12">
       <c r="A62" s="19">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B62" s="73"/>
       <c r="C62" s="80"/>
-      <c r="D62" s="74"/>
-      <c r="E62" s="74"/>
-      <c r="F62" s="74"/>
-      <c r="G62" s="75"/>
-      <c r="H62" s="74"/>
-      <c r="I62" s="76"/>
-      <c r="J62" s="76"/>
-      <c r="K62" s="77"/>
+      <c r="D62" s="20"/>
+      <c r="E62" s="20"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="69"/>
+      <c r="H62" s="20"/>
+      <c r="I62" s="21"/>
+      <c r="J62" s="21"/>
+      <c r="K62" s="22"/>
       <c r="L62" s="15"/>
     </row>
     <row r="63" spans="1:12">
-      <c r="A63" s="23"/>
-      <c r="B63" s="24"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
-      <c r="F63" s="25"/>
-      <c r="G63" s="70"/>
-      <c r="H63" s="25"/>
-      <c r="I63" s="26"/>
-      <c r="J63" s="26"/>
-      <c r="K63" s="27"/>
+      <c r="A63" s="19">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B63" s="73"/>
+      <c r="C63" s="80"/>
+      <c r="D63" s="74"/>
+      <c r="E63" s="74"/>
+      <c r="F63" s="74"/>
+      <c r="G63" s="75"/>
+      <c r="H63" s="74"/>
+      <c r="I63" s="76"/>
+      <c r="J63" s="76"/>
+      <c r="K63" s="77"/>
       <c r="L63" s="15"/>
     </row>
+    <row r="64" spans="1:12">
+      <c r="A64" s="23"/>
+      <c r="B64" s="24"/>
+      <c r="C64" s="25"/>
+      <c r="D64" s="25"/>
+      <c r="E64" s="25"/>
+      <c r="F64" s="25"/>
+      <c r="G64" s="70"/>
+      <c r="H64" s="25"/>
+      <c r="I64" s="26"/>
+      <c r="J64" s="26"/>
+      <c r="K64" s="27"/>
+      <c r="L64" s="15"/>
+    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H45:I46"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="A23:B23"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C13:E13"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H44:I45"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="G44:G45"/>
-    <mergeCell ref="F44:F45"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E79:G79" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E80:G80" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C22" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C22:C23" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
       <formula1>adjustFiledName</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
       <formula1>componentKind</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F46:G63 C16:C20" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F47:G64 C16:C20" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>yesNo</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C21" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">

</xml_diff>

<commit_message>
Enable parser for vue3 adapted meta files. TODO: * Generate typescript codes from parsed informations.
</commit_message>
<xml_diff>
--- a/meta/components/BoxSample.xlsx
+++ b/meta/components/BoxSample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVueComponent/meta/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417A40FE-518D-384B-945F-BDCE9859E04E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF133BD0-B2AC-724D-B448-4DBDDE0D71BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13200" yWindow="2260" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1400" yWindow="1840" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VueComponent" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="118">
   <si>
     <t>パッケージ</t>
   </si>
@@ -84,10 +84,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>様式 ver 0.0.2 (2019.01.23)</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>No.</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -189,10 +185,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>Labels Class for i18n</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>1.Vueコンポーネント定義書は、blancoVueComponentが入力ファイルとして利用します。</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -204,10 +196,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>Vueコンポーネント定義・共通</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>コンポーネント名</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -246,13 +234,6 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>styleを使用</t>
-    <rPh sb="6" eb="8">
-      <t xml:space="preserve">シヨウ </t>
-    </rPh>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>templateを使用</t>
     <rPh sb="9" eb="11">
       <t xml:space="preserve">シヨウ </t>
@@ -267,26 +248,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>/* HTML形式。拡張子はhtmlです。 */</t>
-    <rPh sb="7" eb="9">
-      <t xml:space="preserve">ケイシキ </t>
-    </rPh>
-    <rPh sb="10" eb="13">
-      <t xml:space="preserve">カクチョウシハ </t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>/* scss形式。拡張子は scss です。 */</t>
-    <rPh sb="7" eb="9">
-      <t xml:space="preserve">ケイシキ </t>
-    </rPh>
-    <rPh sb="10" eb="13">
-      <t xml:space="preserve">カクチョウシハ </t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>Yes / No</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -307,17 +268,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>Vueコンポーネント定義・プロパティ</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Vueコンポーネント定義書 (Typescript専用)</t>
-    <rPh sb="25" eb="27">
-      <t xml:space="preserve">センヨウ </t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>必須</t>
     <rPh sb="0" eb="2">
       <t xml:space="preserve">ヒッス </t>
@@ -354,19 +304,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>※ このコンポーネントにプロパティを定義する場合はここに記述します</t>
-    <rPh sb="18" eb="20">
-      <t xml:space="preserve">テイギ </t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t xml:space="preserve">バアイハ </t>
-    </rPh>
-    <rPh sb="28" eb="30">
-      <t xml:space="preserve">キジュツ </t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>/* 当面の間、画面でのみ有効 */</t>
     <rPh sb="3" eb="5">
       <t xml:space="preserve">トウメｎ </t>
@@ -453,12 +390,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>Labels Class for i18n&lt;br&gt;
-改行も入れておく&lt;br&gt;
-いかが？</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>router-path</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -531,22 +462,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>/* 変数定義されます, i18n などと併用する場合は、ここにタグを記述します */</t>
-    <rPh sb="3" eb="7">
-      <t xml:space="preserve">ヘンスウテイギ </t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t xml:space="preserve">ヘイヨウスル </t>
-    </rPh>
-    <rPh sb="25" eb="27">
-      <t xml:space="preserve">バアイハ </t>
-    </rPh>
-    <rPh sb="35" eb="37">
-      <t xml:space="preserve">キジュツ </t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>prop04</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -566,39 +481,11 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>import { TitleHeader, BreadCrumbs } from "SampleComponents"</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Vueコンポーネント定義・ヘッダ情報（クラス用）</t>
-    <rPh sb="0" eb="18">
-      <t xml:space="preserve">ジョウホウ </t>
-    </rPh>
-    <rPh sb="22" eb="23">
-      <t xml:space="preserve">ヨウ </t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Vueコンポーネント定義・ヘッダ情報（インタフェイス用）</t>
-    <rPh sb="0" eb="18">
-      <t xml:space="preserve">ジョウホウ </t>
-    </rPh>
-    <rPh sb="26" eb="27">
-      <t xml:space="preserve">ヨウ </t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>ボックスサンプル</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>BoxSample</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>sample.views.boxSample</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -622,6 +509,486 @@
       <t xml:space="preserve">ジドウセイセイ </t>
     </rPh>
     <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>様式 ver 1.0.0 (2022.05.05)</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>コンポーネント名</t>
+    <rPh sb="7" eb="8">
+      <t xml:space="preserve">メイ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>/* nameプロパティに定義されます。一意な識別子となることを想定しています。 */</t>
+    <rPh sb="13" eb="15">
+      <t xml:space="preserve">ヘンスウテイギ </t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t xml:space="preserve">イチイナ </t>
+    </rPh>
+    <rPh sb="23" eb="26">
+      <t xml:space="preserve">シキベツシ </t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t xml:space="preserve">ソウテイ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>コンポーネント別名</t>
+    <rPh sb="7" eb="9">
+      <t xml:space="preserve">ベツメイ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>/* aliasプロパティに定義されます。Human readable な名前が記述されることを想定しています。 */</t>
+    <rPh sb="14" eb="16">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t xml:space="preserve">ナマエヲ </t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t xml:space="preserve">キジュツ </t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t xml:space="preserve">ソウテイ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>sample.pages.boxSample</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>/* プロジェクトの sample/pages/BoxSample ディレクトリに配置されます */</t>
+    <rPh sb="41" eb="43">
+      <t xml:space="preserve">ハイチ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Box画面のサンプルです。&lt;br&gt;
+改行も入れておく&lt;br&gt;
+いかが？</t>
+    <rPh sb="3" eb="5">
+      <t xml:space="preserve">ガメｎ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Box画面コンポーネントを定義します。</t>
+    <rPh sb="3" eb="4">
+      <t xml:space="preserve">ガメｎ </t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t xml:space="preserve">テイギシマス。 </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>/* HTML形式。拡張子はhtmlです。ここにチェックが無い場合はrender()関数の定義を強制されます。 */</t>
+    <rPh sb="7" eb="9">
+      <t xml:space="preserve">ケイシキ </t>
+    </rPh>
+    <rPh sb="10" eb="13">
+      <t xml:space="preserve">カクチョウシハ </t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t xml:space="preserve">ナイバアイハ </t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t xml:space="preserve">テイギヲ </t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t xml:space="preserve">キョウセイ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>/* setup関数を実装する場合はここにチェックを入れます。 */</t>
+    <rPh sb="8" eb="10">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t xml:space="preserve">ジッソウ </t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t xml:space="preserve">バアイハ </t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t xml:space="preserve">イレマス </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>/* data関数を実装する場合はここにチェックを入れます。 */</t>
+    <rPh sb="7" eb="9">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t xml:space="preserve">ジッソウ </t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t xml:space="preserve">バアイハ </t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t xml:space="preserve">イレマス </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>setup関数を実装する</t>
+    <rPh sb="5" eb="7">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t xml:space="preserve">ジッソウスル </t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>data関数を実装する</t>
+    <rPh sb="4" eb="6">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t xml:space="preserve">ジッソウスル </t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>※ このコンポーネントにプロパティを定義する場合はここに記述します。titleとaliasプロパティは強制的に定義されます。</t>
+    <rPh sb="18" eb="20">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t xml:space="preserve">バアイハ </t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t xml:space="preserve">キジュツ </t>
+    </rPh>
+    <rPh sb="51" eb="54">
+      <t xml:space="preserve">キョウセイテキニ </t>
+    </rPh>
+    <rPh sb="55" eb="57">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Vueコンポーネント定義・使用API</t>
+    <rPh sb="13" eb="15">
+      <t xml:space="preserve">シヨウ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>API名</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>クラス名</t>
+    <rPh sb="3" eb="4">
+      <t xml:space="preserve">メイ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>説明</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">セツメイ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>/* API呼び出しを使用する場合はここにAPIに関する情報を記述し、import 文をヘッダ情報に記述してください。 */</t>
+    <rPh sb="6" eb="7">
+      <t xml:space="preserve">ヨビダシ </t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t xml:space="preserve">シヨウスル </t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t xml:space="preserve">バアイハ </t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t xml:space="preserve">カンスル </t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t xml:space="preserve">ジョウホウ </t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t xml:space="preserve">キジュツシ </t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t xml:space="preserve">ブｎ </t>
+    </rPh>
+    <rPh sb="50" eb="52">
+      <t xml:space="preserve">キジュツ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>SampleApi</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>DummyApi</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ダミーAPIを呼び出します。</t>
+    <rPh sb="7" eb="8">
+      <t xml:space="preserve">ヨビダシマス。 </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>サンプルAPIを呼び出します。</t>
+    <rPh sb="8" eb="9">
+      <t xml:space="preserve">ヨビダシマス。 </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Vueコンポーネント定義・emits</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>イベント名</t>
+    <rPh sb="4" eb="5">
+      <t xml:space="preserve">メイ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>※ このコンポーネントにイベントを定義する場合はここに記述します。定義されたイベントはsetup関数からcontext.emit関数を呼び出す事で発火させることができます。</t>
+    <rPh sb="17" eb="19">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t xml:space="preserve">バアイハ </t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t xml:space="preserve">キジュツ </t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="64" eb="66">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="67" eb="68">
+      <t xml:space="preserve">ヨビダス </t>
+    </rPh>
+    <rPh sb="71" eb="72">
+      <t xml:space="preserve">コトデ </t>
+    </rPh>
+    <rPh sb="73" eb="75">
+      <t xml:space="preserve">ハッカ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ペイロード・型</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ペイロード・総称型</t>
+    <rPh sb="6" eb="8">
+      <t>ソウショウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>update:message</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>increment</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>number</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>/* subjectプロパティに定義されます, i18n などと併用する場合は、ここにタグを記述します */</t>
+    <rPh sb="16" eb="18">
+      <t xml:space="preserve">ヘンスウテイギ </t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t xml:space="preserve">ヘイヨウスル </t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t xml:space="preserve">バアイハ </t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t xml:space="preserve">キジュツ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Vueコンポーネント定義・ヘッダ情報（コンポーネント定義用）</t>
+    <rPh sb="0" eb="18">
+      <t xml:space="preserve">ジョウホウ </t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Vueコンポーネント定義・ヘッダ情報（使用API定義用）</t>
+    <rPh sb="0" eb="18">
+      <t xml:space="preserve">ジョウホウ </t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t xml:space="preserve">シヨウ </t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t xml:space="preserve">ヨウ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Vueコンポーネント定義書 (Typescript専用, Composition API 対応版)</t>
+    <rPh sb="25" eb="27">
+      <t xml:space="preserve">センヨウ </t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t xml:space="preserve">タイオウ </t>
+    </rPh>
+    <rPh sb="47" eb="48">
+      <t xml:space="preserve">バｎ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Vueコンポーネント定義・共通（Composition API用）</t>
+    <rPh sb="31" eb="32">
+      <t xml:space="preserve">ヨウ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Vueコンポーネント定義・ヘッダ情報（props定義用）</t>
+    <rPh sb="0" eb="18">
+      <t xml:space="preserve">ジョウホウ </t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t xml:space="preserve">ヨウ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Vueコンポーネント定義・props</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Vueコンポーネント定義・ヘッダ情報（emits定義用）</t>
+    <rPh sb="0" eb="18">
+      <t xml:space="preserve">ジョウホウ </t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t xml:space="preserve">ヨウ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>v-model:message イベントのペイロードの型を決定します。</t>
+    <rPh sb="27" eb="28">
+      <t xml:space="preserve">カタヲ </t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t xml:space="preserve">ケッテイ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>incrementイベントのペイロードの型を決定します。</t>
+    <rPh sb="20" eb="21">
+      <t xml:space="preserve">カタヲ </t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t xml:space="preserve">ケッテイシマス。 </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>notification</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>notificationイベントのペイロードの型を決定します。</t>
+    <rPh sb="23" eb="24">
+      <t xml:space="preserve">カタヲ </t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t xml:space="preserve">ケッテイシマス。 </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>/* 事前にblancoValueObjectTSで生成されたtmpディレクトリをbuild.gradleに記述しておくことで、import文が自動生成される場合があります。 */</t>
+    <rPh sb="3" eb="5">
+      <t xml:space="preserve">ジゼｎ </t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t xml:space="preserve">セイセイ </t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t xml:space="preserve">キジュツ </t>
+    </rPh>
+    <rPh sb="70" eb="71">
+      <t xml:space="preserve">ブｎ </t>
+    </rPh>
+    <rPh sb="72" eb="74">
+      <t xml:space="preserve">ジドウ </t>
+    </rPh>
+    <rPh sb="74" eb="76">
+      <t xml:space="preserve">セイセイ </t>
+    </rPh>
+    <rPh sb="79" eb="81">
+      <t xml:space="preserve">バアイガ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>import TitleHeader from "@/samples/pages/TitleHeader.vue"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>import BreadCrumbs from "@/samples/pages/BreadCrumbs.vue"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>import { DummyApi } from "@/smples/api/DummyApi"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>import { SmpleApi } from "@/smples/api/SampleApi"</t>
+    <phoneticPr fontId="3"/>
   </si>
 </sst>
 </file>
@@ -712,7 +1079,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -1217,12 +1584,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1377,6 +1789,24 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1391,23 +1821,25 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1820,10 +2252,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L64"/>
+  <dimension ref="A1:L96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1841,25 +2273,25 @@
   <sheetData>
     <row r="1" spans="1:10" ht="19">
       <c r="A1" s="2" t="s">
-        <v>40</v>
+        <v>104</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="3" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1870,170 +2302,174 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="3" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="8"/>
       <c r="F6" s="34" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G6" s="34"/>
       <c r="H6" s="35"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="7" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="34"/>
+      <c r="F7" s="34" t="s">
+        <v>101</v>
+      </c>
       <c r="G7" s="34"/>
       <c r="H7" s="35"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="3" t="s">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="34"/>
+      <c r="C8" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="34" t="s">
+        <v>73</v>
+      </c>
       <c r="G8" s="34"/>
       <c r="H8" s="35"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="87" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="88"/>
+      <c r="A9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="6"/>
       <c r="C9" s="10" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D9" s="33"/>
       <c r="E9" s="11"/>
       <c r="F9" s="34" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="G9" s="34"/>
       <c r="H9" s="35"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="87" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="88"/>
+      <c r="A10" s="93" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="94"/>
       <c r="C10" s="10" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="D10" s="33"/>
       <c r="E10" s="11"/>
       <c r="F10" s="34" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="G10" s="34"/>
       <c r="H10" s="35"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="87" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="88"/>
+      <c r="A11" s="93" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="94"/>
       <c r="C11" s="10" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="11"/>
       <c r="F11" s="34" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="G11" s="34"/>
       <c r="H11" s="35"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="87" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="88"/>
-      <c r="C12" s="86" t="s">
-        <v>82</v>
+      <c r="A12" s="93" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="94"/>
+      <c r="C12" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="D12" s="33"/>
       <c r="E12" s="11"/>
       <c r="F12" s="34" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="G12" s="34"/>
       <c r="H12" s="35"/>
     </row>
-    <row r="13" spans="1:10" ht="45" customHeight="1">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:10">
+      <c r="A13" s="93" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="94"/>
+      <c r="C13" s="86" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="33"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="34"/>
+      <c r="H13" s="35"/>
+    </row>
+    <row r="14" spans="1:10" ht="45" customHeight="1">
+      <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="89" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="90"/>
-      <c r="E13" s="91"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="65"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="3" t="s">
-        <v>2</v>
-      </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
+      <c r="C14" s="95" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="96"/>
+      <c r="E14" s="97"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
       <c r="H14" s="34"/>
       <c r="I14" s="34"/>
       <c r="J14" s="34"/>
     </row>
-    <row r="15" spans="1:10" s="32" customFormat="1">
-      <c r="A15" s="62" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="63"/>
-      <c r="C15" s="64" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15"/>
-      <c r="F15"/>
-      <c r="G15" s="66"/>
-      <c r="H15"/>
+    <row r="15" spans="1:10">
+      <c r="A15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
     </row>
     <row r="16" spans="1:10" s="32" customFormat="1">
       <c r="A16" s="62" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="B16" s="63"/>
       <c r="C16" s="64" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="E16"/>
       <c r="F16"/>
@@ -2042,12 +2478,14 @@
     </row>
     <row r="17" spans="1:12" s="32" customFormat="1">
       <c r="A17" s="62" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B17" s="63"/>
-      <c r="C17" s="64"/>
+      <c r="C17" s="64" t="s">
+        <v>14</v>
+      </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E17"/>
       <c r="F17"/>
@@ -2056,14 +2494,12 @@
     </row>
     <row r="18" spans="1:12" s="32" customFormat="1">
       <c r="A18" s="62" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B18" s="63"/>
-      <c r="C18" s="64" t="s">
-        <v>15</v>
-      </c>
+      <c r="C18" s="64"/>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E18"/>
       <c r="F18"/>
@@ -2072,14 +2508,14 @@
     </row>
     <row r="19" spans="1:12" s="32" customFormat="1">
       <c r="A19" s="62" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="B19" s="63"/>
       <c r="C19" s="64" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="E19"/>
       <c r="F19"/>
@@ -2087,15 +2523,15 @@
       <c r="H19"/>
     </row>
     <row r="20" spans="1:12" s="32" customFormat="1">
-      <c r="A20" s="92" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="93"/>
+      <c r="A20" s="62" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="63"/>
       <c r="C20" s="64" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E20"/>
       <c r="F20"/>
@@ -2104,28 +2540,30 @@
     </row>
     <row r="21" spans="1:12" s="32" customFormat="1">
       <c r="A21" s="62" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="B21" s="63"/>
       <c r="C21" s="64" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21"/>
+        <v>14</v>
+      </c>
+      <c r="D21" t="s">
+        <v>79</v>
+      </c>
       <c r="E21"/>
       <c r="F21"/>
       <c r="G21" s="66"/>
       <c r="H21"/>
     </row>
     <row r="22" spans="1:12" s="32" customFormat="1">
-      <c r="A22" s="92" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="93"/>
+      <c r="A22" s="87" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="88"/>
       <c r="C22" s="64" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="E22"/>
       <c r="F22"/>
@@ -2133,12 +2571,12 @@
       <c r="H22"/>
     </row>
     <row r="23" spans="1:12" s="32" customFormat="1">
-      <c r="A23" s="92" t="s">
-        <v>83</v>
-      </c>
-      <c r="B23" s="93"/>
+      <c r="A23" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="63"/>
       <c r="C23" s="64" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D23"/>
       <c r="E23"/>
@@ -2146,92 +2584,94 @@
       <c r="G23" s="66"/>
       <c r="H23"/>
     </row>
-    <row r="24" spans="1:12" s="37" customFormat="1">
-      <c r="A24" s="34"/>
-      <c r="B24" s="36"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="81"/>
-      <c r="F25" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="43"/>
-      <c r="J25" s="43"/>
-      <c r="K25" s="43"/>
-      <c r="L25" s="43"/>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="42" t="s">
+    <row r="24" spans="1:12" s="32" customFormat="1">
+      <c r="A24" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="82"/>
-      <c r="F26" s="67"/>
-      <c r="G26" s="67"/>
-      <c r="H26" s="67"/>
-      <c r="I26" s="44"/>
-      <c r="J26" s="45"/>
-      <c r="K26" s="45"/>
-      <c r="L26" s="35"/>
+      <c r="B24" s="88"/>
+      <c r="C24" s="64" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24" s="66"/>
+      <c r="H24"/>
+    </row>
+    <row r="25" spans="1:12" s="32" customFormat="1">
+      <c r="A25" s="87" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="88"/>
+      <c r="C25" s="64" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25" s="66"/>
+      <c r="H25"/>
+    </row>
+    <row r="26" spans="1:12" s="37" customFormat="1">
+      <c r="A26" s="34"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="34"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="51">
+      <c r="A27" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="81"/>
+      <c r="F27" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="43"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="82"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="67"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="45"/>
+      <c r="K28" s="45"/>
+      <c r="L28" s="35"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="51">
         <v>1</v>
       </c>
-      <c r="B27" s="46" t="s">
-        <v>74</v>
-      </c>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
-      <c r="K27" s="36"/>
-      <c r="L27" s="35"/>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="51"/>
-      <c r="B28" s="46"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="68"/>
-      <c r="G28" s="68"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
-      <c r="K28" s="36"/>
-      <c r="L28" s="35"/>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="52"/>
-      <c r="B29" s="48"/>
-      <c r="C29" s="49"/>
-      <c r="D29" s="49"/>
-      <c r="E29" s="50"/>
+      <c r="B29" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="39"/>
       <c r="F29" s="68"/>
       <c r="G29" s="68"/>
       <c r="H29" s="34"/>
@@ -2241,86 +2681,94 @@
       <c r="L29" s="35"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
+      <c r="A30" s="51">
+        <v>2</v>
+      </c>
+      <c r="B30" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="68"/>
+      <c r="G30" s="68"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="36"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="35"/>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="81"/>
-      <c r="F31" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="G31" s="44"/>
-      <c r="H31" s="44"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="43"/>
-      <c r="K31" s="43"/>
-      <c r="L31" s="43"/>
+      <c r="A31" s="52"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="68"/>
+      <c r="G31" s="68"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="36"/>
+      <c r="J31" s="36"/>
+      <c r="K31" s="36"/>
+      <c r="L31" s="35"/>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" s="42"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="82"/>
-      <c r="F32" s="67"/>
-      <c r="G32" s="67"/>
-      <c r="H32" s="67"/>
-      <c r="I32" s="44"/>
-      <c r="J32" s="45"/>
-      <c r="K32" s="45"/>
-      <c r="L32" s="35"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
     </row>
     <row r="33" spans="1:12">
-      <c r="A33" s="51"/>
-      <c r="B33" s="46"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="68"/>
-      <c r="G33" s="68"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="36"/>
-      <c r="J33" s="36"/>
-      <c r="K33" s="36"/>
-      <c r="L33" s="35"/>
+      <c r="A33" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="81"/>
+      <c r="F33" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="43"/>
+      <c r="L33" s="43"/>
     </row>
     <row r="34" spans="1:12">
-      <c r="A34" s="51"/>
-      <c r="B34" s="46"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="68"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="36"/>
-      <c r="J34" s="36"/>
-      <c r="K34" s="36"/>
+      <c r="A34" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="82"/>
+      <c r="F34" s="67"/>
+      <c r="G34" s="67"/>
+      <c r="H34" s="67"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="45"/>
+      <c r="K34" s="45"/>
       <c r="L34" s="35"/>
     </row>
     <row r="35" spans="1:12">
-      <c r="A35" s="52"/>
-      <c r="B35" s="48"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="50"/>
+      <c r="A35" s="51">
+        <v>1</v>
+      </c>
+      <c r="B35" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="39"/>
       <c r="F35" s="68"/>
       <c r="G35" s="68"/>
       <c r="H35" s="34"/>
@@ -2330,94 +2778,97 @@
       <c r="L35" s="35"/>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
+      <c r="A36" s="51">
+        <v>2</v>
+      </c>
+      <c r="B36" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="68"/>
+      <c r="G36" s="68"/>
+      <c r="H36" s="34"/>
+      <c r="I36" s="36"/>
+      <c r="J36" s="36"/>
+      <c r="K36" s="36"/>
+      <c r="L36" s="35"/>
     </row>
     <row r="37" spans="1:12">
-      <c r="A37" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="B37" s="31"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="81"/>
-      <c r="F37" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="G37" s="44"/>
-      <c r="H37" s="44"/>
-      <c r="I37" s="43"/>
-      <c r="J37" s="43"/>
-      <c r="K37" s="43"/>
-      <c r="L37" s="43"/>
+      <c r="A37" s="52"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="68"/>
+      <c r="G37" s="68"/>
+      <c r="H37" s="34"/>
+      <c r="I37" s="36"/>
+      <c r="J37" s="36"/>
+      <c r="K37" s="36"/>
+      <c r="L37" s="35"/>
     </row>
     <row r="38" spans="1:12">
-      <c r="A38" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="B38" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="C38" s="42"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="82"/>
-      <c r="F38" s="67"/>
-      <c r="G38" s="67"/>
-      <c r="H38" s="67"/>
-      <c r="I38" s="44"/>
-      <c r="J38" s="45"/>
-      <c r="K38" s="45"/>
+      <c r="A38" s="83"/>
+      <c r="B38" s="84"/>
+      <c r="C38" s="85"/>
+      <c r="D38" s="85"/>
+      <c r="E38" s="85"/>
+      <c r="F38" s="68"/>
+      <c r="G38" s="68"/>
+      <c r="H38" s="34"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="36"/>
+      <c r="K38" s="36"/>
       <c r="L38" s="35"/>
     </row>
     <row r="39" spans="1:12">
-      <c r="A39" s="51">
+      <c r="A39" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="B39" s="31"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="81"/>
+      <c r="F39" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G39" s="44"/>
+      <c r="H39" s="44"/>
+      <c r="I39" s="43"/>
+      <c r="J39" s="43"/>
+      <c r="K39" s="43"/>
+      <c r="L39" s="43"/>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="42"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="82"/>
+      <c r="F40" s="67"/>
+      <c r="G40" s="67"/>
+      <c r="H40" s="67"/>
+      <c r="I40" s="44"/>
+      <c r="J40" s="45"/>
+      <c r="K40" s="45"/>
+      <c r="L40" s="35"/>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="51">
         <v>1</v>
       </c>
-      <c r="B39" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="39"/>
-      <c r="F39" s="68"/>
-      <c r="G39" s="68"/>
-      <c r="H39" s="34"/>
-      <c r="I39" s="36"/>
-      <c r="J39" s="36"/>
-      <c r="K39" s="36"/>
-      <c r="L39" s="35"/>
-    </row>
-    <row r="40" spans="1:12">
-      <c r="A40" s="51">
-        <v>2</v>
-      </c>
-      <c r="B40" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="C40" s="40"/>
-      <c r="D40" s="40"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="68"/>
-      <c r="G40" s="68"/>
-      <c r="H40" s="34"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="36"/>
-      <c r="K40" s="36"/>
-      <c r="L40" s="35"/>
-    </row>
-    <row r="41" spans="1:12">
-      <c r="A41" s="52"/>
-      <c r="B41" s="48"/>
-      <c r="C41" s="49"/>
-      <c r="D41" s="49"/>
-      <c r="E41" s="50"/>
+      <c r="B41" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="39"/>
       <c r="F41" s="68"/>
       <c r="G41" s="68"/>
       <c r="H41" s="34"/>
@@ -2427,11 +2878,15 @@
       <c r="L41" s="35"/>
     </row>
     <row r="42" spans="1:12">
-      <c r="A42" s="83"/>
-      <c r="B42" s="84"/>
-      <c r="C42" s="85"/>
-      <c r="D42" s="85"/>
-      <c r="E42" s="85"/>
+      <c r="A42" s="51">
+        <v>2</v>
+      </c>
+      <c r="B42" s="46" t="s">
+        <v>117</v>
+      </c>
+      <c r="C42" s="40"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="41"/>
       <c r="F42" s="68"/>
       <c r="G42" s="68"/>
       <c r="H42" s="34"/>
@@ -2441,451 +2896,981 @@
       <c r="L42" s="35"/>
     </row>
     <row r="43" spans="1:12">
-      <c r="A43" s="13"/>
-      <c r="B43" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
-      <c r="I43" s="13"/>
+      <c r="A43" s="52"/>
+      <c r="B43" s="48"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="49"/>
+      <c r="E43" s="50"/>
+      <c r="F43" s="68"/>
+      <c r="G43" s="68"/>
+      <c r="H43" s="34"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
+      <c r="K43" s="36"/>
+      <c r="L43" s="35"/>
     </row>
     <row r="44" spans="1:12">
-      <c r="A44" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="6"/>
-      <c r="L44" s="15"/>
-    </row>
-    <row r="45" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A45" s="95" t="s">
-        <v>8</v>
-      </c>
-      <c r="B45" s="95" t="s">
+      <c r="A44" s="13"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" s="31"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="81"/>
+      <c r="F45" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="G45" s="44"/>
+      <c r="H45" s="44"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
+      <c r="K45" s="43"/>
+      <c r="L45" s="43"/>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" s="47" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="E46" s="82"/>
+      <c r="F46" s="67"/>
+      <c r="G46" s="67"/>
+      <c r="H46" s="67"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="45"/>
+      <c r="K46" s="45"/>
+      <c r="L46" s="35"/>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" s="51">
+        <v>1</v>
+      </c>
+      <c r="B47" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" s="98" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" s="39"/>
+      <c r="F47" s="68"/>
+      <c r="G47" s="68"/>
+      <c r="H47" s="34"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="36"/>
+      <c r="K47" s="36"/>
+      <c r="L47" s="35"/>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" s="51">
+        <v>2</v>
+      </c>
+      <c r="B48" s="46" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" s="99" t="s">
+        <v>89</v>
+      </c>
+      <c r="D48" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="E48" s="41"/>
+      <c r="F48" s="68"/>
+      <c r="G48" s="68"/>
+      <c r="H48" s="34"/>
+      <c r="I48" s="36"/>
+      <c r="J48" s="36"/>
+      <c r="K48" s="36"/>
+      <c r="L48" s="35"/>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49" s="52"/>
+      <c r="B49" s="48"/>
+      <c r="C49" s="100"/>
+      <c r="D49" s="49"/>
+      <c r="E49" s="50"/>
+      <c r="F49" s="68"/>
+      <c r="G49" s="68"/>
+      <c r="H49" s="34"/>
+      <c r="I49" s="36"/>
+      <c r="J49" s="36"/>
+      <c r="K49" s="36"/>
+      <c r="L49" s="35"/>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50" s="83"/>
+      <c r="B50" s="84"/>
+      <c r="C50" s="85"/>
+      <c r="D50" s="85"/>
+      <c r="E50" s="85"/>
+      <c r="F50" s="68"/>
+      <c r="G50" s="68"/>
+      <c r="H50" s="34"/>
+      <c r="I50" s="36"/>
+      <c r="J50" s="36"/>
+      <c r="K50" s="36"/>
+      <c r="L50" s="35"/>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="B51" s="31"/>
+      <c r="C51" s="31"/>
+      <c r="D51" s="31"/>
+      <c r="E51" s="81"/>
+      <c r="F51" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G51" s="44"/>
+      <c r="H51" s="44"/>
+      <c r="I51" s="43"/>
+      <c r="J51" s="43"/>
+      <c r="K51" s="43"/>
+      <c r="L51" s="43"/>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52" s="42"/>
+      <c r="D52" s="42"/>
+      <c r="E52" s="82"/>
+      <c r="F52" s="67" t="s">
+        <v>113</v>
+      </c>
+      <c r="G52" s="67"/>
+      <c r="H52" s="67"/>
+      <c r="I52" s="44"/>
+      <c r="J52" s="45"/>
+      <c r="K52" s="45"/>
+      <c r="L52" s="35"/>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53" s="51"/>
+      <c r="B53" s="46"/>
+      <c r="C53" s="38"/>
+      <c r="D53" s="38"/>
+      <c r="E53" s="39"/>
+      <c r="F53" s="68"/>
+      <c r="G53" s="68"/>
+      <c r="H53" s="34"/>
+      <c r="I53" s="36"/>
+      <c r="J53" s="36"/>
+      <c r="K53" s="36"/>
+      <c r="L53" s="35"/>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54" s="51"/>
+      <c r="B54" s="46"/>
+      <c r="C54" s="40"/>
+      <c r="D54" s="40"/>
+      <c r="E54" s="41"/>
+      <c r="F54" s="68"/>
+      <c r="G54" s="68"/>
+      <c r="H54" s="34"/>
+      <c r="I54" s="36"/>
+      <c r="J54" s="36"/>
+      <c r="K54" s="36"/>
+      <c r="L54" s="35"/>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55" s="52"/>
+      <c r="B55" s="48"/>
+      <c r="C55" s="49"/>
+      <c r="D55" s="49"/>
+      <c r="E55" s="50"/>
+      <c r="F55" s="68"/>
+      <c r="G55" s="68"/>
+      <c r="H55" s="34"/>
+      <c r="I55" s="36"/>
+      <c r="J55" s="36"/>
+      <c r="K55" s="36"/>
+      <c r="L55" s="35"/>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56" s="13"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" s="13"/>
+      <c r="B57" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="13"/>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
+      <c r="J58" s="14"/>
+      <c r="K58" s="6"/>
+      <c r="L58" s="15"/>
+    </row>
+    <row r="59" spans="1:12" ht="13.5" customHeight="1">
+      <c r="A59" s="90" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="C45" s="94" t="s">
+      <c r="C59" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="94" t="s">
+      <c r="D59" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="E45" s="94" t="s">
+      <c r="E59" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="F45" s="96" t="s">
-        <v>41</v>
-      </c>
-      <c r="G45" s="96" t="s">
-        <v>17</v>
-      </c>
-      <c r="H45" s="94" t="s">
+      <c r="F59" s="91" t="s">
+        <v>33</v>
+      </c>
+      <c r="G59" s="91" t="s">
+        <v>16</v>
+      </c>
+      <c r="H59" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="I45" s="94"/>
-      <c r="J45" s="16"/>
-      <c r="K45" s="17"/>
-      <c r="L45" s="9"/>
-    </row>
-    <row r="46" spans="1:12">
-      <c r="A46" s="95"/>
-      <c r="B46" s="95"/>
-      <c r="C46" s="94"/>
-      <c r="D46" s="94"/>
-      <c r="E46" s="94"/>
-      <c r="F46" s="97"/>
-      <c r="G46" s="97"/>
-      <c r="H46" s="94"/>
-      <c r="I46" s="94"/>
-      <c r="J46" s="18"/>
-      <c r="K46" s="29"/>
-      <c r="L46" s="15"/>
-    </row>
-    <row r="47" spans="1:12">
-      <c r="A47" s="19">
+      <c r="I59" s="89"/>
+      <c r="J59" s="16"/>
+      <c r="K59" s="17"/>
+      <c r="L59" s="9"/>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60" s="90"/>
+      <c r="B60" s="90"/>
+      <c r="C60" s="89"/>
+      <c r="D60" s="89"/>
+      <c r="E60" s="89"/>
+      <c r="F60" s="92"/>
+      <c r="G60" s="92"/>
+      <c r="H60" s="89"/>
+      <c r="I60" s="89"/>
+      <c r="J60" s="18"/>
+      <c r="K60" s="29"/>
+      <c r="L60" s="15"/>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61" s="19">
         <v>1</v>
       </c>
-      <c r="B47" s="71" t="s">
+      <c r="B61" s="71" t="s">
+        <v>47</v>
+      </c>
+      <c r="C61" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="D61" s="20"/>
+      <c r="E61" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F61" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G61" s="69"/>
+      <c r="H61" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="78" t="s">
-        <v>58</v>
-      </c>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="F47" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="G47" s="69"/>
-      <c r="H47" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="I47" s="21"/>
-      <c r="J47" s="21"/>
-      <c r="K47" s="28"/>
-      <c r="L47" s="15"/>
-    </row>
-    <row r="48" spans="1:12">
-      <c r="A48" s="19">
-        <f>A47+1</f>
+      <c r="I61" s="21"/>
+      <c r="J61" s="21"/>
+      <c r="K61" s="28"/>
+      <c r="L61" s="15"/>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62" s="19">
+        <f>A61+1</f>
         <v>2</v>
       </c>
-      <c r="B48" s="71" t="s">
-        <v>60</v>
-      </c>
-      <c r="C48" s="78" t="s">
-        <v>61</v>
-      </c>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20" t="b">
+      <c r="B62" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="C62" s="78" t="s">
+        <v>51</v>
+      </c>
+      <c r="D62" s="20"/>
+      <c r="E62" s="20" t="b">
         <v>1</v>
       </c>
-      <c r="F48" s="20"/>
-      <c r="G48" s="69"/>
-      <c r="H48" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="I48" s="21"/>
-      <c r="J48" s="21"/>
-      <c r="K48" s="28"/>
-      <c r="L48" s="15"/>
-    </row>
-    <row r="49" spans="1:12">
-      <c r="A49" s="19">
-        <f t="shared" ref="A49:A63" si="0">A48+1</f>
+      <c r="F62" s="20"/>
+      <c r="G62" s="69"/>
+      <c r="H62" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="I62" s="21"/>
+      <c r="J62" s="21"/>
+      <c r="K62" s="28"/>
+      <c r="L62" s="15"/>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63" s="19">
+        <f t="shared" ref="A63:A77" si="0">A62+1</f>
         <v>3</v>
       </c>
-      <c r="B49" s="72" t="s">
-        <v>63</v>
-      </c>
-      <c r="C49" s="79" t="s">
-        <v>64</v>
-      </c>
-      <c r="D49" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
-      <c r="G49" s="69" t="s">
-        <v>15</v>
-      </c>
-      <c r="H49" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="I49" s="21"/>
-      <c r="J49" s="21"/>
-      <c r="K49" s="22"/>
-      <c r="L49" s="15"/>
-    </row>
-    <row r="50" spans="1:12">
-      <c r="A50" s="19">
+      <c r="B63" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="C63" s="79" t="s">
+        <v>54</v>
+      </c>
+      <c r="D63" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="E63" s="20"/>
+      <c r="F63" s="20"/>
+      <c r="G63" s="69" t="s">
+        <v>14</v>
+      </c>
+      <c r="H63" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="I63" s="21"/>
+      <c r="J63" s="21"/>
+      <c r="K63" s="22"/>
+      <c r="L63" s="15"/>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64" s="19">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B50" s="73" t="s">
-        <v>70</v>
-      </c>
-      <c r="C50" s="80" t="s">
-        <v>65</v>
-      </c>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="69" t="s">
-        <v>15</v>
-      </c>
-      <c r="H50" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="I50" s="21"/>
-      <c r="J50" s="21"/>
-      <c r="K50" s="22"/>
-      <c r="L50" s="15"/>
-    </row>
-    <row r="51" spans="1:12">
-      <c r="A51" s="19">
+      <c r="B64" s="73" t="s">
+        <v>59</v>
+      </c>
+      <c r="C64" s="80" t="s">
+        <v>55</v>
+      </c>
+      <c r="D64" s="20"/>
+      <c r="E64" s="20"/>
+      <c r="F64" s="20"/>
+      <c r="G64" s="69" t="s">
+        <v>14</v>
+      </c>
+      <c r="H64" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="I64" s="21"/>
+      <c r="J64" s="21"/>
+      <c r="K64" s="22"/>
+      <c r="L64" s="15"/>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65" s="19">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B51" s="73"/>
-      <c r="C51" s="80"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="69"/>
-      <c r="H51" s="20"/>
-      <c r="I51" s="21"/>
-      <c r="J51" s="21"/>
-      <c r="K51" s="22"/>
-      <c r="L51" s="15"/>
-    </row>
-    <row r="52" spans="1:12">
-      <c r="A52" s="19">
+      <c r="B65" s="73"/>
+      <c r="C65" s="80"/>
+      <c r="D65" s="20"/>
+      <c r="E65" s="20"/>
+      <c r="F65" s="20"/>
+      <c r="G65" s="69"/>
+      <c r="H65" s="20"/>
+      <c r="I65" s="21"/>
+      <c r="J65" s="21"/>
+      <c r="K65" s="22"/>
+      <c r="L65" s="15"/>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66" s="19">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B52" s="73"/>
-      <c r="C52" s="80"/>
-      <c r="D52" s="74"/>
-      <c r="E52" s="74"/>
-      <c r="F52" s="74"/>
-      <c r="G52" s="75"/>
-      <c r="H52" s="74"/>
-      <c r="I52" s="76"/>
-      <c r="J52" s="76"/>
-      <c r="K52" s="77"/>
-      <c r="L52" s="15"/>
-    </row>
-    <row r="53" spans="1:12">
-      <c r="A53" s="19">
+      <c r="B66" s="73"/>
+      <c r="C66" s="80"/>
+      <c r="D66" s="74"/>
+      <c r="E66" s="74"/>
+      <c r="F66" s="74"/>
+      <c r="G66" s="75"/>
+      <c r="H66" s="74"/>
+      <c r="I66" s="76"/>
+      <c r="J66" s="76"/>
+      <c r="K66" s="77"/>
+      <c r="L66" s="15"/>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67" s="19">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B53" s="73"/>
-      <c r="C53" s="80"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
-      <c r="G53" s="69"/>
-      <c r="H53" s="20"/>
-      <c r="I53" s="21"/>
-      <c r="J53" s="21"/>
-      <c r="K53" s="22"/>
-      <c r="L53" s="15"/>
-    </row>
-    <row r="54" spans="1:12">
-      <c r="A54" s="19">
+      <c r="B67" s="73"/>
+      <c r="C67" s="80"/>
+      <c r="D67" s="20"/>
+      <c r="E67" s="20"/>
+      <c r="F67" s="20"/>
+      <c r="G67" s="69"/>
+      <c r="H67" s="20"/>
+      <c r="I67" s="21"/>
+      <c r="J67" s="21"/>
+      <c r="K67" s="22"/>
+      <c r="L67" s="15"/>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="A68" s="19">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B54" s="73"/>
-      <c r="C54" s="80"/>
-      <c r="D54" s="74"/>
-      <c r="E54" s="74"/>
-      <c r="F54" s="74"/>
-      <c r="G54" s="75"/>
-      <c r="H54" s="74"/>
-      <c r="I54" s="76"/>
-      <c r="J54" s="76"/>
-      <c r="K54" s="77"/>
-      <c r="L54" s="15"/>
-    </row>
-    <row r="55" spans="1:12">
-      <c r="A55" s="19">
+      <c r="B68" s="73"/>
+      <c r="C68" s="80"/>
+      <c r="D68" s="74"/>
+      <c r="E68" s="74"/>
+      <c r="F68" s="74"/>
+      <c r="G68" s="75"/>
+      <c r="H68" s="74"/>
+      <c r="I68" s="76"/>
+      <c r="J68" s="76"/>
+      <c r="K68" s="77"/>
+      <c r="L68" s="15"/>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69" s="19">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B55" s="73"/>
-      <c r="C55" s="80"/>
-      <c r="D55" s="74"/>
-      <c r="E55" s="74"/>
-      <c r="F55" s="74"/>
-      <c r="G55" s="75"/>
-      <c r="H55" s="74"/>
-      <c r="I55" s="76"/>
-      <c r="J55" s="76"/>
-      <c r="K55" s="77"/>
-      <c r="L55" s="15"/>
-    </row>
-    <row r="56" spans="1:12">
-      <c r="A56" s="19">
+      <c r="B69" s="73"/>
+      <c r="C69" s="80"/>
+      <c r="D69" s="74"/>
+      <c r="E69" s="74"/>
+      <c r="F69" s="74"/>
+      <c r="G69" s="75"/>
+      <c r="H69" s="74"/>
+      <c r="I69" s="76"/>
+      <c r="J69" s="76"/>
+      <c r="K69" s="77"/>
+      <c r="L69" s="15"/>
+    </row>
+    <row r="70" spans="1:12">
+      <c r="A70" s="19">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B56" s="73"/>
-      <c r="C56" s="80"/>
-      <c r="D56" s="20"/>
-      <c r="E56" s="20"/>
-      <c r="F56" s="20"/>
-      <c r="G56" s="69"/>
-      <c r="H56" s="20"/>
-      <c r="I56" s="21"/>
-      <c r="J56" s="21"/>
-      <c r="K56" s="22"/>
-      <c r="L56" s="15"/>
-    </row>
-    <row r="57" spans="1:12">
-      <c r="A57" s="19">
+      <c r="B70" s="73"/>
+      <c r="C70" s="80"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="20"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="69"/>
+      <c r="H70" s="20"/>
+      <c r="I70" s="21"/>
+      <c r="J70" s="21"/>
+      <c r="K70" s="22"/>
+      <c r="L70" s="15"/>
+    </row>
+    <row r="71" spans="1:12">
+      <c r="A71" s="19">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B57" s="73"/>
-      <c r="C57" s="80"/>
-      <c r="D57" s="74"/>
-      <c r="E57" s="74"/>
-      <c r="F57" s="74"/>
-      <c r="G57" s="75"/>
-      <c r="H57" s="74"/>
-      <c r="I57" s="76"/>
-      <c r="J57" s="76"/>
-      <c r="K57" s="77"/>
-      <c r="L57" s="15"/>
-    </row>
-    <row r="58" spans="1:12">
-      <c r="A58" s="19">
+      <c r="B71" s="73"/>
+      <c r="C71" s="80"/>
+      <c r="D71" s="74"/>
+      <c r="E71" s="74"/>
+      <c r="F71" s="74"/>
+      <c r="G71" s="75"/>
+      <c r="H71" s="74"/>
+      <c r="I71" s="76"/>
+      <c r="J71" s="76"/>
+      <c r="K71" s="77"/>
+      <c r="L71" s="15"/>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72" s="19">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B58" s="73"/>
-      <c r="C58" s="80"/>
-      <c r="D58" s="74"/>
-      <c r="E58" s="74"/>
-      <c r="F58" s="74"/>
-      <c r="G58" s="75"/>
-      <c r="H58" s="74"/>
-      <c r="I58" s="76"/>
-      <c r="J58" s="76"/>
-      <c r="K58" s="77"/>
-      <c r="L58" s="15"/>
-    </row>
-    <row r="59" spans="1:12">
-      <c r="A59" s="19">
+      <c r="B72" s="73"/>
+      <c r="C72" s="80"/>
+      <c r="D72" s="74"/>
+      <c r="E72" s="74"/>
+      <c r="F72" s="74"/>
+      <c r="G72" s="75"/>
+      <c r="H72" s="74"/>
+      <c r="I72" s="76"/>
+      <c r="J72" s="76"/>
+      <c r="K72" s="77"/>
+      <c r="L72" s="15"/>
+    </row>
+    <row r="73" spans="1:12">
+      <c r="A73" s="19">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B59" s="73"/>
-      <c r="C59" s="80"/>
-      <c r="D59" s="20"/>
-      <c r="E59" s="20"/>
-      <c r="F59" s="20"/>
-      <c r="G59" s="69"/>
-      <c r="H59" s="20"/>
-      <c r="I59" s="21"/>
-      <c r="J59" s="21"/>
-      <c r="K59" s="22"/>
-      <c r="L59" s="15"/>
-    </row>
-    <row r="60" spans="1:12">
-      <c r="A60" s="19">
+      <c r="B73" s="73"/>
+      <c r="C73" s="80"/>
+      <c r="D73" s="20"/>
+      <c r="E73" s="20"/>
+      <c r="F73" s="20"/>
+      <c r="G73" s="69"/>
+      <c r="H73" s="20"/>
+      <c r="I73" s="21"/>
+      <c r="J73" s="21"/>
+      <c r="K73" s="22"/>
+      <c r="L73" s="15"/>
+    </row>
+    <row r="74" spans="1:12">
+      <c r="A74" s="19">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B60" s="73"/>
-      <c r="C60" s="80"/>
-      <c r="D60" s="74"/>
-      <c r="E60" s="74"/>
-      <c r="F60" s="74"/>
-      <c r="G60" s="75"/>
-      <c r="H60" s="74"/>
-      <c r="I60" s="76"/>
-      <c r="J60" s="76"/>
-      <c r="K60" s="77"/>
-      <c r="L60" s="15"/>
-    </row>
-    <row r="61" spans="1:12">
-      <c r="A61" s="19">
+      <c r="B74" s="73"/>
+      <c r="C74" s="80"/>
+      <c r="D74" s="74"/>
+      <c r="E74" s="74"/>
+      <c r="F74" s="74"/>
+      <c r="G74" s="75"/>
+      <c r="H74" s="74"/>
+      <c r="I74" s="76"/>
+      <c r="J74" s="76"/>
+      <c r="K74" s="77"/>
+      <c r="L74" s="15"/>
+    </row>
+    <row r="75" spans="1:12">
+      <c r="A75" s="19">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B61" s="73"/>
-      <c r="C61" s="80"/>
-      <c r="D61" s="74"/>
-      <c r="E61" s="74"/>
-      <c r="F61" s="74"/>
-      <c r="G61" s="75"/>
-      <c r="H61" s="74"/>
-      <c r="I61" s="76"/>
-      <c r="J61" s="76"/>
-      <c r="K61" s="77"/>
-      <c r="L61" s="15"/>
-    </row>
-    <row r="62" spans="1:12">
-      <c r="A62" s="19">
+      <c r="B75" s="73"/>
+      <c r="C75" s="80"/>
+      <c r="D75" s="74"/>
+      <c r="E75" s="74"/>
+      <c r="F75" s="74"/>
+      <c r="G75" s="75"/>
+      <c r="H75" s="74"/>
+      <c r="I75" s="76"/>
+      <c r="J75" s="76"/>
+      <c r="K75" s="77"/>
+      <c r="L75" s="15"/>
+    </row>
+    <row r="76" spans="1:12">
+      <c r="A76" s="19">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B62" s="73"/>
-      <c r="C62" s="80"/>
-      <c r="D62" s="20"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="20"/>
-      <c r="G62" s="69"/>
-      <c r="H62" s="20"/>
-      <c r="I62" s="21"/>
-      <c r="J62" s="21"/>
-      <c r="K62" s="22"/>
-      <c r="L62" s="15"/>
-    </row>
-    <row r="63" spans="1:12">
-      <c r="A63" s="19">
+      <c r="B76" s="73"/>
+      <c r="C76" s="80"/>
+      <c r="D76" s="20"/>
+      <c r="E76" s="20"/>
+      <c r="F76" s="20"/>
+      <c r="G76" s="69"/>
+      <c r="H76" s="20"/>
+      <c r="I76" s="21"/>
+      <c r="J76" s="21"/>
+      <c r="K76" s="22"/>
+      <c r="L76" s="15"/>
+    </row>
+    <row r="77" spans="1:12">
+      <c r="A77" s="19">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B63" s="73"/>
-      <c r="C63" s="80"/>
-      <c r="D63" s="74"/>
-      <c r="E63" s="74"/>
-      <c r="F63" s="74"/>
-      <c r="G63" s="75"/>
-      <c r="H63" s="74"/>
-      <c r="I63" s="76"/>
-      <c r="J63" s="76"/>
-      <c r="K63" s="77"/>
-      <c r="L63" s="15"/>
-    </row>
-    <row r="64" spans="1:12">
-      <c r="A64" s="23"/>
-      <c r="B64" s="24"/>
-      <c r="C64" s="25"/>
-      <c r="D64" s="25"/>
-      <c r="E64" s="25"/>
-      <c r="F64" s="25"/>
-      <c r="G64" s="70"/>
-      <c r="H64" s="25"/>
-      <c r="I64" s="26"/>
-      <c r="J64" s="26"/>
-      <c r="K64" s="27"/>
-      <c r="L64" s="15"/>
+      <c r="B77" s="73"/>
+      <c r="C77" s="80"/>
+      <c r="D77" s="74"/>
+      <c r="E77" s="74"/>
+      <c r="F77" s="74"/>
+      <c r="G77" s="75"/>
+      <c r="H77" s="74"/>
+      <c r="I77" s="76"/>
+      <c r="J77" s="76"/>
+      <c r="K77" s="77"/>
+      <c r="L77" s="15"/>
+    </row>
+    <row r="78" spans="1:12">
+      <c r="A78" s="23"/>
+      <c r="B78" s="24"/>
+      <c r="C78" s="25"/>
+      <c r="D78" s="25"/>
+      <c r="E78" s="25"/>
+      <c r="F78" s="25"/>
+      <c r="G78" s="70"/>
+      <c r="H78" s="25"/>
+      <c r="I78" s="26"/>
+      <c r="J78" s="26"/>
+      <c r="K78" s="27"/>
+      <c r="L78" s="15"/>
+    </row>
+    <row r="80" spans="1:12">
+      <c r="A80" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="B80" s="31"/>
+      <c r="C80" s="31"/>
+      <c r="D80" s="31"/>
+      <c r="E80" s="81"/>
+      <c r="F80" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G80" s="44"/>
+      <c r="H80" s="44"/>
+      <c r="I80" s="43"/>
+      <c r="J80" s="43"/>
+      <c r="K80" s="43"/>
+      <c r="L80" s="43"/>
+    </row>
+    <row r="81" spans="1:12">
+      <c r="A81" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="B81" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C81" s="42"/>
+      <c r="D81" s="42"/>
+      <c r="E81" s="82"/>
+      <c r="F81" s="67"/>
+      <c r="G81" s="67"/>
+      <c r="H81" s="67"/>
+      <c r="I81" s="44"/>
+      <c r="J81" s="45"/>
+      <c r="K81" s="45"/>
+      <c r="L81" s="35"/>
+    </row>
+    <row r="82" spans="1:12">
+      <c r="A82" s="51"/>
+      <c r="B82" s="46"/>
+      <c r="C82" s="38"/>
+      <c r="D82" s="38"/>
+      <c r="E82" s="39"/>
+      <c r="F82" s="68"/>
+      <c r="G82" s="68"/>
+      <c r="H82" s="34"/>
+      <c r="I82" s="36"/>
+      <c r="J82" s="36"/>
+      <c r="K82" s="36"/>
+      <c r="L82" s="35"/>
+    </row>
+    <row r="83" spans="1:12">
+      <c r="A83" s="51"/>
+      <c r="B83" s="46"/>
+      <c r="C83" s="40"/>
+      <c r="D83" s="40"/>
+      <c r="E83" s="41"/>
+      <c r="F83" s="68"/>
+      <c r="G83" s="68"/>
+      <c r="H83" s="34"/>
+      <c r="I83" s="36"/>
+      <c r="J83" s="36"/>
+      <c r="K83" s="36"/>
+      <c r="L83" s="35"/>
+    </row>
+    <row r="84" spans="1:12">
+      <c r="A84" s="52"/>
+      <c r="B84" s="48"/>
+      <c r="C84" s="49"/>
+      <c r="D84" s="49"/>
+      <c r="E84" s="50"/>
+      <c r="F84" s="68"/>
+      <c r="G84" s="68"/>
+      <c r="H84" s="34"/>
+      <c r="I84" s="36"/>
+      <c r="J84" s="36"/>
+      <c r="K84" s="36"/>
+      <c r="L84" s="35"/>
+    </row>
+    <row r="85" spans="1:12">
+      <c r="A85" s="13"/>
+      <c r="B85" s="13"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="13"/>
+      <c r="E85" s="13"/>
+      <c r="F85" s="13"/>
+      <c r="G85" s="13"/>
+      <c r="H85" s="13"/>
+      <c r="I85" s="13"/>
+    </row>
+    <row r="86" spans="1:12">
+      <c r="A86" s="13"/>
+      <c r="B86" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C86" s="13"/>
+      <c r="D86" s="13"/>
+      <c r="E86" s="13"/>
+      <c r="F86" s="13"/>
+      <c r="G86" s="13"/>
+      <c r="H86" s="13"/>
+      <c r="I86" s="13"/>
+    </row>
+    <row r="87" spans="1:12">
+      <c r="A87" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B87" s="14"/>
+      <c r="C87" s="14"/>
+      <c r="D87" s="14"/>
+      <c r="E87" s="14"/>
+      <c r="F87" s="14"/>
+      <c r="G87" s="14"/>
+      <c r="H87" s="14"/>
+      <c r="I87" s="14"/>
+      <c r="J87" s="14"/>
+      <c r="K87" s="6"/>
+      <c r="L87" s="15"/>
+    </row>
+    <row r="88" spans="1:12" ht="13.5" customHeight="1">
+      <c r="A88" s="90" t="s">
+        <v>7</v>
+      </c>
+      <c r="B88" s="90" t="s">
+        <v>94</v>
+      </c>
+      <c r="C88" s="89" t="s">
+        <v>96</v>
+      </c>
+      <c r="D88" s="89" t="s">
+        <v>97</v>
+      </c>
+      <c r="E88" s="89" t="s">
+        <v>87</v>
+      </c>
+      <c r="F88" s="101"/>
+      <c r="G88" s="101"/>
+      <c r="H88" s="105"/>
+      <c r="I88" s="89"/>
+      <c r="J88" s="16"/>
+      <c r="K88" s="17"/>
+      <c r="L88" s="9"/>
+    </row>
+    <row r="89" spans="1:12">
+      <c r="A89" s="90"/>
+      <c r="B89" s="90"/>
+      <c r="C89" s="89"/>
+      <c r="D89" s="89"/>
+      <c r="E89" s="89"/>
+      <c r="F89" s="102"/>
+      <c r="G89" s="102"/>
+      <c r="H89" s="105"/>
+      <c r="I89" s="89"/>
+      <c r="J89" s="18"/>
+      <c r="K89" s="29"/>
+      <c r="L89" s="15"/>
+    </row>
+    <row r="90" spans="1:12">
+      <c r="A90" s="19">
+        <v>1</v>
+      </c>
+      <c r="B90" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="C90" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="D90" s="20"/>
+      <c r="E90" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F90" s="103"/>
+      <c r="G90" s="106"/>
+      <c r="H90" s="103"/>
+      <c r="I90" s="21"/>
+      <c r="J90" s="21"/>
+      <c r="K90" s="28"/>
+      <c r="L90" s="15"/>
+    </row>
+    <row r="91" spans="1:12">
+      <c r="A91" s="19">
+        <f>A90+1</f>
+        <v>2</v>
+      </c>
+      <c r="B91" s="71" t="s">
+        <v>99</v>
+      </c>
+      <c r="C91" s="78" t="s">
+        <v>100</v>
+      </c>
+      <c r="D91" s="20"/>
+      <c r="E91" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="F91" s="103"/>
+      <c r="G91" s="106"/>
+      <c r="H91" s="103"/>
+      <c r="I91" s="21"/>
+      <c r="J91" s="21"/>
+      <c r="K91" s="28"/>
+      <c r="L91" s="15"/>
+    </row>
+    <row r="92" spans="1:12">
+      <c r="A92" s="19">
+        <f t="shared" ref="A92:A96" si="1">A91+1</f>
+        <v>3</v>
+      </c>
+      <c r="B92" s="72" t="s">
+        <v>111</v>
+      </c>
+      <c r="C92" s="79" t="s">
+        <v>54</v>
+      </c>
+      <c r="D92" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="E92" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="F92" s="103"/>
+      <c r="G92" s="106"/>
+      <c r="H92" s="103"/>
+      <c r="I92" s="21"/>
+      <c r="J92" s="21"/>
+      <c r="K92" s="22"/>
+      <c r="L92" s="15"/>
+    </row>
+    <row r="93" spans="1:12">
+      <c r="A93" s="19">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B93" s="73"/>
+      <c r="C93" s="80"/>
+      <c r="D93" s="20"/>
+      <c r="E93" s="20"/>
+      <c r="F93" s="103"/>
+      <c r="G93" s="106"/>
+      <c r="H93" s="103"/>
+      <c r="I93" s="21"/>
+      <c r="J93" s="21"/>
+      <c r="K93" s="22"/>
+      <c r="L93" s="15"/>
+    </row>
+    <row r="94" spans="1:12">
+      <c r="A94" s="19">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B94" s="73"/>
+      <c r="C94" s="80"/>
+      <c r="D94" s="20"/>
+      <c r="E94" s="20"/>
+      <c r="F94" s="103"/>
+      <c r="G94" s="106"/>
+      <c r="H94" s="103"/>
+      <c r="I94" s="21"/>
+      <c r="J94" s="21"/>
+      <c r="K94" s="22"/>
+      <c r="L94" s="15"/>
+    </row>
+    <row r="95" spans="1:12">
+      <c r="A95" s="19">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B95" s="73"/>
+      <c r="C95" s="80"/>
+      <c r="D95" s="74"/>
+      <c r="E95" s="74"/>
+      <c r="F95" s="104"/>
+      <c r="G95" s="107"/>
+      <c r="H95" s="104"/>
+      <c r="I95" s="76"/>
+      <c r="J95" s="76"/>
+      <c r="K95" s="77"/>
+      <c r="L95" s="15"/>
+    </row>
+    <row r="96" spans="1:12">
+      <c r="A96" s="19">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B96" s="73"/>
+      <c r="C96" s="80"/>
+      <c r="D96" s="20"/>
+      <c r="E96" s="20"/>
+      <c r="F96" s="103"/>
+      <c r="G96" s="106"/>
+      <c r="H96" s="103"/>
+      <c r="I96" s="21"/>
+      <c r="J96" s="21"/>
+      <c r="K96" s="22"/>
+      <c r="L96" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H45:I46"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A9:B9"/>
+  <mergeCells count="24">
+    <mergeCell ref="F88:F89"/>
+    <mergeCell ref="G88:G89"/>
+    <mergeCell ref="H88:I89"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="B88:B89"/>
+    <mergeCell ref="C88:C89"/>
+    <mergeCell ref="D88:D89"/>
+    <mergeCell ref="E88:E89"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="H59:I60"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="A25:B25"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
-  <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E80:G80" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations disablePrompts="1" count="5">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E100:G100" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C22:C23" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C24:C25" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
       <formula1>adjustFiledName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
       <formula1>componentKind</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F47:G64 C16:C20" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F61:G78 C17:C22" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>yesNo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C21" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C23" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">
       <formula1>adjustFieldName</formula1>
     </dataValidation>
   </dataValidations>
@@ -2924,7 +3909,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="19">
       <c r="A1" s="53" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="53"/>
       <c r="C1" s="53"/>
@@ -2935,32 +3920,32 @@
       <c r="H1" s="53"/>
       <c r="I1" s="53"/>
       <c r="J1" s="54" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="B3" s="56" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D3" s="56" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F3" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="56" t="s">
+      <c r="J3" s="56" t="s">
         <v>12</v>
-      </c>
-      <c r="J3" s="56" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="B4" s="57" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D4" s="60" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" s="58"/>
       <c r="H4" s="58"/>
@@ -2968,17 +3953,17 @@
     </row>
     <row r="5" spans="1:10">
       <c r="B5" s="59" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D5" s="60"/>
       <c r="F5" s="60" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H5" s="60" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J5" s="60" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:10">

</xml_diff>

<commit_message>
First revision of blancoVueComponent for vue3.
</commit_message>
<xml_diff>
--- a/meta/components/BoxSample.xlsx
+++ b/meta/components/BoxSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVueComponent/meta/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF133BD0-B2AC-724D-B448-4DBDDE0D71BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5731473B-F7B1-5F4E-8F8B-BEA3EB8ACCF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="1840" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21480" yWindow="2280" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VueComponent" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="121">
   <si>
     <t>パッケージ</t>
   </si>
@@ -988,6 +988,24 @@
   </si>
   <si>
     <t>import { SmpleApi } from "@/smples/api/SampleApi"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>クエリ文字列</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>secret</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>URLクエリとして設定される文字列です。</t>
+    <rPh sb="9" eb="11">
+      <t xml:space="preserve">セッテイ </t>
+    </rPh>
+    <rPh sb="14" eb="17">
+      <t xml:space="preserve">モジレツ </t>
+    </rPh>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1634,7 +1652,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1840,6 +1858,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2252,10 +2276,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L96"/>
+  <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="I66" sqref="I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2263,33 +2287,33 @@
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
     <col min="2" max="5" width="23.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.83203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="28" style="1" customWidth="1"/>
-    <col min="11" max="11" width="33.33203125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="1"/>
+    <col min="7" max="8" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.83203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="28" style="1" customWidth="1"/>
+    <col min="12" max="12" width="33.33203125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19">
+    <row r="1" spans="1:11" ht="19">
       <c r="A1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5" s="3" t="s">
         <v>105</v>
       </c>
@@ -2299,8 +2323,9 @@
       <c r="E5" s="5"/>
       <c r="F5" s="34"/>
       <c r="G5" s="34"/>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="H5" s="34"/>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="3" t="s">
         <v>58</v>
       </c>
@@ -2314,9 +2339,10 @@
         <v>71</v>
       </c>
       <c r="G6" s="34"/>
-      <c r="H6" s="35"/>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="H6" s="34"/>
+      <c r="I6" s="35"/>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="3" t="s">
         <v>70</v>
       </c>
@@ -2330,9 +2356,10 @@
         <v>101</v>
       </c>
       <c r="G7" s="34"/>
-      <c r="H7" s="35"/>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="H7" s="34"/>
+      <c r="I7" s="35"/>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="3" t="s">
         <v>72</v>
       </c>
@@ -2346,9 +2373,10 @@
         <v>73</v>
       </c>
       <c r="G8" s="34"/>
-      <c r="H8" s="35"/>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="H8" s="34"/>
+      <c r="I8" s="35"/>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="3" t="s">
         <v>0</v>
       </c>
@@ -2362,9 +2390,10 @@
         <v>75</v>
       </c>
       <c r="G9" s="34"/>
-      <c r="H9" s="35"/>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="H9" s="34"/>
+      <c r="I9" s="35"/>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="93" t="s">
         <v>44</v>
       </c>
@@ -2378,9 +2407,10 @@
         <v>40</v>
       </c>
       <c r="G10" s="34"/>
-      <c r="H10" s="35"/>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="H10" s="34"/>
+      <c r="I10" s="35"/>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="93" t="s">
         <v>45</v>
       </c>
@@ -2394,9 +2424,10 @@
         <v>43</v>
       </c>
       <c r="G11" s="34"/>
-      <c r="H11" s="35"/>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="H11" s="34"/>
+      <c r="I11" s="35"/>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="93" t="s">
         <v>20</v>
       </c>
@@ -2410,9 +2441,10 @@
         <v>41</v>
       </c>
       <c r="G12" s="34"/>
-      <c r="H12" s="35"/>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="H12" s="34"/>
+      <c r="I12" s="35"/>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="93" t="s">
         <v>39</v>
       </c>
@@ -2426,9 +2458,10 @@
         <v>42</v>
       </c>
       <c r="G13" s="34"/>
-      <c r="H13" s="35"/>
-    </row>
-    <row r="14" spans="1:10" ht="45" customHeight="1">
+      <c r="H13" s="34"/>
+      <c r="I13" s="35"/>
+    </row>
+    <row r="14" spans="1:11" ht="45" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
@@ -2440,11 +2473,12 @@
       <c r="E14" s="97"/>
       <c r="F14" s="65"/>
       <c r="G14" s="65"/>
-      <c r="H14" s="34"/>
+      <c r="H14" s="65"/>
       <c r="I14" s="34"/>
       <c r="J14" s="34"/>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="K14" s="34"/>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
@@ -2459,8 +2493,9 @@
       <c r="H15" s="34"/>
       <c r="I15" s="34"/>
       <c r="J15" s="34"/>
-    </row>
-    <row r="16" spans="1:10" s="32" customFormat="1">
+      <c r="K15" s="34"/>
+    </row>
+    <row r="16" spans="1:11" s="32" customFormat="1">
       <c r="A16" s="62" t="s">
         <v>25</v>
       </c>
@@ -2474,9 +2509,10 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16" s="66"/>
-      <c r="H16"/>
-    </row>
-    <row r="17" spans="1:12" s="32" customFormat="1">
+      <c r="H16" s="66"/>
+      <c r="I16"/>
+    </row>
+    <row r="17" spans="1:13" s="32" customFormat="1">
       <c r="A17" s="62" t="s">
         <v>37</v>
       </c>
@@ -2490,9 +2526,10 @@
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17" s="66"/>
-      <c r="H17"/>
-    </row>
-    <row r="18" spans="1:12" s="32" customFormat="1">
+      <c r="H17" s="66"/>
+      <c r="I17"/>
+    </row>
+    <row r="18" spans="1:13" s="32" customFormat="1">
       <c r="A18" s="62" t="s">
         <v>38</v>
       </c>
@@ -2504,9 +2541,10 @@
       <c r="E18"/>
       <c r="F18"/>
       <c r="G18" s="66"/>
-      <c r="H18"/>
-    </row>
-    <row r="19" spans="1:12" s="32" customFormat="1">
+      <c r="H18" s="66"/>
+      <c r="I18"/>
+    </row>
+    <row r="19" spans="1:13" s="32" customFormat="1">
       <c r="A19" s="62" t="s">
         <v>29</v>
       </c>
@@ -2520,9 +2558,10 @@
       <c r="E19"/>
       <c r="F19"/>
       <c r="G19" s="66"/>
-      <c r="H19"/>
-    </row>
-    <row r="20" spans="1:12" s="32" customFormat="1">
+      <c r="H19" s="66"/>
+      <c r="I19"/>
+    </row>
+    <row r="20" spans="1:13" s="32" customFormat="1">
       <c r="A20" s="62" t="s">
         <v>46</v>
       </c>
@@ -2536,9 +2575,10 @@
       <c r="E20"/>
       <c r="F20"/>
       <c r="G20" s="66"/>
-      <c r="H20"/>
-    </row>
-    <row r="21" spans="1:12" s="32" customFormat="1">
+      <c r="H20" s="66"/>
+      <c r="I20"/>
+    </row>
+    <row r="21" spans="1:13" s="32" customFormat="1">
       <c r="A21" s="62" t="s">
         <v>81</v>
       </c>
@@ -2552,9 +2592,10 @@
       <c r="E21"/>
       <c r="F21"/>
       <c r="G21" s="66"/>
-      <c r="H21"/>
-    </row>
-    <row r="22" spans="1:12" s="32" customFormat="1">
+      <c r="H21" s="66"/>
+      <c r="I21"/>
+    </row>
+    <row r="22" spans="1:13" s="32" customFormat="1">
       <c r="A22" s="87" t="s">
         <v>82</v>
       </c>
@@ -2568,9 +2609,10 @@
       <c r="E22"/>
       <c r="F22"/>
       <c r="G22" s="66"/>
-      <c r="H22"/>
-    </row>
-    <row r="23" spans="1:12" s="32" customFormat="1">
+      <c r="H22" s="66"/>
+      <c r="I22"/>
+    </row>
+    <row r="23" spans="1:13" s="32" customFormat="1">
       <c r="A23" s="62" t="s">
         <v>15</v>
       </c>
@@ -2582,9 +2624,10 @@
       <c r="E23"/>
       <c r="F23"/>
       <c r="G23" s="66"/>
-      <c r="H23"/>
-    </row>
-    <row r="24" spans="1:12" s="32" customFormat="1">
+      <c r="H23" s="66"/>
+      <c r="I23"/>
+    </row>
+    <row r="24" spans="1:13" s="32" customFormat="1">
       <c r="A24" s="87" t="s">
         <v>18</v>
       </c>
@@ -2598,9 +2641,10 @@
       <c r="E24"/>
       <c r="F24"/>
       <c r="G24" s="66"/>
-      <c r="H24"/>
-    </row>
-    <row r="25" spans="1:12" s="32" customFormat="1">
+      <c r="H24" s="66"/>
+      <c r="I24"/>
+    </row>
+    <row r="25" spans="1:13" s="32" customFormat="1">
       <c r="A25" s="87" t="s">
         <v>68</v>
       </c>
@@ -2612,9 +2656,10 @@
       <c r="E25"/>
       <c r="F25"/>
       <c r="G25" s="66"/>
-      <c r="H25"/>
-    </row>
-    <row r="26" spans="1:12" s="37" customFormat="1">
+      <c r="H25" s="66"/>
+      <c r="I25"/>
+    </row>
+    <row r="26" spans="1:13" s="37" customFormat="1">
       <c r="A26" s="34"/>
       <c r="B26" s="36"/>
       <c r="C26" s="34"/>
@@ -2625,8 +2670,9 @@
       <c r="H26" s="34"/>
       <c r="I26" s="34"/>
       <c r="J26" s="34"/>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="K26" s="34"/>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" s="30" t="s">
         <v>102</v>
       </c>
@@ -2639,12 +2685,13 @@
       </c>
       <c r="G27" s="44"/>
       <c r="H27" s="44"/>
-      <c r="I27" s="43"/>
+      <c r="I27" s="44"/>
       <c r="J27" s="43"/>
       <c r="K27" s="43"/>
       <c r="L27" s="43"/>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="M27" s="43"/>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" s="47" t="s">
         <v>7</v>
       </c>
@@ -2657,12 +2704,13 @@
       <c r="F28" s="67"/>
       <c r="G28" s="67"/>
       <c r="H28" s="67"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="45"/>
+      <c r="I28" s="67"/>
+      <c r="J28" s="44"/>
       <c r="K28" s="45"/>
-      <c r="L28" s="35"/>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="L28" s="45"/>
+      <c r="M28" s="35"/>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" s="51">
         <v>1</v>
       </c>
@@ -2674,13 +2722,14 @@
       <c r="E29" s="39"/>
       <c r="F29" s="68"/>
       <c r="G29" s="68"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="36"/>
+      <c r="H29" s="68"/>
+      <c r="I29" s="34"/>
       <c r="J29" s="36"/>
       <c r="K29" s="36"/>
-      <c r="L29" s="35"/>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="L29" s="36"/>
+      <c r="M29" s="35"/>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" s="51">
         <v>2</v>
       </c>
@@ -2692,13 +2741,14 @@
       <c r="E30" s="41"/>
       <c r="F30" s="68"/>
       <c r="G30" s="68"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="36"/>
+      <c r="H30" s="68"/>
+      <c r="I30" s="34"/>
       <c r="J30" s="36"/>
       <c r="K30" s="36"/>
-      <c r="L30" s="35"/>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="L30" s="36"/>
+      <c r="M30" s="35"/>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" s="52"/>
       <c r="B31" s="48"/>
       <c r="C31" s="49"/>
@@ -2706,13 +2756,14 @@
       <c r="E31" s="50"/>
       <c r="F31" s="68"/>
       <c r="G31" s="68"/>
-      <c r="H31" s="34"/>
-      <c r="I31" s="36"/>
+      <c r="H31" s="68"/>
+      <c r="I31" s="34"/>
       <c r="J31" s="36"/>
       <c r="K31" s="36"/>
-      <c r="L31" s="35"/>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="L31" s="36"/>
+      <c r="M31" s="35"/>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
@@ -2722,8 +2773,9 @@
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
       <c r="I32" s="13"/>
-    </row>
-    <row r="33" spans="1:12">
+      <c r="J32" s="13"/>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" s="30" t="s">
         <v>34</v>
       </c>
@@ -2736,12 +2788,13 @@
       </c>
       <c r="G33" s="44"/>
       <c r="H33" s="44"/>
-      <c r="I33" s="43"/>
+      <c r="I33" s="44"/>
       <c r="J33" s="43"/>
       <c r="K33" s="43"/>
       <c r="L33" s="43"/>
-    </row>
-    <row r="34" spans="1:12">
+      <c r="M33" s="43"/>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34" s="47" t="s">
         <v>7</v>
       </c>
@@ -2754,12 +2807,13 @@
       <c r="F34" s="67"/>
       <c r="G34" s="67"/>
       <c r="H34" s="67"/>
-      <c r="I34" s="44"/>
-      <c r="J34" s="45"/>
+      <c r="I34" s="67"/>
+      <c r="J34" s="44"/>
       <c r="K34" s="45"/>
-      <c r="L34" s="35"/>
-    </row>
-    <row r="35" spans="1:12">
+      <c r="L34" s="45"/>
+      <c r="M34" s="35"/>
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35" s="51">
         <v>1</v>
       </c>
@@ -2771,13 +2825,14 @@
       <c r="E35" s="39"/>
       <c r="F35" s="68"/>
       <c r="G35" s="68"/>
-      <c r="H35" s="34"/>
-      <c r="I35" s="36"/>
+      <c r="H35" s="68"/>
+      <c r="I35" s="34"/>
       <c r="J35" s="36"/>
       <c r="K35" s="36"/>
-      <c r="L35" s="35"/>
-    </row>
-    <row r="36" spans="1:12">
+      <c r="L35" s="36"/>
+      <c r="M35" s="35"/>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36" s="51">
         <v>2</v>
       </c>
@@ -2789,13 +2844,14 @@
       <c r="E36" s="41"/>
       <c r="F36" s="68"/>
       <c r="G36" s="68"/>
-      <c r="H36" s="34"/>
-      <c r="I36" s="36"/>
+      <c r="H36" s="68"/>
+      <c r="I36" s="34"/>
       <c r="J36" s="36"/>
       <c r="K36" s="36"/>
-      <c r="L36" s="35"/>
-    </row>
-    <row r="37" spans="1:12">
+      <c r="L36" s="36"/>
+      <c r="M36" s="35"/>
+    </row>
+    <row r="37" spans="1:13">
       <c r="A37" s="52"/>
       <c r="B37" s="48"/>
       <c r="C37" s="49"/>
@@ -2803,13 +2859,14 @@
       <c r="E37" s="50"/>
       <c r="F37" s="68"/>
       <c r="G37" s="68"/>
-      <c r="H37" s="34"/>
-      <c r="I37" s="36"/>
+      <c r="H37" s="68"/>
+      <c r="I37" s="34"/>
       <c r="J37" s="36"/>
       <c r="K37" s="36"/>
-      <c r="L37" s="35"/>
-    </row>
-    <row r="38" spans="1:12">
+      <c r="L37" s="36"/>
+      <c r="M37" s="35"/>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38" s="83"/>
       <c r="B38" s="84"/>
       <c r="C38" s="85"/>
@@ -2817,13 +2874,14 @@
       <c r="E38" s="85"/>
       <c r="F38" s="68"/>
       <c r="G38" s="68"/>
-      <c r="H38" s="34"/>
-      <c r="I38" s="36"/>
+      <c r="H38" s="68"/>
+      <c r="I38" s="34"/>
       <c r="J38" s="36"/>
       <c r="K38" s="36"/>
-      <c r="L38" s="35"/>
-    </row>
-    <row r="39" spans="1:12">
+      <c r="L38" s="36"/>
+      <c r="M38" s="35"/>
+    </row>
+    <row r="39" spans="1:13">
       <c r="A39" s="30" t="s">
         <v>103</v>
       </c>
@@ -2836,12 +2894,13 @@
       </c>
       <c r="G39" s="44"/>
       <c r="H39" s="44"/>
-      <c r="I39" s="43"/>
+      <c r="I39" s="44"/>
       <c r="J39" s="43"/>
       <c r="K39" s="43"/>
       <c r="L39" s="43"/>
-    </row>
-    <row r="40" spans="1:12">
+      <c r="M39" s="43"/>
+    </row>
+    <row r="40" spans="1:13">
       <c r="A40" s="47" t="s">
         <v>7</v>
       </c>
@@ -2854,12 +2913,13 @@
       <c r="F40" s="67"/>
       <c r="G40" s="67"/>
       <c r="H40" s="67"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="45"/>
+      <c r="I40" s="67"/>
+      <c r="J40" s="44"/>
       <c r="K40" s="45"/>
-      <c r="L40" s="35"/>
-    </row>
-    <row r="41" spans="1:12">
+      <c r="L40" s="45"/>
+      <c r="M40" s="35"/>
+    </row>
+    <row r="41" spans="1:13">
       <c r="A41" s="51">
         <v>1</v>
       </c>
@@ -2871,13 +2931,14 @@
       <c r="E41" s="39"/>
       <c r="F41" s="68"/>
       <c r="G41" s="68"/>
-      <c r="H41" s="34"/>
-      <c r="I41" s="36"/>
+      <c r="H41" s="68"/>
+      <c r="I41" s="34"/>
       <c r="J41" s="36"/>
       <c r="K41" s="36"/>
-      <c r="L41" s="35"/>
-    </row>
-    <row r="42" spans="1:12">
+      <c r="L41" s="36"/>
+      <c r="M41" s="35"/>
+    </row>
+    <row r="42" spans="1:13">
       <c r="A42" s="51">
         <v>2</v>
       </c>
@@ -2889,13 +2950,14 @@
       <c r="E42" s="41"/>
       <c r="F42" s="68"/>
       <c r="G42" s="68"/>
-      <c r="H42" s="34"/>
-      <c r="I42" s="36"/>
+      <c r="H42" s="68"/>
+      <c r="I42" s="34"/>
       <c r="J42" s="36"/>
       <c r="K42" s="36"/>
-      <c r="L42" s="35"/>
-    </row>
-    <row r="43" spans="1:12">
+      <c r="L42" s="36"/>
+      <c r="M42" s="35"/>
+    </row>
+    <row r="43" spans="1:13">
       <c r="A43" s="52"/>
       <c r="B43" s="48"/>
       <c r="C43" s="49"/>
@@ -2903,13 +2965,14 @@
       <c r="E43" s="50"/>
       <c r="F43" s="68"/>
       <c r="G43" s="68"/>
-      <c r="H43" s="34"/>
-      <c r="I43" s="36"/>
+      <c r="H43" s="68"/>
+      <c r="I43" s="34"/>
       <c r="J43" s="36"/>
       <c r="K43" s="36"/>
-      <c r="L43" s="35"/>
-    </row>
-    <row r="44" spans="1:12">
+      <c r="L43" s="36"/>
+      <c r="M43" s="35"/>
+    </row>
+    <row r="44" spans="1:13">
       <c r="A44" s="13"/>
       <c r="B44" s="13"/>
       <c r="C44" s="13"/>
@@ -2919,8 +2982,9 @@
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
       <c r="I44" s="13"/>
-    </row>
-    <row r="45" spans="1:12">
+      <c r="J44" s="13"/>
+    </row>
+    <row r="45" spans="1:13">
       <c r="A45" s="30" t="s">
         <v>84</v>
       </c>
@@ -2933,12 +2997,13 @@
       </c>
       <c r="G45" s="44"/>
       <c r="H45" s="44"/>
-      <c r="I45" s="43"/>
+      <c r="I45" s="44"/>
       <c r="J45" s="43"/>
       <c r="K45" s="43"/>
       <c r="L45" s="43"/>
-    </row>
-    <row r="46" spans="1:12">
+      <c r="M45" s="43"/>
+    </row>
+    <row r="46" spans="1:13">
       <c r="A46" s="47" t="s">
         <v>7</v>
       </c>
@@ -2955,12 +3020,13 @@
       <c r="F46" s="67"/>
       <c r="G46" s="67"/>
       <c r="H46" s="67"/>
-      <c r="I46" s="44"/>
-      <c r="J46" s="45"/>
+      <c r="I46" s="67"/>
+      <c r="J46" s="44"/>
       <c r="K46" s="45"/>
-      <c r="L46" s="35"/>
-    </row>
-    <row r="47" spans="1:12">
+      <c r="L46" s="45"/>
+      <c r="M46" s="35"/>
+    </row>
+    <row r="47" spans="1:13">
       <c r="A47" s="51">
         <v>1</v>
       </c>
@@ -2976,13 +3042,14 @@
       <c r="E47" s="39"/>
       <c r="F47" s="68"/>
       <c r="G47" s="68"/>
-      <c r="H47" s="34"/>
-      <c r="I47" s="36"/>
+      <c r="H47" s="68"/>
+      <c r="I47" s="34"/>
       <c r="J47" s="36"/>
       <c r="K47" s="36"/>
-      <c r="L47" s="35"/>
-    </row>
-    <row r="48" spans="1:12">
+      <c r="L47" s="36"/>
+      <c r="M47" s="35"/>
+    </row>
+    <row r="48" spans="1:13">
       <c r="A48" s="51">
         <v>2</v>
       </c>
@@ -2998,13 +3065,14 @@
       <c r="E48" s="41"/>
       <c r="F48" s="68"/>
       <c r="G48" s="68"/>
-      <c r="H48" s="34"/>
-      <c r="I48" s="36"/>
+      <c r="H48" s="68"/>
+      <c r="I48" s="34"/>
       <c r="J48" s="36"/>
       <c r="K48" s="36"/>
-      <c r="L48" s="35"/>
-    </row>
-    <row r="49" spans="1:12">
+      <c r="L48" s="36"/>
+      <c r="M48" s="35"/>
+    </row>
+    <row r="49" spans="1:13">
       <c r="A49" s="52"/>
       <c r="B49" s="48"/>
       <c r="C49" s="100"/>
@@ -3012,13 +3080,14 @@
       <c r="E49" s="50"/>
       <c r="F49" s="68"/>
       <c r="G49" s="68"/>
-      <c r="H49" s="34"/>
-      <c r="I49" s="36"/>
+      <c r="H49" s="68"/>
+      <c r="I49" s="34"/>
       <c r="J49" s="36"/>
       <c r="K49" s="36"/>
-      <c r="L49" s="35"/>
-    </row>
-    <row r="50" spans="1:12">
+      <c r="L49" s="36"/>
+      <c r="M49" s="35"/>
+    </row>
+    <row r="50" spans="1:13">
       <c r="A50" s="83"/>
       <c r="B50" s="84"/>
       <c r="C50" s="85"/>
@@ -3026,13 +3095,14 @@
       <c r="E50" s="85"/>
       <c r="F50" s="68"/>
       <c r="G50" s="68"/>
-      <c r="H50" s="34"/>
-      <c r="I50" s="36"/>
+      <c r="H50" s="68"/>
+      <c r="I50" s="34"/>
       <c r="J50" s="36"/>
       <c r="K50" s="36"/>
-      <c r="L50" s="35"/>
-    </row>
-    <row r="51" spans="1:12">
+      <c r="L50" s="36"/>
+      <c r="M50" s="35"/>
+    </row>
+    <row r="51" spans="1:13">
       <c r="A51" s="30" t="s">
         <v>106</v>
       </c>
@@ -3045,12 +3115,13 @@
       </c>
       <c r="G51" s="44"/>
       <c r="H51" s="44"/>
-      <c r="I51" s="43"/>
+      <c r="I51" s="44"/>
       <c r="J51" s="43"/>
       <c r="K51" s="43"/>
       <c r="L51" s="43"/>
-    </row>
-    <row r="52" spans="1:12">
+      <c r="M51" s="43"/>
+    </row>
+    <row r="52" spans="1:13">
       <c r="A52" s="47" t="s">
         <v>7</v>
       </c>
@@ -3065,12 +3136,13 @@
       </c>
       <c r="G52" s="67"/>
       <c r="H52" s="67"/>
-      <c r="I52" s="44"/>
-      <c r="J52" s="45"/>
+      <c r="I52" s="67"/>
+      <c r="J52" s="44"/>
       <c r="K52" s="45"/>
-      <c r="L52" s="35"/>
-    </row>
-    <row r="53" spans="1:12">
+      <c r="L52" s="45"/>
+      <c r="M52" s="35"/>
+    </row>
+    <row r="53" spans="1:13">
       <c r="A53" s="51"/>
       <c r="B53" s="46"/>
       <c r="C53" s="38"/>
@@ -3078,13 +3150,14 @@
       <c r="E53" s="39"/>
       <c r="F53" s="68"/>
       <c r="G53" s="68"/>
-      <c r="H53" s="34"/>
-      <c r="I53" s="36"/>
+      <c r="H53" s="68"/>
+      <c r="I53" s="34"/>
       <c r="J53" s="36"/>
       <c r="K53" s="36"/>
-      <c r="L53" s="35"/>
-    </row>
-    <row r="54" spans="1:12">
+      <c r="L53" s="36"/>
+      <c r="M53" s="35"/>
+    </row>
+    <row r="54" spans="1:13">
       <c r="A54" s="51"/>
       <c r="B54" s="46"/>
       <c r="C54" s="40"/>
@@ -3092,13 +3165,14 @@
       <c r="E54" s="41"/>
       <c r="F54" s="68"/>
       <c r="G54" s="68"/>
-      <c r="H54" s="34"/>
-      <c r="I54" s="36"/>
+      <c r="H54" s="68"/>
+      <c r="I54" s="34"/>
       <c r="J54" s="36"/>
       <c r="K54" s="36"/>
-      <c r="L54" s="35"/>
-    </row>
-    <row r="55" spans="1:12">
+      <c r="L54" s="36"/>
+      <c r="M54" s="35"/>
+    </row>
+    <row r="55" spans="1:13">
       <c r="A55" s="52"/>
       <c r="B55" s="48"/>
       <c r="C55" s="49"/>
@@ -3106,13 +3180,14 @@
       <c r="E55" s="50"/>
       <c r="F55" s="68"/>
       <c r="G55" s="68"/>
-      <c r="H55" s="34"/>
-      <c r="I55" s="36"/>
+      <c r="H55" s="68"/>
+      <c r="I55" s="34"/>
       <c r="J55" s="36"/>
       <c r="K55" s="36"/>
-      <c r="L55" s="35"/>
-    </row>
-    <row r="56" spans="1:12">
+      <c r="L55" s="36"/>
+      <c r="M55" s="35"/>
+    </row>
+    <row r="56" spans="1:13">
       <c r="A56" s="13"/>
       <c r="B56" s="13"/>
       <c r="C56" s="13"/>
@@ -3122,8 +3197,9 @@
       <c r="G56" s="13"/>
       <c r="H56" s="13"/>
       <c r="I56" s="13"/>
-    </row>
-    <row r="57" spans="1:12">
+      <c r="J56" s="13"/>
+    </row>
+    <row r="57" spans="1:13">
       <c r="A57" s="13"/>
       <c r="B57" s="13" t="s">
         <v>83</v>
@@ -3135,8 +3211,9 @@
       <c r="G57" s="13"/>
       <c r="H57" s="13"/>
       <c r="I57" s="13"/>
-    </row>
-    <row r="58" spans="1:12">
+      <c r="J57" s="13"/>
+    </row>
+    <row r="58" spans="1:13">
       <c r="A58" s="3" t="s">
         <v>107</v>
       </c>
@@ -3149,10 +3226,11 @@
       <c r="H58" s="14"/>
       <c r="I58" s="14"/>
       <c r="J58" s="14"/>
-      <c r="K58" s="6"/>
-      <c r="L58" s="15"/>
-    </row>
-    <row r="59" spans="1:12" ht="13.5" customHeight="1">
+      <c r="K58" s="14"/>
+      <c r="L58" s="6"/>
+      <c r="M58" s="15"/>
+    </row>
+    <row r="59" spans="1:13" ht="13.5" customHeight="1">
       <c r="A59" s="90" t="s">
         <v>7</v>
       </c>
@@ -3174,15 +3252,18 @@
       <c r="G59" s="91" t="s">
         <v>16</v>
       </c>
-      <c r="H59" s="89" t="s">
+      <c r="H59" s="108" t="s">
+        <v>118</v>
+      </c>
+      <c r="I59" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="I59" s="89"/>
-      <c r="J59" s="16"/>
-      <c r="K59" s="17"/>
-      <c r="L59" s="9"/>
-    </row>
-    <row r="60" spans="1:12">
+      <c r="J59" s="89"/>
+      <c r="K59" s="16"/>
+      <c r="L59" s="17"/>
+      <c r="M59" s="9"/>
+    </row>
+    <row r="60" spans="1:13">
       <c r="A60" s="90"/>
       <c r="B60" s="90"/>
       <c r="C60" s="89"/>
@@ -3190,13 +3271,14 @@
       <c r="E60" s="89"/>
       <c r="F60" s="92"/>
       <c r="G60" s="92"/>
-      <c r="H60" s="89"/>
+      <c r="H60" s="109"/>
       <c r="I60" s="89"/>
-      <c r="J60" s="18"/>
-      <c r="K60" s="29"/>
-      <c r="L60" s="15"/>
-    </row>
-    <row r="61" spans="1:12">
+      <c r="J60" s="89"/>
+      <c r="K60" s="18"/>
+      <c r="L60" s="29"/>
+      <c r="M60" s="15"/>
+    </row>
+    <row r="61" spans="1:13">
       <c r="A61" s="19">
         <v>1</v>
       </c>
@@ -3214,15 +3296,16 @@
         <v>14</v>
       </c>
       <c r="G61" s="69"/>
-      <c r="H61" s="20" t="s">
+      <c r="H61" s="69"/>
+      <c r="I61" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="I61" s="21"/>
       <c r="J61" s="21"/>
-      <c r="K61" s="28"/>
-      <c r="L61" s="15"/>
-    </row>
-    <row r="62" spans="1:12">
+      <c r="K61" s="21"/>
+      <c r="L61" s="28"/>
+      <c r="M61" s="15"/>
+    </row>
+    <row r="62" spans="1:13">
       <c r="A62" s="19">
         <f>A61+1</f>
         <v>2</v>
@@ -3239,15 +3322,16 @@
       </c>
       <c r="F62" s="20"/>
       <c r="G62" s="69"/>
-      <c r="H62" s="20" t="s">
+      <c r="H62" s="69"/>
+      <c r="I62" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="I62" s="21"/>
       <c r="J62" s="21"/>
-      <c r="K62" s="28"/>
-      <c r="L62" s="15"/>
-    </row>
-    <row r="63" spans="1:12">
+      <c r="K62" s="21"/>
+      <c r="L62" s="28"/>
+      <c r="M62" s="15"/>
+    </row>
+    <row r="63" spans="1:13">
       <c r="A63" s="19">
         <f t="shared" ref="A63:A77" si="0">A62+1</f>
         <v>3</v>
@@ -3266,15 +3350,16 @@
       <c r="G63" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="H63" s="20" t="s">
+      <c r="H63" s="69"/>
+      <c r="I63" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="I63" s="21"/>
       <c r="J63" s="21"/>
-      <c r="K63" s="22"/>
-      <c r="L63" s="15"/>
-    </row>
-    <row r="64" spans="1:12">
+      <c r="K63" s="21"/>
+      <c r="L63" s="22"/>
+      <c r="M63" s="15"/>
+    </row>
+    <row r="64" spans="1:13">
       <c r="A64" s="19">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3291,32 +3376,44 @@
       <c r="G64" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="H64" s="20" t="s">
+      <c r="H64" s="69"/>
+      <c r="I64" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="I64" s="21"/>
       <c r="J64" s="21"/>
-      <c r="K64" s="22"/>
-      <c r="L64" s="15"/>
-    </row>
-    <row r="65" spans="1:12">
+      <c r="K64" s="21"/>
+      <c r="L64" s="22"/>
+      <c r="M64" s="15"/>
+    </row>
+    <row r="65" spans="1:13">
       <c r="A65" s="19">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B65" s="73"/>
-      <c r="C65" s="80"/>
+      <c r="B65" s="73" t="s">
+        <v>119</v>
+      </c>
+      <c r="C65" s="80" t="s">
+        <v>48</v>
+      </c>
       <c r="D65" s="20"/>
       <c r="E65" s="20"/>
       <c r="F65" s="20"/>
-      <c r="G65" s="69"/>
-      <c r="H65" s="20"/>
-      <c r="I65" s="21"/>
+      <c r="G65" s="69" t="s">
+        <v>14</v>
+      </c>
+      <c r="H65" s="69" t="s">
+        <v>119</v>
+      </c>
+      <c r="I65" s="20" t="s">
+        <v>120</v>
+      </c>
       <c r="J65" s="21"/>
-      <c r="K65" s="22"/>
-      <c r="L65" s="15"/>
-    </row>
-    <row r="66" spans="1:12">
+      <c r="K65" s="21"/>
+      <c r="L65" s="22"/>
+      <c r="M65" s="15"/>
+    </row>
+    <row r="66" spans="1:13">
       <c r="A66" s="19">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3327,13 +3424,14 @@
       <c r="E66" s="74"/>
       <c r="F66" s="74"/>
       <c r="G66" s="75"/>
-      <c r="H66" s="74"/>
-      <c r="I66" s="76"/>
+      <c r="H66" s="75"/>
+      <c r="I66" s="74"/>
       <c r="J66" s="76"/>
-      <c r="K66" s="77"/>
-      <c r="L66" s="15"/>
-    </row>
-    <row r="67" spans="1:12">
+      <c r="K66" s="76"/>
+      <c r="L66" s="77"/>
+      <c r="M66" s="15"/>
+    </row>
+    <row r="67" spans="1:13">
       <c r="A67" s="19">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3344,13 +3442,14 @@
       <c r="E67" s="20"/>
       <c r="F67" s="20"/>
       <c r="G67" s="69"/>
-      <c r="H67" s="20"/>
-      <c r="I67" s="21"/>
+      <c r="H67" s="69"/>
+      <c r="I67" s="20"/>
       <c r="J67" s="21"/>
-      <c r="K67" s="22"/>
-      <c r="L67" s="15"/>
-    </row>
-    <row r="68" spans="1:12">
+      <c r="K67" s="21"/>
+      <c r="L67" s="22"/>
+      <c r="M67" s="15"/>
+    </row>
+    <row r="68" spans="1:13">
       <c r="A68" s="19">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -3361,13 +3460,14 @@
       <c r="E68" s="74"/>
       <c r="F68" s="74"/>
       <c r="G68" s="75"/>
-      <c r="H68" s="74"/>
-      <c r="I68" s="76"/>
+      <c r="H68" s="75"/>
+      <c r="I68" s="74"/>
       <c r="J68" s="76"/>
-      <c r="K68" s="77"/>
-      <c r="L68" s="15"/>
-    </row>
-    <row r="69" spans="1:12">
+      <c r="K68" s="76"/>
+      <c r="L68" s="77"/>
+      <c r="M68" s="15"/>
+    </row>
+    <row r="69" spans="1:13">
       <c r="A69" s="19">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3378,13 +3478,14 @@
       <c r="E69" s="74"/>
       <c r="F69" s="74"/>
       <c r="G69" s="75"/>
-      <c r="H69" s="74"/>
-      <c r="I69" s="76"/>
+      <c r="H69" s="75"/>
+      <c r="I69" s="74"/>
       <c r="J69" s="76"/>
-      <c r="K69" s="77"/>
-      <c r="L69" s="15"/>
-    </row>
-    <row r="70" spans="1:12">
+      <c r="K69" s="76"/>
+      <c r="L69" s="77"/>
+      <c r="M69" s="15"/>
+    </row>
+    <row r="70" spans="1:13">
       <c r="A70" s="19">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -3395,13 +3496,14 @@
       <c r="E70" s="20"/>
       <c r="F70" s="20"/>
       <c r="G70" s="69"/>
-      <c r="H70" s="20"/>
-      <c r="I70" s="21"/>
+      <c r="H70" s="69"/>
+      <c r="I70" s="20"/>
       <c r="J70" s="21"/>
-      <c r="K70" s="22"/>
-      <c r="L70" s="15"/>
-    </row>
-    <row r="71" spans="1:12">
+      <c r="K70" s="21"/>
+      <c r="L70" s="22"/>
+      <c r="M70" s="15"/>
+    </row>
+    <row r="71" spans="1:13">
       <c r="A71" s="19">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -3412,13 +3514,14 @@
       <c r="E71" s="74"/>
       <c r="F71" s="74"/>
       <c r="G71" s="75"/>
-      <c r="H71" s="74"/>
-      <c r="I71" s="76"/>
+      <c r="H71" s="75"/>
+      <c r="I71" s="74"/>
       <c r="J71" s="76"/>
-      <c r="K71" s="77"/>
-      <c r="L71" s="15"/>
-    </row>
-    <row r="72" spans="1:12">
+      <c r="K71" s="76"/>
+      <c r="L71" s="77"/>
+      <c r="M71" s="15"/>
+    </row>
+    <row r="72" spans="1:13">
       <c r="A72" s="19">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -3429,13 +3532,14 @@
       <c r="E72" s="74"/>
       <c r="F72" s="74"/>
       <c r="G72" s="75"/>
-      <c r="H72" s="74"/>
-      <c r="I72" s="76"/>
+      <c r="H72" s="75"/>
+      <c r="I72" s="74"/>
       <c r="J72" s="76"/>
-      <c r="K72" s="77"/>
-      <c r="L72" s="15"/>
-    </row>
-    <row r="73" spans="1:12">
+      <c r="K72" s="76"/>
+      <c r="L72" s="77"/>
+      <c r="M72" s="15"/>
+    </row>
+    <row r="73" spans="1:13">
       <c r="A73" s="19">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -3446,13 +3550,14 @@
       <c r="E73" s="20"/>
       <c r="F73" s="20"/>
       <c r="G73" s="69"/>
-      <c r="H73" s="20"/>
-      <c r="I73" s="21"/>
+      <c r="H73" s="69"/>
+      <c r="I73" s="20"/>
       <c r="J73" s="21"/>
-      <c r="K73" s="22"/>
-      <c r="L73" s="15"/>
-    </row>
-    <row r="74" spans="1:12">
+      <c r="K73" s="21"/>
+      <c r="L73" s="22"/>
+      <c r="M73" s="15"/>
+    </row>
+    <row r="74" spans="1:13">
       <c r="A74" s="19">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3463,13 +3568,14 @@
       <c r="E74" s="74"/>
       <c r="F74" s="74"/>
       <c r="G74" s="75"/>
-      <c r="H74" s="74"/>
-      <c r="I74" s="76"/>
+      <c r="H74" s="75"/>
+      <c r="I74" s="74"/>
       <c r="J74" s="76"/>
-      <c r="K74" s="77"/>
-      <c r="L74" s="15"/>
-    </row>
-    <row r="75" spans="1:12">
+      <c r="K74" s="76"/>
+      <c r="L74" s="77"/>
+      <c r="M74" s="15"/>
+    </row>
+    <row r="75" spans="1:13">
       <c r="A75" s="19">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -3480,13 +3586,14 @@
       <c r="E75" s="74"/>
       <c r="F75" s="74"/>
       <c r="G75" s="75"/>
-      <c r="H75" s="74"/>
-      <c r="I75" s="76"/>
+      <c r="H75" s="75"/>
+      <c r="I75" s="74"/>
       <c r="J75" s="76"/>
-      <c r="K75" s="77"/>
-      <c r="L75" s="15"/>
-    </row>
-    <row r="76" spans="1:12">
+      <c r="K75" s="76"/>
+      <c r="L75" s="77"/>
+      <c r="M75" s="15"/>
+    </row>
+    <row r="76" spans="1:13">
       <c r="A76" s="19">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3497,13 +3604,14 @@
       <c r="E76" s="20"/>
       <c r="F76" s="20"/>
       <c r="G76" s="69"/>
-      <c r="H76" s="20"/>
-      <c r="I76" s="21"/>
+      <c r="H76" s="69"/>
+      <c r="I76" s="20"/>
       <c r="J76" s="21"/>
-      <c r="K76" s="22"/>
-      <c r="L76" s="15"/>
-    </row>
-    <row r="77" spans="1:12">
+      <c r="K76" s="21"/>
+      <c r="L76" s="22"/>
+      <c r="M76" s="15"/>
+    </row>
+    <row r="77" spans="1:13">
       <c r="A77" s="19">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3514,13 +3622,14 @@
       <c r="E77" s="74"/>
       <c r="F77" s="74"/>
       <c r="G77" s="75"/>
-      <c r="H77" s="74"/>
-      <c r="I77" s="76"/>
+      <c r="H77" s="75"/>
+      <c r="I77" s="74"/>
       <c r="J77" s="76"/>
-      <c r="K77" s="77"/>
-      <c r="L77" s="15"/>
-    </row>
-    <row r="78" spans="1:12">
+      <c r="K77" s="76"/>
+      <c r="L77" s="77"/>
+      <c r="M77" s="15"/>
+    </row>
+    <row r="78" spans="1:13">
       <c r="A78" s="23"/>
       <c r="B78" s="24"/>
       <c r="C78" s="25"/>
@@ -3528,13 +3637,14 @@
       <c r="E78" s="25"/>
       <c r="F78" s="25"/>
       <c r="G78" s="70"/>
-      <c r="H78" s="25"/>
-      <c r="I78" s="26"/>
+      <c r="H78" s="70"/>
+      <c r="I78" s="25"/>
       <c r="J78" s="26"/>
-      <c r="K78" s="27"/>
-      <c r="L78" s="15"/>
-    </row>
-    <row r="80" spans="1:12">
+      <c r="K78" s="26"/>
+      <c r="L78" s="27"/>
+      <c r="M78" s="15"/>
+    </row>
+    <row r="80" spans="1:13">
       <c r="A80" s="30" t="s">
         <v>108</v>
       </c>
@@ -3547,12 +3657,13 @@
       </c>
       <c r="G80" s="44"/>
       <c r="H80" s="44"/>
-      <c r="I80" s="43"/>
+      <c r="I80" s="44"/>
       <c r="J80" s="43"/>
       <c r="K80" s="43"/>
       <c r="L80" s="43"/>
-    </row>
-    <row r="81" spans="1:12">
+      <c r="M80" s="43"/>
+    </row>
+    <row r="81" spans="1:13">
       <c r="A81" s="47" t="s">
         <v>7</v>
       </c>
@@ -3565,12 +3676,13 @@
       <c r="F81" s="67"/>
       <c r="G81" s="67"/>
       <c r="H81" s="67"/>
-      <c r="I81" s="44"/>
-      <c r="J81" s="45"/>
+      <c r="I81" s="67"/>
+      <c r="J81" s="44"/>
       <c r="K81" s="45"/>
-      <c r="L81" s="35"/>
-    </row>
-    <row r="82" spans="1:12">
+      <c r="L81" s="45"/>
+      <c r="M81" s="35"/>
+    </row>
+    <row r="82" spans="1:13">
       <c r="A82" s="51"/>
       <c r="B82" s="46"/>
       <c r="C82" s="38"/>
@@ -3578,13 +3690,14 @@
       <c r="E82" s="39"/>
       <c r="F82" s="68"/>
       <c r="G82" s="68"/>
-      <c r="H82" s="34"/>
-      <c r="I82" s="36"/>
+      <c r="H82" s="68"/>
+      <c r="I82" s="34"/>
       <c r="J82" s="36"/>
       <c r="K82" s="36"/>
-      <c r="L82" s="35"/>
-    </row>
-    <row r="83" spans="1:12">
+      <c r="L82" s="36"/>
+      <c r="M82" s="35"/>
+    </row>
+    <row r="83" spans="1:13">
       <c r="A83" s="51"/>
       <c r="B83" s="46"/>
       <c r="C83" s="40"/>
@@ -3592,13 +3705,14 @@
       <c r="E83" s="41"/>
       <c r="F83" s="68"/>
       <c r="G83" s="68"/>
-      <c r="H83" s="34"/>
-      <c r="I83" s="36"/>
+      <c r="H83" s="68"/>
+      <c r="I83" s="34"/>
       <c r="J83" s="36"/>
       <c r="K83" s="36"/>
-      <c r="L83" s="35"/>
-    </row>
-    <row r="84" spans="1:12">
+      <c r="L83" s="36"/>
+      <c r="M83" s="35"/>
+    </row>
+    <row r="84" spans="1:13">
       <c r="A84" s="52"/>
       <c r="B84" s="48"/>
       <c r="C84" s="49"/>
@@ -3606,13 +3720,14 @@
       <c r="E84" s="50"/>
       <c r="F84" s="68"/>
       <c r="G84" s="68"/>
-      <c r="H84" s="34"/>
-      <c r="I84" s="36"/>
+      <c r="H84" s="68"/>
+      <c r="I84" s="34"/>
       <c r="J84" s="36"/>
       <c r="K84" s="36"/>
-      <c r="L84" s="35"/>
-    </row>
-    <row r="85" spans="1:12">
+      <c r="L84" s="36"/>
+      <c r="M84" s="35"/>
+    </row>
+    <row r="85" spans="1:13">
       <c r="A85" s="13"/>
       <c r="B85" s="13"/>
       <c r="C85" s="13"/>
@@ -3622,8 +3737,9 @@
       <c r="G85" s="13"/>
       <c r="H85" s="13"/>
       <c r="I85" s="13"/>
-    </row>
-    <row r="86" spans="1:12">
+      <c r="J85" s="13"/>
+    </row>
+    <row r="86" spans="1:13">
       <c r="A86" s="13"/>
       <c r="B86" s="13" t="s">
         <v>95</v>
@@ -3635,8 +3751,9 @@
       <c r="G86" s="13"/>
       <c r="H86" s="13"/>
       <c r="I86" s="13"/>
-    </row>
-    <row r="87" spans="1:12">
+      <c r="J86" s="13"/>
+    </row>
+    <row r="87" spans="1:13">
       <c r="A87" s="3" t="s">
         <v>93</v>
       </c>
@@ -3649,10 +3766,11 @@
       <c r="H87" s="14"/>
       <c r="I87" s="14"/>
       <c r="J87" s="14"/>
-      <c r="K87" s="6"/>
-      <c r="L87" s="15"/>
-    </row>
-    <row r="88" spans="1:12" ht="13.5" customHeight="1">
+      <c r="K87" s="14"/>
+      <c r="L87" s="6"/>
+      <c r="M87" s="15"/>
+    </row>
+    <row r="88" spans="1:13" ht="13.5" customHeight="1">
       <c r="A88" s="90" t="s">
         <v>7</v>
       </c>
@@ -3670,13 +3788,14 @@
       </c>
       <c r="F88" s="101"/>
       <c r="G88" s="101"/>
-      <c r="H88" s="105"/>
-      <c r="I88" s="89"/>
-      <c r="J88" s="16"/>
-      <c r="K88" s="17"/>
-      <c r="L88" s="9"/>
-    </row>
-    <row r="89" spans="1:12">
+      <c r="H88" s="101"/>
+      <c r="I88" s="105"/>
+      <c r="J88" s="89"/>
+      <c r="K88" s="16"/>
+      <c r="L88" s="17"/>
+      <c r="M88" s="9"/>
+    </row>
+    <row r="89" spans="1:13">
       <c r="A89" s="90"/>
       <c r="B89" s="90"/>
       <c r="C89" s="89"/>
@@ -3684,13 +3803,14 @@
       <c r="E89" s="89"/>
       <c r="F89" s="102"/>
       <c r="G89" s="102"/>
-      <c r="H89" s="105"/>
-      <c r="I89" s="89"/>
-      <c r="J89" s="18"/>
-      <c r="K89" s="29"/>
-      <c r="L89" s="15"/>
-    </row>
-    <row r="90" spans="1:12">
+      <c r="H89" s="102"/>
+      <c r="I89" s="105"/>
+      <c r="J89" s="89"/>
+      <c r="K89" s="18"/>
+      <c r="L89" s="29"/>
+      <c r="M89" s="15"/>
+    </row>
+    <row r="90" spans="1:13">
       <c r="A90" s="19">
         <v>1</v>
       </c>
@@ -3706,13 +3826,14 @@
       </c>
       <c r="F90" s="103"/>
       <c r="G90" s="106"/>
-      <c r="H90" s="103"/>
-      <c r="I90" s="21"/>
+      <c r="H90" s="106"/>
+      <c r="I90" s="103"/>
       <c r="J90" s="21"/>
-      <c r="K90" s="28"/>
-      <c r="L90" s="15"/>
-    </row>
-    <row r="91" spans="1:12">
+      <c r="K90" s="21"/>
+      <c r="L90" s="28"/>
+      <c r="M90" s="15"/>
+    </row>
+    <row r="91" spans="1:13">
       <c r="A91" s="19">
         <f>A90+1</f>
         <v>2</v>
@@ -3729,13 +3850,14 @@
       </c>
       <c r="F91" s="103"/>
       <c r="G91" s="106"/>
-      <c r="H91" s="103"/>
-      <c r="I91" s="21"/>
+      <c r="H91" s="106"/>
+      <c r="I91" s="103"/>
       <c r="J91" s="21"/>
-      <c r="K91" s="28"/>
-      <c r="L91" s="15"/>
-    </row>
-    <row r="92" spans="1:12">
+      <c r="K91" s="21"/>
+      <c r="L91" s="28"/>
+      <c r="M91" s="15"/>
+    </row>
+    <row r="92" spans="1:13">
       <c r="A92" s="19">
         <f t="shared" ref="A92:A96" si="1">A91+1</f>
         <v>3</v>
@@ -3754,13 +3876,14 @@
       </c>
       <c r="F92" s="103"/>
       <c r="G92" s="106"/>
-      <c r="H92" s="103"/>
-      <c r="I92" s="21"/>
+      <c r="H92" s="106"/>
+      <c r="I92" s="103"/>
       <c r="J92" s="21"/>
-      <c r="K92" s="22"/>
-      <c r="L92" s="15"/>
-    </row>
-    <row r="93" spans="1:12">
+      <c r="K92" s="21"/>
+      <c r="L92" s="22"/>
+      <c r="M92" s="15"/>
+    </row>
+    <row r="93" spans="1:13">
       <c r="A93" s="19">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -3771,13 +3894,14 @@
       <c r="E93" s="20"/>
       <c r="F93" s="103"/>
       <c r="G93" s="106"/>
-      <c r="H93" s="103"/>
-      <c r="I93" s="21"/>
+      <c r="H93" s="106"/>
+      <c r="I93" s="103"/>
       <c r="J93" s="21"/>
-      <c r="K93" s="22"/>
-      <c r="L93" s="15"/>
-    </row>
-    <row r="94" spans="1:12">
+      <c r="K93" s="21"/>
+      <c r="L93" s="22"/>
+      <c r="M93" s="15"/>
+    </row>
+    <row r="94" spans="1:13">
       <c r="A94" s="19">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -3788,13 +3912,14 @@
       <c r="E94" s="20"/>
       <c r="F94" s="103"/>
       <c r="G94" s="106"/>
-      <c r="H94" s="103"/>
-      <c r="I94" s="21"/>
+      <c r="H94" s="106"/>
+      <c r="I94" s="103"/>
       <c r="J94" s="21"/>
-      <c r="K94" s="22"/>
-      <c r="L94" s="15"/>
-    </row>
-    <row r="95" spans="1:12">
+      <c r="K94" s="21"/>
+      <c r="L94" s="22"/>
+      <c r="M94" s="15"/>
+    </row>
+    <row r="95" spans="1:13">
       <c r="A95" s="19">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -3805,13 +3930,14 @@
       <c r="E95" s="74"/>
       <c r="F95" s="104"/>
       <c r="G95" s="107"/>
-      <c r="H95" s="104"/>
-      <c r="I95" s="76"/>
+      <c r="H95" s="107"/>
+      <c r="I95" s="104"/>
       <c r="J95" s="76"/>
-      <c r="K95" s="77"/>
-      <c r="L95" s="15"/>
-    </row>
-    <row r="96" spans="1:12">
+      <c r="K95" s="76"/>
+      <c r="L95" s="77"/>
+      <c r="M95" s="15"/>
+    </row>
+    <row r="96" spans="1:13">
       <c r="A96" s="19">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -3822,17 +3948,20 @@
       <c r="E96" s="20"/>
       <c r="F96" s="103"/>
       <c r="G96" s="106"/>
-      <c r="H96" s="103"/>
-      <c r="I96" s="21"/>
+      <c r="H96" s="106"/>
+      <c r="I96" s="103"/>
       <c r="J96" s="21"/>
-      <c r="K96" s="22"/>
-      <c r="L96" s="15"/>
+      <c r="K96" s="21"/>
+      <c r="L96" s="22"/>
+      <c r="M96" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="26">
     <mergeCell ref="F88:F89"/>
+    <mergeCell ref="H88:H89"/>
+    <mergeCell ref="I88:J89"/>
+    <mergeCell ref="G59:G60"/>
     <mergeCell ref="G88:G89"/>
-    <mergeCell ref="H88:I89"/>
     <mergeCell ref="A88:A89"/>
     <mergeCell ref="B88:B89"/>
     <mergeCell ref="C88:C89"/>
@@ -3845,19 +3974,19 @@
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A22:B22"/>
-    <mergeCell ref="H59:I60"/>
+    <mergeCell ref="I59:J60"/>
     <mergeCell ref="A59:A60"/>
     <mergeCell ref="B59:B60"/>
     <mergeCell ref="C59:C60"/>
     <mergeCell ref="E59:E60"/>
     <mergeCell ref="D59:D60"/>
-    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="H59:H60"/>
     <mergeCell ref="F59:F60"/>
     <mergeCell ref="A25:B25"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
-  <dataValidations disablePrompts="1" count="5">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E100:G100" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E100:H100" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3867,7 +3996,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
       <formula1>componentKind</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F61:G78 C17:C22" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17:C22 F61:G78" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>yesNo</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C23" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">

</xml_diff>

<commit_message>
1.0.3: To create RequestFactory if API's are specified in definition sheet.
</commit_message>
<xml_diff>
--- a/meta/components/BoxSample.xlsx
+++ b/meta/components/BoxSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVueComponent/meta/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5731473B-F7B1-5F4E-8F8B-BEA3EB8ACCF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42C528D-425B-F34E-9CEB-A97BFF885791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21480" yWindow="2280" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,11 +17,12 @@
     <sheet name="config" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="adjustDefaultValue">config!$J$4:$J$5</definedName>
-    <definedName name="adjustFieldName">config!$H$4:$H$5</definedName>
-    <definedName name="adjustFiledName">config!$H$4:$H$5</definedName>
+    <definedName name="adjustDefaultValue">config!$L$4:$L$5</definedName>
+    <definedName name="adjustFieldName">config!$J$4:$J$5</definedName>
+    <definedName name="adjustFiledName">config!$J$4:$J$5</definedName>
     <definedName name="componentKind">config!$B$4:$B$5</definedName>
-    <definedName name="createToString">config!$F$4:$F$5</definedName>
+    <definedName name="createToString">config!$H$4:$H$5</definedName>
+    <definedName name="httpdMethod">config!$F$4:$F$8</definedName>
     <definedName name="yesNo">config!$D$4:$D$5</definedName>
     <definedName name="チェック種別" localSheetId="1">#REF!</definedName>
     <definedName name="チェック種別">#REF!</definedName>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="128">
   <si>
     <t>パッケージ</t>
   </si>
@@ -695,13 +696,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>クラス名</t>
-    <rPh sb="3" eb="4">
-      <t xml:space="preserve">メイ </t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>説明</t>
     <rPh sb="0" eb="2">
       <t xml:space="preserve">セツメイ </t>
@@ -983,14 +977,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>import { DummyApi } from "@/smples/api/DummyApi"</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>import { SmpleApi } from "@/smples/api/SampleApi"</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>クエリ文字列</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -1006,6 +992,44 @@
     <rPh sb="14" eb="17">
       <t xml:space="preserve">モジレツ </t>
     </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>メソッド</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>import { DummyApiPostRequest } from "@/smples/api/DummyApiPostRequest"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>HTTPメソッド</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>GET</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>PUT</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>DELETE</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>import { SampleApiGetRequest } from "@/smples/api/SampleApiGetRequest"</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1013,7 +1037,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -1058,6 +1082,12 @@
       <family val="3"/>
       <charset val="128"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="ＭＳ ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1097,7 +1127,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -1647,12 +1677,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1806,65 +1881,77 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -2278,8 +2365,8 @@
   </sheetPr>
   <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="I66" sqref="I66"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2297,7 +2384,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="19">
       <c r="A1" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>69</v>
@@ -2315,7 +2402,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -2353,7 +2440,7 @@
       <c r="D7" s="12"/>
       <c r="E7" s="8"/>
       <c r="F7" s="34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G7" s="34"/>
       <c r="H7" s="34"/>
@@ -2394,10 +2481,10 @@
       <c r="I9" s="35"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="93" t="s">
+      <c r="A10" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="94"/>
+      <c r="B10" s="99"/>
       <c r="C10" s="10" t="s">
         <v>65</v>
       </c>
@@ -2411,10 +2498,10 @@
       <c r="I10" s="35"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="93" t="s">
+      <c r="A11" s="98" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="94"/>
+      <c r="B11" s="99"/>
       <c r="C11" s="10" t="s">
         <v>66</v>
       </c>
@@ -2428,10 +2515,10 @@
       <c r="I11" s="35"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="93" t="s">
+      <c r="A12" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="94"/>
+      <c r="B12" s="99"/>
       <c r="C12" s="10" t="s">
         <v>21</v>
       </c>
@@ -2445,10 +2532,10 @@
       <c r="I12" s="35"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="93" t="s">
+      <c r="A13" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="94"/>
+      <c r="B13" s="99"/>
       <c r="C13" s="86" t="s">
         <v>67</v>
       </c>
@@ -2466,11 +2553,11 @@
         <v>1</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="95" t="s">
+      <c r="C14" s="100" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="96"/>
-      <c r="E14" s="97"/>
+      <c r="D14" s="101"/>
+      <c r="E14" s="102"/>
       <c r="F14" s="65"/>
       <c r="G14" s="65"/>
       <c r="H14" s="65"/>
@@ -2596,10 +2683,10 @@
       <c r="I21"/>
     </row>
     <row r="22" spans="1:13" s="32" customFormat="1">
-      <c r="A22" s="87" t="s">
+      <c r="A22" s="103" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="88"/>
+      <c r="B22" s="104"/>
       <c r="C22" s="64" t="s">
         <v>14</v>
       </c>
@@ -2628,10 +2715,10 @@
       <c r="I23"/>
     </row>
     <row r="24" spans="1:13" s="32" customFormat="1">
-      <c r="A24" s="87" t="s">
+      <c r="A24" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="88"/>
+      <c r="B24" s="104"/>
       <c r="C24" s="64" t="s">
         <v>14</v>
       </c>
@@ -2645,10 +2732,10 @@
       <c r="I24"/>
     </row>
     <row r="25" spans="1:13" s="32" customFormat="1">
-      <c r="A25" s="87" t="s">
+      <c r="A25" s="103" t="s">
         <v>68</v>
       </c>
-      <c r="B25" s="88"/>
+      <c r="B25" s="104"/>
       <c r="C25" s="64" t="s">
         <v>14</v>
       </c>
@@ -2674,7 +2761,7 @@
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B27" s="31"/>
       <c r="C27" s="31"/>
@@ -2715,7 +2802,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="46" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C29" s="38"/>
       <c r="D29" s="38"/>
@@ -2734,7 +2821,7 @@
         <v>2</v>
       </c>
       <c r="B30" s="46" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C30" s="40"/>
       <c r="D30" s="40"/>
@@ -2883,7 +2970,7 @@
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B39" s="31"/>
       <c r="C39" s="31"/>
@@ -2924,7 +3011,7 @@
         <v>1</v>
       </c>
       <c r="B41" s="46" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C41" s="38"/>
       <c r="D41" s="38"/>
@@ -2943,7 +3030,7 @@
         <v>2</v>
       </c>
       <c r="B42" s="46" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="C42" s="40"/>
       <c r="D42" s="40"/>
@@ -2993,7 +3080,7 @@
       <c r="D45" s="31"/>
       <c r="E45" s="81"/>
       <c r="F45" s="44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G45" s="44"/>
       <c r="H45" s="44"/>
@@ -3011,10 +3098,10 @@
         <v>85</v>
       </c>
       <c r="C46" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="D46" s="42" t="s">
         <v>86</v>
-      </c>
-      <c r="D46" s="42" t="s">
-        <v>87</v>
       </c>
       <c r="E46" s="82"/>
       <c r="F46" s="67"/>
@@ -3031,13 +3118,13 @@
         <v>1</v>
       </c>
       <c r="B47" s="46" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" s="111" t="s">
+        <v>121</v>
+      </c>
+      <c r="D47" s="38" t="s">
         <v>90</v>
-      </c>
-      <c r="C47" s="98" t="s">
-        <v>90</v>
-      </c>
-      <c r="D47" s="38" t="s">
-        <v>91</v>
       </c>
       <c r="E47" s="39"/>
       <c r="F47" s="68"/>
@@ -3054,13 +3141,13 @@
         <v>2</v>
       </c>
       <c r="B48" s="46" t="s">
-        <v>89</v>
-      </c>
-      <c r="C48" s="99" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="C48" s="112" t="s">
+        <v>123</v>
       </c>
       <c r="D48" s="40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E48" s="41"/>
       <c r="F48" s="68"/>
@@ -3075,7 +3162,7 @@
     <row r="49" spans="1:13">
       <c r="A49" s="52"/>
       <c r="B49" s="48"/>
-      <c r="C49" s="100"/>
+      <c r="C49" s="113"/>
       <c r="D49" s="49"/>
       <c r="E49" s="50"/>
       <c r="F49" s="68"/>
@@ -3104,7 +3191,7 @@
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B51" s="31"/>
       <c r="C51" s="31"/>
@@ -3132,7 +3219,7 @@
       <c r="D52" s="42"/>
       <c r="E52" s="82"/>
       <c r="F52" s="67" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G52" s="67"/>
       <c r="H52" s="67"/>
@@ -3215,7 +3302,7 @@
     </row>
     <row r="58" spans="1:13">
       <c r="A58" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B58" s="14"/>
       <c r="C58" s="14"/>
@@ -3231,49 +3318,49 @@
       <c r="M58" s="15"/>
     </row>
     <row r="59" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A59" s="90" t="s">
+      <c r="A59" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="B59" s="90" t="s">
+      <c r="B59" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="C59" s="89" t="s">
+      <c r="C59" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="D59" s="89" t="s">
+      <c r="D59" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="E59" s="89" t="s">
+      <c r="E59" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="F59" s="91" t="s">
+      <c r="F59" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="G59" s="91" t="s">
+      <c r="G59" s="95" t="s">
         <v>16</v>
       </c>
-      <c r="H59" s="108" t="s">
-        <v>118</v>
-      </c>
-      <c r="I59" s="89" t="s">
+      <c r="H59" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="I59" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="J59" s="89"/>
+      <c r="J59" s="94"/>
       <c r="K59" s="16"/>
       <c r="L59" s="17"/>
       <c r="M59" s="9"/>
     </row>
     <row r="60" spans="1:13">
-      <c r="A60" s="90"/>
-      <c r="B60" s="90"/>
-      <c r="C60" s="89"/>
-      <c r="D60" s="89"/>
-      <c r="E60" s="89"/>
-      <c r="F60" s="92"/>
-      <c r="G60" s="92"/>
-      <c r="H60" s="109"/>
-      <c r="I60" s="89"/>
-      <c r="J60" s="89"/>
+      <c r="A60" s="97"/>
+      <c r="B60" s="97"/>
+      <c r="C60" s="94"/>
+      <c r="D60" s="94"/>
+      <c r="E60" s="94"/>
+      <c r="F60" s="96"/>
+      <c r="G60" s="96"/>
+      <c r="H60" s="106"/>
+      <c r="I60" s="94"/>
+      <c r="J60" s="94"/>
       <c r="K60" s="18"/>
       <c r="L60" s="29"/>
       <c r="M60" s="15"/>
@@ -3391,7 +3478,7 @@
         <v>5</v>
       </c>
       <c r="B65" s="73" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C65" s="80" t="s">
         <v>48</v>
@@ -3403,10 +3490,10 @@
         <v>14</v>
       </c>
       <c r="H65" s="69" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="I65" s="20" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J65" s="21"/>
       <c r="K65" s="21"/>
@@ -3646,7 +3733,7 @@
     </row>
     <row r="80" spans="1:13">
       <c r="A80" s="30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B80" s="31"/>
       <c r="C80" s="31"/>
@@ -3742,7 +3829,7 @@
     <row r="86" spans="1:13">
       <c r="A86" s="13"/>
       <c r="B86" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C86" s="13"/>
       <c r="D86" s="13"/>
@@ -3755,7 +3842,7 @@
     </row>
     <row r="87" spans="1:13">
       <c r="A87" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B87" s="14"/>
       <c r="C87" s="14"/>
@@ -3771,41 +3858,41 @@
       <c r="M87" s="15"/>
     </row>
     <row r="88" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A88" s="90" t="s">
+      <c r="A88" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="B88" s="90" t="s">
-        <v>94</v>
-      </c>
-      <c r="C88" s="89" t="s">
+      <c r="B88" s="97" t="s">
+        <v>93</v>
+      </c>
+      <c r="C88" s="94" t="s">
+        <v>95</v>
+      </c>
+      <c r="D88" s="94" t="s">
         <v>96</v>
       </c>
-      <c r="D88" s="89" t="s">
-        <v>97</v>
-      </c>
-      <c r="E88" s="89" t="s">
-        <v>87</v>
-      </c>
-      <c r="F88" s="101"/>
-      <c r="G88" s="101"/>
-      <c r="H88" s="101"/>
-      <c r="I88" s="105"/>
-      <c r="J88" s="89"/>
+      <c r="E88" s="94" t="s">
+        <v>86</v>
+      </c>
+      <c r="F88" s="91"/>
+      <c r="G88" s="91"/>
+      <c r="H88" s="91"/>
+      <c r="I88" s="93"/>
+      <c r="J88" s="94"/>
       <c r="K88" s="16"/>
       <c r="L88" s="17"/>
       <c r="M88" s="9"/>
     </row>
     <row r="89" spans="1:13">
-      <c r="A89" s="90"/>
-      <c r="B89" s="90"/>
-      <c r="C89" s="89"/>
-      <c r="D89" s="89"/>
-      <c r="E89" s="89"/>
-      <c r="F89" s="102"/>
-      <c r="G89" s="102"/>
-      <c r="H89" s="102"/>
-      <c r="I89" s="105"/>
-      <c r="J89" s="89"/>
+      <c r="A89" s="97"/>
+      <c r="B89" s="97"/>
+      <c r="C89" s="94"/>
+      <c r="D89" s="94"/>
+      <c r="E89" s="94"/>
+      <c r="F89" s="92"/>
+      <c r="G89" s="92"/>
+      <c r="H89" s="92"/>
+      <c r="I89" s="93"/>
+      <c r="J89" s="94"/>
       <c r="K89" s="18"/>
       <c r="L89" s="29"/>
       <c r="M89" s="15"/>
@@ -3815,19 +3902,19 @@
         <v>1</v>
       </c>
       <c r="B90" s="71" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C90" s="78" t="s">
         <v>48</v>
       </c>
       <c r="D90" s="20"/>
       <c r="E90" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="F90" s="103"/>
-      <c r="G90" s="106"/>
-      <c r="H90" s="106"/>
-      <c r="I90" s="103"/>
+        <v>108</v>
+      </c>
+      <c r="F90" s="87"/>
+      <c r="G90" s="89"/>
+      <c r="H90" s="89"/>
+      <c r="I90" s="87"/>
       <c r="J90" s="21"/>
       <c r="K90" s="21"/>
       <c r="L90" s="28"/>
@@ -3839,19 +3926,19 @@
         <v>2</v>
       </c>
       <c r="B91" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="C91" s="78" t="s">
         <v>99</v>
-      </c>
-      <c r="C91" s="78" t="s">
-        <v>100</v>
       </c>
       <c r="D91" s="20"/>
       <c r="E91" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="F91" s="103"/>
-      <c r="G91" s="106"/>
-      <c r="H91" s="106"/>
-      <c r="I91" s="103"/>
+        <v>109</v>
+      </c>
+      <c r="F91" s="87"/>
+      <c r="G91" s="89"/>
+      <c r="H91" s="89"/>
+      <c r="I91" s="87"/>
       <c r="J91" s="21"/>
       <c r="K91" s="21"/>
       <c r="L91" s="28"/>
@@ -3863,7 +3950,7 @@
         <v>3</v>
       </c>
       <c r="B92" s="72" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C92" s="79" t="s">
         <v>54</v>
@@ -3872,12 +3959,12 @@
         <v>55</v>
       </c>
       <c r="E92" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="F92" s="103"/>
-      <c r="G92" s="106"/>
-      <c r="H92" s="106"/>
-      <c r="I92" s="103"/>
+        <v>111</v>
+      </c>
+      <c r="F92" s="87"/>
+      <c r="G92" s="89"/>
+      <c r="H92" s="89"/>
+      <c r="I92" s="87"/>
       <c r="J92" s="21"/>
       <c r="K92" s="21"/>
       <c r="L92" s="22"/>
@@ -3892,10 +3979,10 @@
       <c r="C93" s="80"/>
       <c r="D93" s="20"/>
       <c r="E93" s="20"/>
-      <c r="F93" s="103"/>
-      <c r="G93" s="106"/>
-      <c r="H93" s="106"/>
-      <c r="I93" s="103"/>
+      <c r="F93" s="87"/>
+      <c r="G93" s="89"/>
+      <c r="H93" s="89"/>
+      <c r="I93" s="87"/>
       <c r="J93" s="21"/>
       <c r="K93" s="21"/>
       <c r="L93" s="22"/>
@@ -3910,10 +3997,10 @@
       <c r="C94" s="80"/>
       <c r="D94" s="20"/>
       <c r="E94" s="20"/>
-      <c r="F94" s="103"/>
-      <c r="G94" s="106"/>
-      <c r="H94" s="106"/>
-      <c r="I94" s="103"/>
+      <c r="F94" s="87"/>
+      <c r="G94" s="89"/>
+      <c r="H94" s="89"/>
+      <c r="I94" s="87"/>
       <c r="J94" s="21"/>
       <c r="K94" s="21"/>
       <c r="L94" s="22"/>
@@ -3928,10 +4015,10 @@
       <c r="C95" s="80"/>
       <c r="D95" s="74"/>
       <c r="E95" s="74"/>
-      <c r="F95" s="104"/>
-      <c r="G95" s="107"/>
-      <c r="H95" s="107"/>
-      <c r="I95" s="104"/>
+      <c r="F95" s="88"/>
+      <c r="G95" s="90"/>
+      <c r="H95" s="90"/>
+      <c r="I95" s="88"/>
       <c r="J95" s="76"/>
       <c r="K95" s="76"/>
       <c r="L95" s="77"/>
@@ -3946,10 +4033,10 @@
       <c r="C96" s="80"/>
       <c r="D96" s="20"/>
       <c r="E96" s="20"/>
-      <c r="F96" s="103"/>
-      <c r="G96" s="106"/>
-      <c r="H96" s="106"/>
-      <c r="I96" s="103"/>
+      <c r="F96" s="87"/>
+      <c r="G96" s="89"/>
+      <c r="H96" s="89"/>
+      <c r="I96" s="87"/>
       <c r="J96" s="21"/>
       <c r="K96" s="21"/>
       <c r="L96" s="22"/>
@@ -3957,21 +4044,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="F88:F89"/>
-    <mergeCell ref="H88:H89"/>
-    <mergeCell ref="I88:J89"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="G88:G89"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="B88:B89"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="D88:D89"/>
-    <mergeCell ref="E88:E89"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C14:E14"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="I59:J60"/>
@@ -3983,9 +4055,24 @@
     <mergeCell ref="H59:H60"/>
     <mergeCell ref="F59:F60"/>
     <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="B88:B89"/>
+    <mergeCell ref="C88:C89"/>
+    <mergeCell ref="D88:D89"/>
+    <mergeCell ref="E88:E89"/>
+    <mergeCell ref="F88:F89"/>
+    <mergeCell ref="H88:H89"/>
+    <mergeCell ref="I88:J89"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="G88:G89"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
-  <dataValidations count="5">
+  <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E100:H100" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
@@ -4002,6 +4089,9 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C23" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">
       <formula1>adjustFieldName</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C47:C49" xr:uid="{BDE40890-40F7-4E41-B7E1-478CEBD85557}">
+      <formula1>httpdMethod</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.59027777777777779" right="0.59027777777777779" top="0.59027777777777779" bottom="0.59027777777777779" header="0.51180555555555562" footer="0.11805555555555557"/>
   <pageSetup paperSize="9" scale="82" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -4016,10 +4106,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -4029,14 +4119,16 @@
     <col min="5" max="5" width="8.83203125" style="55" customWidth="1"/>
     <col min="6" max="6" width="18.5" style="55" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.83203125" style="55" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" style="55" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5" style="55" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.83203125" style="55" customWidth="1"/>
     <col min="10" max="10" width="18.6640625" style="55" bestFit="1" customWidth="1"/>
-    <col min="11" max="251" width="8.83203125" style="55" customWidth="1"/>
-    <col min="252" max="16384" width="10.83203125" style="55"/>
+    <col min="11" max="11" width="8.83203125" style="55" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" style="55" bestFit="1" customWidth="1"/>
+    <col min="13" max="253" width="8.83203125" style="55" customWidth="1"/>
+    <col min="254" max="16384" width="10.83203125" style="55"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19">
+    <row r="1" spans="1:12" ht="19">
       <c r="A1" s="53" t="s">
         <v>8</v>
       </c>
@@ -4048,11 +4140,13 @@
       <c r="G1" s="53"/>
       <c r="H1" s="53"/>
       <c r="I1" s="53"/>
-      <c r="J1" s="54" t="s">
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="54" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:12">
       <c r="B3" s="56" t="s">
         <v>25</v>
       </c>
@@ -4060,33 +4154,37 @@
         <v>31</v>
       </c>
       <c r="F3" s="56" t="s">
+        <v>120</v>
+      </c>
+      <c r="H3" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="56" t="s">
+      <c r="J3" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="56" t="s">
+      <c r="L3" s="56" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:12">
       <c r="B4" s="57" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="58"/>
+      <c r="F4" s="107"/>
       <c r="H4" s="58"/>
       <c r="J4" s="58"/>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="L4" s="58"/>
+    </row>
+    <row r="5" spans="1:12">
       <c r="B5" s="59" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="60"/>
-      <c r="F5" s="60" t="s">
-        <v>13</v>
+      <c r="F5" s="108" t="s">
+        <v>122</v>
       </c>
       <c r="H5" s="60" t="s">
         <v>13</v>
@@ -4094,9 +4192,25 @@
       <c r="J5" s="60" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="L5" s="60" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="B6" s="61"/>
+      <c r="F6" s="108" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="F7" s="109" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="F8" s="110" t="s">
+        <v>126</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6"/>

</xml_diff>

<commit_message>
1.0.5: onBeforeRouterLeave guard is available.
</commit_message>
<xml_diff>
--- a/meta/components/BoxSample.xlsx
+++ b/meta/components/BoxSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVueComponent/meta/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42C528D-425B-F34E-9CEB-A97BFF885791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E968AE2-E77B-974B-A76F-B6CE299FDFEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="2280" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VueComponent" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="132">
   <si>
     <t>パッケージ</t>
   </si>
@@ -1030,6 +1030,52 @@
   </si>
   <si>
     <t>import { SampleApiGetRequest } from "@/smples/api/SampleApiGetRequest"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>import { RouterHooks } from "@/utils/RouterHooks"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>BeforeRouterLeave関数名</t>
+    <rPh sb="17" eb="19">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t xml:space="preserve">メイ </t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>RouterHooks.beforeRouterLeave</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>/* BeforeRouterLeave関数を実装する場合はここに関数名を定義し、Vueコンポーネント定義・ヘッダ情報（コンポーネント定義用）に関数のインポートを定義します。 */</t>
+    <rPh sb="20" eb="22">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t xml:space="preserve">ジッソウ </t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t xml:space="preserve">バアイハ </t>
+    </rPh>
+    <rPh sb="33" eb="36">
+      <t xml:space="preserve">カンスウメイヲ </t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t xml:space="preserve">テイギシ </t>
+    </rPh>
+    <rPh sb="48" eb="51">
+      <t xml:space="preserve">テイギヨウ </t>
+    </rPh>
+    <rPh sb="72" eb="74">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="81" eb="83">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1889,54 +1935,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1952,6 +1950,54 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -2363,10 +2409,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M96"/>
+  <dimension ref="A1:M98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2481,10 +2527,10 @@
       <c r="I9" s="35"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="98" t="s">
+      <c r="A10" s="106" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="99"/>
+      <c r="B10" s="107"/>
       <c r="C10" s="10" t="s">
         <v>65</v>
       </c>
@@ -2498,10 +2544,10 @@
       <c r="I10" s="35"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="98" t="s">
+      <c r="A11" s="106" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="99"/>
+      <c r="B11" s="107"/>
       <c r="C11" s="10" t="s">
         <v>66</v>
       </c>
@@ -2515,10 +2561,10 @@
       <c r="I11" s="35"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="98" t="s">
+      <c r="A12" s="106" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="99"/>
+      <c r="B12" s="107"/>
       <c r="C12" s="10" t="s">
         <v>21</v>
       </c>
@@ -2532,10 +2578,10 @@
       <c r="I12" s="35"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="98" t="s">
+      <c r="A13" s="106" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="99"/>
+      <c r="B13" s="107"/>
       <c r="C13" s="86" t="s">
         <v>67</v>
       </c>
@@ -2553,11 +2599,11 @@
         <v>1</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="100" t="s">
+      <c r="C14" s="108" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="101"/>
-      <c r="E14" s="102"/>
+      <c r="D14" s="109"/>
+      <c r="E14" s="110"/>
       <c r="F14" s="65"/>
       <c r="G14" s="65"/>
       <c r="H14" s="65"/>
@@ -2683,10 +2729,10 @@
       <c r="I21"/>
     </row>
     <row r="22" spans="1:13" s="32" customFormat="1">
-      <c r="A22" s="103" t="s">
+      <c r="A22" s="98" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="104"/>
+      <c r="B22" s="99"/>
       <c r="C22" s="64" t="s">
         <v>14</v>
       </c>
@@ -2700,14 +2746,16 @@
       <c r="I22"/>
     </row>
     <row r="23" spans="1:13" s="32" customFormat="1">
-      <c r="A23" s="62" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="63"/>
+      <c r="A23" s="98" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23" s="99"/>
       <c r="C23" s="64" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23"/>
+        <v>130</v>
+      </c>
+      <c r="D23" t="s">
+        <v>131</v>
+      </c>
       <c r="E23"/>
       <c r="F23"/>
       <c r="G23" s="66"/>
@@ -2715,16 +2763,14 @@
       <c r="I23"/>
     </row>
     <row r="24" spans="1:13" s="32" customFormat="1">
-      <c r="A24" s="103" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" s="104"/>
+      <c r="A24" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="63"/>
       <c r="C24" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="D24" t="s">
-        <v>19</v>
-      </c>
+      <c r="D24"/>
       <c r="E24"/>
       <c r="F24"/>
       <c r="G24" s="66"/>
@@ -2732,100 +2778,98 @@
       <c r="I24"/>
     </row>
     <row r="25" spans="1:13" s="32" customFormat="1">
-      <c r="A25" s="103" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25" s="104"/>
+      <c r="A25" s="98" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="99"/>
       <c r="C25" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="D25"/>
+      <c r="D25" t="s">
+        <v>19</v>
+      </c>
       <c r="E25"/>
       <c r="F25"/>
       <c r="G25" s="66"/>
       <c r="H25" s="66"/>
       <c r="I25"/>
     </row>
-    <row r="26" spans="1:13" s="37" customFormat="1">
-      <c r="A26" s="34"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
-    </row>
-    <row r="27" spans="1:13">
-      <c r="A27" s="30" t="s">
+    <row r="26" spans="1:13" s="32" customFormat="1">
+      <c r="A26" s="98" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="99"/>
+      <c r="C26" s="64" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26" s="66"/>
+      <c r="H26" s="66"/>
+      <c r="I26"/>
+    </row>
+    <row r="27" spans="1:13" s="37" customFormat="1">
+      <c r="A27" s="34"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="34"/>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="81"/>
-      <c r="F27" s="44" t="s">
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="81"/>
+      <c r="F28" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="43"/>
-      <c r="L27" s="43"/>
-      <c r="M27" s="43"/>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28" s="47" t="s">
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="43"/>
+      <c r="L28" s="43"/>
+      <c r="M28" s="43"/>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="42" t="s">
+      <c r="B29" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="82"/>
-      <c r="F28" s="67"/>
-      <c r="G28" s="67"/>
-      <c r="H28" s="67"/>
-      <c r="I28" s="67"/>
-      <c r="J28" s="44"/>
-      <c r="K28" s="45"/>
-      <c r="L28" s="45"/>
-      <c r="M28" s="35"/>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="A29" s="51">
-        <v>1</v>
-      </c>
-      <c r="B29" s="46" t="s">
-        <v>113</v>
-      </c>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="68"/>
-      <c r="G29" s="68"/>
-      <c r="H29" s="68"/>
-      <c r="I29" s="34"/>
-      <c r="J29" s="36"/>
-      <c r="K29" s="36"/>
-      <c r="L29" s="36"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="82"/>
+      <c r="F29" s="67"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="67"/>
+      <c r="I29" s="67"/>
+      <c r="J29" s="44"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="45"/>
       <c r="M29" s="35"/>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B30" s="46" t="s">
-        <v>114</v>
-      </c>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="41"/>
+        <v>113</v>
+      </c>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="39"/>
       <c r="F30" s="68"/>
       <c r="G30" s="68"/>
       <c r="H30" s="68"/>
@@ -2836,11 +2880,15 @@
       <c r="M30" s="35"/>
     </row>
     <row r="31" spans="1:13">
-      <c r="A31" s="52"/>
-      <c r="B31" s="48"/>
-      <c r="C31" s="49"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="50"/>
+      <c r="A31" s="51">
+        <v>2</v>
+      </c>
+      <c r="B31" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="41"/>
       <c r="F31" s="68"/>
       <c r="G31" s="68"/>
       <c r="H31" s="68"/>
@@ -2851,99 +2899,99 @@
       <c r="M31" s="35"/>
     </row>
     <row r="32" spans="1:13">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
+      <c r="A32" s="51">
+        <v>3</v>
+      </c>
+      <c r="B32" s="46" t="s">
+        <v>128</v>
+      </c>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="68"/>
+      <c r="G32" s="68"/>
+      <c r="H32" s="68"/>
+      <c r="I32" s="34"/>
+      <c r="J32" s="36"/>
+      <c r="K32" s="36"/>
+      <c r="L32" s="36"/>
+      <c r="M32" s="35"/>
     </row>
     <row r="33" spans="1:13">
-      <c r="A33" s="30" t="s">
+      <c r="A33" s="52"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="50"/>
+      <c r="F33" s="68"/>
+      <c r="G33" s="68"/>
+      <c r="H33" s="68"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="36"/>
+      <c r="L33" s="36"/>
+      <c r="M33" s="35"/>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="81"/>
-      <c r="F33" s="44" t="s">
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="81"/>
+      <c r="F35" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="G33" s="44"/>
-      <c r="H33" s="44"/>
-      <c r="I33" s="44"/>
-      <c r="J33" s="43"/>
-      <c r="K33" s="43"/>
-      <c r="L33" s="43"/>
-      <c r="M33" s="43"/>
-    </row>
-    <row r="34" spans="1:13">
-      <c r="A34" s="47" t="s">
+      <c r="G35" s="44"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="44"/>
+      <c r="J35" s="43"/>
+      <c r="K35" s="43"/>
+      <c r="L35" s="43"/>
+      <c r="M35" s="43"/>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="42" t="s">
+      <c r="B36" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="82"/>
-      <c r="F34" s="67"/>
-      <c r="G34" s="67"/>
-      <c r="H34" s="67"/>
-      <c r="I34" s="67"/>
-      <c r="J34" s="44"/>
-      <c r="K34" s="45"/>
-      <c r="L34" s="45"/>
-      <c r="M34" s="35"/>
-    </row>
-    <row r="35" spans="1:13">
-      <c r="A35" s="51">
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="82"/>
+      <c r="F36" s="67"/>
+      <c r="G36" s="67"/>
+      <c r="H36" s="67"/>
+      <c r="I36" s="67"/>
+      <c r="J36" s="44"/>
+      <c r="K36" s="45"/>
+      <c r="L36" s="45"/>
+      <c r="M36" s="35"/>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="51">
         <v>1</v>
       </c>
-      <c r="B35" s="46" t="s">
+      <c r="B37" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="68"/>
-      <c r="G35" s="68"/>
-      <c r="H35" s="68"/>
-      <c r="I35" s="34"/>
-      <c r="J35" s="36"/>
-      <c r="K35" s="36"/>
-      <c r="L35" s="36"/>
-      <c r="M35" s="35"/>
-    </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="51">
-        <v>2</v>
-      </c>
-      <c r="B36" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="68"/>
-      <c r="G36" s="68"/>
-      <c r="H36" s="68"/>
-      <c r="I36" s="34"/>
-      <c r="J36" s="36"/>
-      <c r="K36" s="36"/>
-      <c r="L36" s="36"/>
-      <c r="M36" s="35"/>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="A37" s="52"/>
-      <c r="B37" s="48"/>
-      <c r="C37" s="49"/>
-      <c r="D37" s="49"/>
-      <c r="E37" s="50"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="39"/>
       <c r="F37" s="68"/>
       <c r="G37" s="68"/>
       <c r="H37" s="68"/>
@@ -2954,11 +3002,15 @@
       <c r="M37" s="35"/>
     </row>
     <row r="38" spans="1:13">
-      <c r="A38" s="83"/>
-      <c r="B38" s="84"/>
-      <c r="C38" s="85"/>
-      <c r="D38" s="85"/>
-      <c r="E38" s="85"/>
+      <c r="A38" s="51">
+        <v>2</v>
+      </c>
+      <c r="B38" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="41"/>
       <c r="F38" s="68"/>
       <c r="G38" s="68"/>
       <c r="H38" s="68"/>
@@ -2969,87 +3021,83 @@
       <c r="M38" s="35"/>
     </row>
     <row r="39" spans="1:13">
-      <c r="A39" s="30" t="s">
+      <c r="A39" s="52"/>
+      <c r="B39" s="48"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="68"/>
+      <c r="G39" s="68"/>
+      <c r="H39" s="68"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="36"/>
+      <c r="K39" s="36"/>
+      <c r="L39" s="36"/>
+      <c r="M39" s="35"/>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="83"/>
+      <c r="B40" s="84"/>
+      <c r="C40" s="85"/>
+      <c r="D40" s="85"/>
+      <c r="E40" s="85"/>
+      <c r="F40" s="68"/>
+      <c r="G40" s="68"/>
+      <c r="H40" s="68"/>
+      <c r="I40" s="34"/>
+      <c r="J40" s="36"/>
+      <c r="K40" s="36"/>
+      <c r="L40" s="36"/>
+      <c r="M40" s="35"/>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="81"/>
-      <c r="F39" s="44" t="s">
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="81"/>
+      <c r="F41" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="G39" s="44"/>
-      <c r="H39" s="44"/>
-      <c r="I39" s="44"/>
-      <c r="J39" s="43"/>
-      <c r="K39" s="43"/>
-      <c r="L39" s="43"/>
-      <c r="M39" s="43"/>
-    </row>
-    <row r="40" spans="1:13">
-      <c r="A40" s="47" t="s">
+      <c r="G41" s="44"/>
+      <c r="H41" s="44"/>
+      <c r="I41" s="44"/>
+      <c r="J41" s="43"/>
+      <c r="K41" s="43"/>
+      <c r="L41" s="43"/>
+      <c r="M41" s="43"/>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="42" t="s">
+      <c r="B42" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="42"/>
-      <c r="D40" s="42"/>
-      <c r="E40" s="82"/>
-      <c r="F40" s="67"/>
-      <c r="G40" s="67"/>
-      <c r="H40" s="67"/>
-      <c r="I40" s="67"/>
-      <c r="J40" s="44"/>
-      <c r="K40" s="45"/>
-      <c r="L40" s="45"/>
-      <c r="M40" s="35"/>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="A41" s="51">
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="82"/>
+      <c r="F42" s="67"/>
+      <c r="G42" s="67"/>
+      <c r="H42" s="67"/>
+      <c r="I42" s="67"/>
+      <c r="J42" s="44"/>
+      <c r="K42" s="45"/>
+      <c r="L42" s="45"/>
+      <c r="M42" s="35"/>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="51">
         <v>1</v>
       </c>
-      <c r="B41" s="46" t="s">
+      <c r="B43" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="68"/>
-      <c r="G41" s="68"/>
-      <c r="H41" s="68"/>
-      <c r="I41" s="34"/>
-      <c r="J41" s="36"/>
-      <c r="K41" s="36"/>
-      <c r="L41" s="36"/>
-      <c r="M41" s="35"/>
-    </row>
-    <row r="42" spans="1:13">
-      <c r="A42" s="51">
-        <v>2</v>
-      </c>
-      <c r="B42" s="46" t="s">
-        <v>127</v>
-      </c>
-      <c r="C42" s="40"/>
-      <c r="D42" s="40"/>
-      <c r="E42" s="41"/>
-      <c r="F42" s="68"/>
-      <c r="G42" s="68"/>
-      <c r="H42" s="68"/>
-      <c r="I42" s="34"/>
-      <c r="J42" s="36"/>
-      <c r="K42" s="36"/>
-      <c r="L42" s="36"/>
-      <c r="M42" s="35"/>
-    </row>
-    <row r="43" spans="1:13">
-      <c r="A43" s="52"/>
-      <c r="B43" s="48"/>
-      <c r="C43" s="49"/>
-      <c r="D43" s="49"/>
-      <c r="E43" s="50"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="39"/>
       <c r="F43" s="68"/>
       <c r="G43" s="68"/>
       <c r="H43" s="68"/>
@@ -3060,111 +3108,107 @@
       <c r="M43" s="35"/>
     </row>
     <row r="44" spans="1:13">
-      <c r="A44" s="13"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="13"/>
-      <c r="J44" s="13"/>
+      <c r="A44" s="51">
+        <v>2</v>
+      </c>
+      <c r="B44" s="46" t="s">
+        <v>127</v>
+      </c>
+      <c r="C44" s="40"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="41"/>
+      <c r="F44" s="68"/>
+      <c r="G44" s="68"/>
+      <c r="H44" s="68"/>
+      <c r="I44" s="34"/>
+      <c r="J44" s="36"/>
+      <c r="K44" s="36"/>
+      <c r="L44" s="36"/>
+      <c r="M44" s="35"/>
     </row>
     <row r="45" spans="1:13">
-      <c r="A45" s="30" t="s">
+      <c r="A45" s="52"/>
+      <c r="B45" s="48"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="49"/>
+      <c r="E45" s="50"/>
+      <c r="F45" s="68"/>
+      <c r="G45" s="68"/>
+      <c r="H45" s="68"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="36"/>
+      <c r="K45" s="36"/>
+      <c r="L45" s="36"/>
+      <c r="M45" s="35"/>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46" s="13"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="13"/>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="B45" s="31"/>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="81"/>
-      <c r="F45" s="44" t="s">
+      <c r="B47" s="31"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="81"/>
+      <c r="F47" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="G45" s="44"/>
-      <c r="H45" s="44"/>
-      <c r="I45" s="44"/>
-      <c r="J45" s="43"/>
-      <c r="K45" s="43"/>
-      <c r="L45" s="43"/>
-      <c r="M45" s="43"/>
-    </row>
-    <row r="46" spans="1:13">
-      <c r="A46" s="47" t="s">
+      <c r="G47" s="44"/>
+      <c r="H47" s="44"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="43"/>
+      <c r="K47" s="43"/>
+      <c r="L47" s="43"/>
+      <c r="M47" s="43"/>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B46" s="42" t="s">
+      <c r="B48" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="C46" s="47" t="s">
+      <c r="C48" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="D46" s="42" t="s">
+      <c r="D48" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="E46" s="82"/>
-      <c r="F46" s="67"/>
-      <c r="G46" s="67"/>
-      <c r="H46" s="67"/>
-      <c r="I46" s="67"/>
-      <c r="J46" s="44"/>
-      <c r="K46" s="45"/>
-      <c r="L46" s="45"/>
-      <c r="M46" s="35"/>
-    </row>
-    <row r="47" spans="1:13">
-      <c r="A47" s="51">
+      <c r="E48" s="82"/>
+      <c r="F48" s="67"/>
+      <c r="G48" s="67"/>
+      <c r="H48" s="67"/>
+      <c r="I48" s="67"/>
+      <c r="J48" s="44"/>
+      <c r="K48" s="45"/>
+      <c r="L48" s="45"/>
+      <c r="M48" s="35"/>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49" s="51">
         <v>1</v>
       </c>
-      <c r="B47" s="46" t="s">
+      <c r="B49" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="C47" s="111" t="s">
+      <c r="C49" s="95" t="s">
         <v>121</v>
       </c>
-      <c r="D47" s="38" t="s">
+      <c r="D49" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="E47" s="39"/>
-      <c r="F47" s="68"/>
-      <c r="G47" s="68"/>
-      <c r="H47" s="68"/>
-      <c r="I47" s="34"/>
-      <c r="J47" s="36"/>
-      <c r="K47" s="36"/>
-      <c r="L47" s="36"/>
-      <c r="M47" s="35"/>
-    </row>
-    <row r="48" spans="1:13">
-      <c r="A48" s="51">
-        <v>2</v>
-      </c>
-      <c r="B48" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="C48" s="112" t="s">
-        <v>123</v>
-      </c>
-      <c r="D48" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="E48" s="41"/>
-      <c r="F48" s="68"/>
-      <c r="G48" s="68"/>
-      <c r="H48" s="68"/>
-      <c r="I48" s="34"/>
-      <c r="J48" s="36"/>
-      <c r="K48" s="36"/>
-      <c r="L48" s="36"/>
-      <c r="M48" s="35"/>
-    </row>
-    <row r="49" spans="1:13">
-      <c r="A49" s="52"/>
-      <c r="B49" s="48"/>
-      <c r="C49" s="113"/>
-      <c r="D49" s="49"/>
-      <c r="E49" s="50"/>
+      <c r="E49" s="39"/>
       <c r="F49" s="68"/>
       <c r="G49" s="68"/>
       <c r="H49" s="68"/>
@@ -3175,11 +3219,19 @@
       <c r="M49" s="35"/>
     </row>
     <row r="50" spans="1:13">
-      <c r="A50" s="83"/>
-      <c r="B50" s="84"/>
-      <c r="C50" s="85"/>
-      <c r="D50" s="85"/>
-      <c r="E50" s="85"/>
+      <c r="A50" s="51">
+        <v>2</v>
+      </c>
+      <c r="B50" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="C50" s="96" t="s">
+        <v>123</v>
+      </c>
+      <c r="D50" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="E50" s="41"/>
       <c r="F50" s="68"/>
       <c r="G50" s="68"/>
       <c r="H50" s="68"/>
@@ -3190,81 +3242,81 @@
       <c r="M50" s="35"/>
     </row>
     <row r="51" spans="1:13">
-      <c r="A51" s="30" t="s">
+      <c r="A51" s="52"/>
+      <c r="B51" s="48"/>
+      <c r="C51" s="97"/>
+      <c r="D51" s="49"/>
+      <c r="E51" s="50"/>
+      <c r="F51" s="68"/>
+      <c r="G51" s="68"/>
+      <c r="H51" s="68"/>
+      <c r="I51" s="34"/>
+      <c r="J51" s="36"/>
+      <c r="K51" s="36"/>
+      <c r="L51" s="36"/>
+      <c r="M51" s="35"/>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" s="83"/>
+      <c r="B52" s="84"/>
+      <c r="C52" s="85"/>
+      <c r="D52" s="85"/>
+      <c r="E52" s="85"/>
+      <c r="F52" s="68"/>
+      <c r="G52" s="68"/>
+      <c r="H52" s="68"/>
+      <c r="I52" s="34"/>
+      <c r="J52" s="36"/>
+      <c r="K52" s="36"/>
+      <c r="L52" s="36"/>
+      <c r="M52" s="35"/>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="B51" s="31"/>
-      <c r="C51" s="31"/>
-      <c r="D51" s="31"/>
-      <c r="E51" s="81"/>
-      <c r="F51" s="44" t="s">
+      <c r="B53" s="31"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="81"/>
+      <c r="F53" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="G51" s="44"/>
-      <c r="H51" s="44"/>
-      <c r="I51" s="44"/>
-      <c r="J51" s="43"/>
-      <c r="K51" s="43"/>
-      <c r="L51" s="43"/>
-      <c r="M51" s="43"/>
-    </row>
-    <row r="52" spans="1:13">
-      <c r="A52" s="47" t="s">
+      <c r="G53" s="44"/>
+      <c r="H53" s="44"/>
+      <c r="I53" s="44"/>
+      <c r="J53" s="43"/>
+      <c r="K53" s="43"/>
+      <c r="L53" s="43"/>
+      <c r="M53" s="43"/>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B52" s="42" t="s">
+      <c r="B54" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C52" s="42"/>
-      <c r="D52" s="42"/>
-      <c r="E52" s="82"/>
-      <c r="F52" s="67" t="s">
+      <c r="C54" s="42"/>
+      <c r="D54" s="42"/>
+      <c r="E54" s="82"/>
+      <c r="F54" s="67" t="s">
         <v>112</v>
       </c>
-      <c r="G52" s="67"/>
-      <c r="H52" s="67"/>
-      <c r="I52" s="67"/>
-      <c r="J52" s="44"/>
-      <c r="K52" s="45"/>
-      <c r="L52" s="45"/>
-      <c r="M52" s="35"/>
-    </row>
-    <row r="53" spans="1:13">
-      <c r="A53" s="51"/>
-      <c r="B53" s="46"/>
-      <c r="C53" s="38"/>
-      <c r="D53" s="38"/>
-      <c r="E53" s="39"/>
-      <c r="F53" s="68"/>
-      <c r="G53" s="68"/>
-      <c r="H53" s="68"/>
-      <c r="I53" s="34"/>
-      <c r="J53" s="36"/>
-      <c r="K53" s="36"/>
-      <c r="L53" s="36"/>
-      <c r="M53" s="35"/>
-    </row>
-    <row r="54" spans="1:13">
-      <c r="A54" s="51"/>
-      <c r="B54" s="46"/>
-      <c r="C54" s="40"/>
-      <c r="D54" s="40"/>
-      <c r="E54" s="41"/>
-      <c r="F54" s="68"/>
-      <c r="G54" s="68"/>
-      <c r="H54" s="68"/>
-      <c r="I54" s="34"/>
-      <c r="J54" s="36"/>
-      <c r="K54" s="36"/>
-      <c r="L54" s="36"/>
+      <c r="G54" s="67"/>
+      <c r="H54" s="67"/>
+      <c r="I54" s="67"/>
+      <c r="J54" s="44"/>
+      <c r="K54" s="45"/>
+      <c r="L54" s="45"/>
       <c r="M54" s="35"/>
     </row>
     <row r="55" spans="1:13">
-      <c r="A55" s="52"/>
-      <c r="B55" s="48"/>
-      <c r="C55" s="49"/>
-      <c r="D55" s="49"/>
-      <c r="E55" s="50"/>
+      <c r="A55" s="51"/>
+      <c r="B55" s="46"/>
+      <c r="C55" s="38"/>
+      <c r="D55" s="38"/>
+      <c r="E55" s="39"/>
       <c r="F55" s="68"/>
       <c r="G55" s="68"/>
       <c r="H55" s="68"/>
@@ -3275,225 +3327,201 @@
       <c r="M55" s="35"/>
     </row>
     <row r="56" spans="1:13">
-      <c r="A56" s="13"/>
-      <c r="B56" s="13"/>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="13"/>
-      <c r="I56" s="13"/>
-      <c r="J56" s="13"/>
+      <c r="A56" s="51"/>
+      <c r="B56" s="46"/>
+      <c r="C56" s="40"/>
+      <c r="D56" s="40"/>
+      <c r="E56" s="41"/>
+      <c r="F56" s="68"/>
+      <c r="G56" s="68"/>
+      <c r="H56" s="68"/>
+      <c r="I56" s="34"/>
+      <c r="J56" s="36"/>
+      <c r="K56" s="36"/>
+      <c r="L56" s="36"/>
+      <c r="M56" s="35"/>
     </row>
     <row r="57" spans="1:13">
-      <c r="A57" s="13"/>
-      <c r="B57" s="13" t="s">
+      <c r="A57" s="52"/>
+      <c r="B57" s="48"/>
+      <c r="C57" s="49"/>
+      <c r="D57" s="49"/>
+      <c r="E57" s="50"/>
+      <c r="F57" s="68"/>
+      <c r="G57" s="68"/>
+      <c r="H57" s="68"/>
+      <c r="I57" s="34"/>
+      <c r="J57" s="36"/>
+      <c r="K57" s="36"/>
+      <c r="L57" s="36"/>
+      <c r="M57" s="35"/>
+    </row>
+    <row r="58" spans="1:13">
+      <c r="A58" s="13"/>
+      <c r="B58" s="13"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="13"/>
+      <c r="J58" s="13"/>
+    </row>
+    <row r="59" spans="1:13">
+      <c r="A59" s="13"/>
+      <c r="B59" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C57" s="13"/>
-      <c r="D57" s="13"/>
-      <c r="E57" s="13"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="13"/>
-      <c r="H57" s="13"/>
-      <c r="I57" s="13"/>
-      <c r="J57" s="13"/>
-    </row>
-    <row r="58" spans="1:13">
-      <c r="A58" s="3" t="s">
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="13"/>
+    </row>
+    <row r="60" spans="1:13">
+      <c r="A60" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B58" s="14"/>
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="14"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="14"/>
-      <c r="I58" s="14"/>
-      <c r="J58" s="14"/>
-      <c r="K58" s="14"/>
-      <c r="L58" s="6"/>
-      <c r="M58" s="15"/>
-    </row>
-    <row r="59" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A59" s="97" t="s">
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="14"/>
+      <c r="I60" s="14"/>
+      <c r="J60" s="14"/>
+      <c r="K60" s="14"/>
+      <c r="L60" s="6"/>
+      <c r="M60" s="15"/>
+    </row>
+    <row r="61" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A61" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="B59" s="97" t="s">
+      <c r="B61" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="C59" s="94" t="s">
+      <c r="C61" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="D59" s="94" t="s">
+      <c r="D61" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="E59" s="94" t="s">
+      <c r="E61" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="F59" s="95" t="s">
+      <c r="F61" s="104" t="s">
         <v>33</v>
       </c>
-      <c r="G59" s="95" t="s">
+      <c r="G61" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="H59" s="105" t="s">
+      <c r="H61" s="102" t="s">
         <v>115</v>
       </c>
-      <c r="I59" s="94" t="s">
+      <c r="I61" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="J59" s="94"/>
-      <c r="K59" s="16"/>
-      <c r="L59" s="17"/>
-      <c r="M59" s="9"/>
-    </row>
-    <row r="60" spans="1:13">
-      <c r="A60" s="97"/>
-      <c r="B60" s="97"/>
-      <c r="C60" s="94"/>
-      <c r="D60" s="94"/>
-      <c r="E60" s="94"/>
-      <c r="F60" s="96"/>
-      <c r="G60" s="96"/>
-      <c r="H60" s="106"/>
-      <c r="I60" s="94"/>
-      <c r="J60" s="94"/>
-      <c r="K60" s="18"/>
-      <c r="L60" s="29"/>
-      <c r="M60" s="15"/>
-    </row>
-    <row r="61" spans="1:13">
-      <c r="A61" s="19">
-        <v>1</v>
-      </c>
-      <c r="B61" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="C61" s="78" t="s">
-        <v>48</v>
-      </c>
-      <c r="D61" s="20"/>
-      <c r="E61" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="F61" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="G61" s="69"/>
-      <c r="H61" s="69"/>
-      <c r="I61" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="J61" s="21"/>
-      <c r="K61" s="21"/>
-      <c r="L61" s="28"/>
-      <c r="M61" s="15"/>
+      <c r="J61" s="100"/>
+      <c r="K61" s="16"/>
+      <c r="L61" s="17"/>
+      <c r="M61" s="9"/>
     </row>
     <row r="62" spans="1:13">
-      <c r="A62" s="19">
-        <f>A61+1</f>
-        <v>2</v>
-      </c>
-      <c r="B62" s="71" t="s">
-        <v>50</v>
-      </c>
-      <c r="C62" s="78" t="s">
-        <v>51</v>
-      </c>
-      <c r="D62" s="20"/>
-      <c r="E62" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="F62" s="20"/>
-      <c r="G62" s="69"/>
-      <c r="H62" s="69"/>
-      <c r="I62" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="J62" s="21"/>
-      <c r="K62" s="21"/>
-      <c r="L62" s="28"/>
+      <c r="A62" s="101"/>
+      <c r="B62" s="101"/>
+      <c r="C62" s="100"/>
+      <c r="D62" s="100"/>
+      <c r="E62" s="100"/>
+      <c r="F62" s="105"/>
+      <c r="G62" s="105"/>
+      <c r="H62" s="103"/>
+      <c r="I62" s="100"/>
+      <c r="J62" s="100"/>
+      <c r="K62" s="18"/>
+      <c r="L62" s="29"/>
       <c r="M62" s="15"/>
     </row>
     <row r="63" spans="1:13">
       <c r="A63" s="19">
-        <f t="shared" ref="A63:A77" si="0">A62+1</f>
-        <v>3</v>
-      </c>
-      <c r="B63" s="72" t="s">
-        <v>53</v>
-      </c>
-      <c r="C63" s="79" t="s">
-        <v>54</v>
-      </c>
-      <c r="D63" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="E63" s="20"/>
-      <c r="F63" s="20"/>
-      <c r="G63" s="69" t="s">
+        <v>1</v>
+      </c>
+      <c r="B63" s="71" t="s">
+        <v>47</v>
+      </c>
+      <c r="C63" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="D63" s="20"/>
+      <c r="E63" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F63" s="20" t="s">
         <v>14</v>
       </c>
+      <c r="G63" s="69"/>
       <c r="H63" s="69"/>
       <c r="I63" s="20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J63" s="21"/>
       <c r="K63" s="21"/>
-      <c r="L63" s="22"/>
+      <c r="L63" s="28"/>
       <c r="M63" s="15"/>
     </row>
     <row r="64" spans="1:13">
       <c r="A64" s="19">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B64" s="73" t="s">
-        <v>59</v>
-      </c>
-      <c r="C64" s="80" t="s">
-        <v>55</v>
+        <f>A63+1</f>
+        <v>2</v>
+      </c>
+      <c r="B64" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="C64" s="78" t="s">
+        <v>51</v>
       </c>
       <c r="D64" s="20"/>
-      <c r="E64" s="20"/>
+      <c r="E64" s="20" t="b">
+        <v>1</v>
+      </c>
       <c r="F64" s="20"/>
-      <c r="G64" s="69" t="s">
-        <v>14</v>
-      </c>
+      <c r="G64" s="69"/>
       <c r="H64" s="69"/>
       <c r="I64" s="20" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="J64" s="21"/>
       <c r="K64" s="21"/>
-      <c r="L64" s="22"/>
+      <c r="L64" s="28"/>
       <c r="M64" s="15"/>
     </row>
     <row r="65" spans="1:13">
       <c r="A65" s="19">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B65" s="73" t="s">
-        <v>116</v>
-      </c>
-      <c r="C65" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="D65" s="20"/>
+        <f t="shared" ref="A65:A79" si="0">A64+1</f>
+        <v>3</v>
+      </c>
+      <c r="B65" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="C65" s="79" t="s">
+        <v>54</v>
+      </c>
+      <c r="D65" s="20" t="s">
+        <v>55</v>
+      </c>
       <c r="E65" s="20"/>
       <c r="F65" s="20"/>
       <c r="G65" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="H65" s="69" t="s">
-        <v>116</v>
-      </c>
+      <c r="H65" s="69"/>
       <c r="I65" s="20" t="s">
-        <v>117</v>
+        <v>56</v>
       </c>
       <c r="J65" s="21"/>
       <c r="K65" s="21"/>
@@ -3503,34 +3531,52 @@
     <row r="66" spans="1:13">
       <c r="A66" s="19">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B66" s="73"/>
-      <c r="C66" s="80"/>
-      <c r="D66" s="74"/>
-      <c r="E66" s="74"/>
-      <c r="F66" s="74"/>
-      <c r="G66" s="75"/>
-      <c r="H66" s="75"/>
-      <c r="I66" s="74"/>
-      <c r="J66" s="76"/>
-      <c r="K66" s="76"/>
-      <c r="L66" s="77"/>
+        <v>4</v>
+      </c>
+      <c r="B66" s="73" t="s">
+        <v>59</v>
+      </c>
+      <c r="C66" s="80" t="s">
+        <v>55</v>
+      </c>
+      <c r="D66" s="20"/>
+      <c r="E66" s="20"/>
+      <c r="F66" s="20"/>
+      <c r="G66" s="69" t="s">
+        <v>14</v>
+      </c>
+      <c r="H66" s="69"/>
+      <c r="I66" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="J66" s="21"/>
+      <c r="K66" s="21"/>
+      <c r="L66" s="22"/>
       <c r="M66" s="15"/>
     </row>
     <row r="67" spans="1:13">
       <c r="A67" s="19">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B67" s="73"/>
-      <c r="C67" s="80"/>
+        <v>5</v>
+      </c>
+      <c r="B67" s="73" t="s">
+        <v>116</v>
+      </c>
+      <c r="C67" s="80" t="s">
+        <v>48</v>
+      </c>
       <c r="D67" s="20"/>
       <c r="E67" s="20"/>
       <c r="F67" s="20"/>
-      <c r="G67" s="69"/>
-      <c r="H67" s="69"/>
-      <c r="I67" s="20"/>
+      <c r="G67" s="69" t="s">
+        <v>14</v>
+      </c>
+      <c r="H67" s="69" t="s">
+        <v>116</v>
+      </c>
+      <c r="I67" s="20" t="s">
+        <v>117</v>
+      </c>
       <c r="J67" s="21"/>
       <c r="K67" s="21"/>
       <c r="L67" s="22"/>
@@ -3539,7 +3585,7 @@
     <row r="68" spans="1:13">
       <c r="A68" s="19">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B68" s="73"/>
       <c r="C68" s="80"/>
@@ -3557,43 +3603,43 @@
     <row r="69" spans="1:13">
       <c r="A69" s="19">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B69" s="73"/>
       <c r="C69" s="80"/>
-      <c r="D69" s="74"/>
-      <c r="E69" s="74"/>
-      <c r="F69" s="74"/>
-      <c r="G69" s="75"/>
-      <c r="H69" s="75"/>
-      <c r="I69" s="74"/>
-      <c r="J69" s="76"/>
-      <c r="K69" s="76"/>
-      <c r="L69" s="77"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="20"/>
+      <c r="F69" s="20"/>
+      <c r="G69" s="69"/>
+      <c r="H69" s="69"/>
+      <c r="I69" s="20"/>
+      <c r="J69" s="21"/>
+      <c r="K69" s="21"/>
+      <c r="L69" s="22"/>
       <c r="M69" s="15"/>
     </row>
     <row r="70" spans="1:13">
       <c r="A70" s="19">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B70" s="73"/>
       <c r="C70" s="80"/>
-      <c r="D70" s="20"/>
-      <c r="E70" s="20"/>
-      <c r="F70" s="20"/>
-      <c r="G70" s="69"/>
-      <c r="H70" s="69"/>
-      <c r="I70" s="20"/>
-      <c r="J70" s="21"/>
-      <c r="K70" s="21"/>
-      <c r="L70" s="22"/>
+      <c r="D70" s="74"/>
+      <c r="E70" s="74"/>
+      <c r="F70" s="74"/>
+      <c r="G70" s="75"/>
+      <c r="H70" s="75"/>
+      <c r="I70" s="74"/>
+      <c r="J70" s="76"/>
+      <c r="K70" s="76"/>
+      <c r="L70" s="77"/>
       <c r="M70" s="15"/>
     </row>
     <row r="71" spans="1:13">
       <c r="A71" s="19">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B71" s="73"/>
       <c r="C71" s="80"/>
@@ -3611,43 +3657,43 @@
     <row r="72" spans="1:13">
       <c r="A72" s="19">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B72" s="73"/>
       <c r="C72" s="80"/>
-      <c r="D72" s="74"/>
-      <c r="E72" s="74"/>
-      <c r="F72" s="74"/>
-      <c r="G72" s="75"/>
-      <c r="H72" s="75"/>
-      <c r="I72" s="74"/>
-      <c r="J72" s="76"/>
-      <c r="K72" s="76"/>
-      <c r="L72" s="77"/>
+      <c r="D72" s="20"/>
+      <c r="E72" s="20"/>
+      <c r="F72" s="20"/>
+      <c r="G72" s="69"/>
+      <c r="H72" s="69"/>
+      <c r="I72" s="20"/>
+      <c r="J72" s="21"/>
+      <c r="K72" s="21"/>
+      <c r="L72" s="22"/>
       <c r="M72" s="15"/>
     </row>
     <row r="73" spans="1:13">
       <c r="A73" s="19">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B73" s="73"/>
       <c r="C73" s="80"/>
-      <c r="D73" s="20"/>
-      <c r="E73" s="20"/>
-      <c r="F73" s="20"/>
-      <c r="G73" s="69"/>
-      <c r="H73" s="69"/>
-      <c r="I73" s="20"/>
-      <c r="J73" s="21"/>
-      <c r="K73" s="21"/>
-      <c r="L73" s="22"/>
+      <c r="D73" s="74"/>
+      <c r="E73" s="74"/>
+      <c r="F73" s="74"/>
+      <c r="G73" s="75"/>
+      <c r="H73" s="75"/>
+      <c r="I73" s="74"/>
+      <c r="J73" s="76"/>
+      <c r="K73" s="76"/>
+      <c r="L73" s="77"/>
       <c r="M73" s="15"/>
     </row>
     <row r="74" spans="1:13">
       <c r="A74" s="19">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B74" s="73"/>
       <c r="C74" s="80"/>
@@ -3665,43 +3711,43 @@
     <row r="75" spans="1:13">
       <c r="A75" s="19">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B75" s="73"/>
       <c r="C75" s="80"/>
-      <c r="D75" s="74"/>
-      <c r="E75" s="74"/>
-      <c r="F75" s="74"/>
-      <c r="G75" s="75"/>
-      <c r="H75" s="75"/>
-      <c r="I75" s="74"/>
-      <c r="J75" s="76"/>
-      <c r="K75" s="76"/>
-      <c r="L75" s="77"/>
+      <c r="D75" s="20"/>
+      <c r="E75" s="20"/>
+      <c r="F75" s="20"/>
+      <c r="G75" s="69"/>
+      <c r="H75" s="69"/>
+      <c r="I75" s="20"/>
+      <c r="J75" s="21"/>
+      <c r="K75" s="21"/>
+      <c r="L75" s="22"/>
       <c r="M75" s="15"/>
     </row>
     <row r="76" spans="1:13">
       <c r="A76" s="19">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B76" s="73"/>
       <c r="C76" s="80"/>
-      <c r="D76" s="20"/>
-      <c r="E76" s="20"/>
-      <c r="F76" s="20"/>
-      <c r="G76" s="69"/>
-      <c r="H76" s="69"/>
-      <c r="I76" s="20"/>
-      <c r="J76" s="21"/>
-      <c r="K76" s="21"/>
-      <c r="L76" s="22"/>
+      <c r="D76" s="74"/>
+      <c r="E76" s="74"/>
+      <c r="F76" s="74"/>
+      <c r="G76" s="75"/>
+      <c r="H76" s="75"/>
+      <c r="I76" s="74"/>
+      <c r="J76" s="76"/>
+      <c r="K76" s="76"/>
+      <c r="L76" s="77"/>
       <c r="M76" s="15"/>
     </row>
     <row r="77" spans="1:13">
       <c r="A77" s="19">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B77" s="73"/>
       <c r="C77" s="80"/>
@@ -3717,94 +3763,100 @@
       <c r="M77" s="15"/>
     </row>
     <row r="78" spans="1:13">
-      <c r="A78" s="23"/>
-      <c r="B78" s="24"/>
-      <c r="C78" s="25"/>
-      <c r="D78" s="25"/>
-      <c r="E78" s="25"/>
-      <c r="F78" s="25"/>
-      <c r="G78" s="70"/>
-      <c r="H78" s="70"/>
-      <c r="I78" s="25"/>
-      <c r="J78" s="26"/>
-      <c r="K78" s="26"/>
-      <c r="L78" s="27"/>
+      <c r="A78" s="19">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B78" s="73"/>
+      <c r="C78" s="80"/>
+      <c r="D78" s="20"/>
+      <c r="E78" s="20"/>
+      <c r="F78" s="20"/>
+      <c r="G78" s="69"/>
+      <c r="H78" s="69"/>
+      <c r="I78" s="20"/>
+      <c r="J78" s="21"/>
+      <c r="K78" s="21"/>
+      <c r="L78" s="22"/>
       <c r="M78" s="15"/>
     </row>
+    <row r="79" spans="1:13">
+      <c r="A79" s="19">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B79" s="73"/>
+      <c r="C79" s="80"/>
+      <c r="D79" s="74"/>
+      <c r="E79" s="74"/>
+      <c r="F79" s="74"/>
+      <c r="G79" s="75"/>
+      <c r="H79" s="75"/>
+      <c r="I79" s="74"/>
+      <c r="J79" s="76"/>
+      <c r="K79" s="76"/>
+      <c r="L79" s="77"/>
+      <c r="M79" s="15"/>
+    </row>
     <row r="80" spans="1:13">
-      <c r="A80" s="30" t="s">
+      <c r="A80" s="23"/>
+      <c r="B80" s="24"/>
+      <c r="C80" s="25"/>
+      <c r="D80" s="25"/>
+      <c r="E80" s="25"/>
+      <c r="F80" s="25"/>
+      <c r="G80" s="70"/>
+      <c r="H80" s="70"/>
+      <c r="I80" s="25"/>
+      <c r="J80" s="26"/>
+      <c r="K80" s="26"/>
+      <c r="L80" s="27"/>
+      <c r="M80" s="15"/>
+    </row>
+    <row r="82" spans="1:13">
+      <c r="A82" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="B80" s="31"/>
-      <c r="C80" s="31"/>
-      <c r="D80" s="31"/>
-      <c r="E80" s="81"/>
-      <c r="F80" s="44" t="s">
+      <c r="B82" s="31"/>
+      <c r="C82" s="31"/>
+      <c r="D82" s="31"/>
+      <c r="E82" s="81"/>
+      <c r="F82" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="G80" s="44"/>
-      <c r="H80" s="44"/>
-      <c r="I80" s="44"/>
-      <c r="J80" s="43"/>
-      <c r="K80" s="43"/>
-      <c r="L80" s="43"/>
-      <c r="M80" s="43"/>
-    </row>
-    <row r="81" spans="1:13">
-      <c r="A81" s="47" t="s">
+      <c r="G82" s="44"/>
+      <c r="H82" s="44"/>
+      <c r="I82" s="44"/>
+      <c r="J82" s="43"/>
+      <c r="K82" s="43"/>
+      <c r="L82" s="43"/>
+      <c r="M82" s="43"/>
+    </row>
+    <row r="83" spans="1:13">
+      <c r="A83" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B81" s="42" t="s">
+      <c r="B83" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C81" s="42"/>
-      <c r="D81" s="42"/>
-      <c r="E81" s="82"/>
-      <c r="F81" s="67"/>
-      <c r="G81" s="67"/>
-      <c r="H81" s="67"/>
-      <c r="I81" s="67"/>
-      <c r="J81" s="44"/>
-      <c r="K81" s="45"/>
-      <c r="L81" s="45"/>
-      <c r="M81" s="35"/>
-    </row>
-    <row r="82" spans="1:13">
-      <c r="A82" s="51"/>
-      <c r="B82" s="46"/>
-      <c r="C82" s="38"/>
-      <c r="D82" s="38"/>
-      <c r="E82" s="39"/>
-      <c r="F82" s="68"/>
-      <c r="G82" s="68"/>
-      <c r="H82" s="68"/>
-      <c r="I82" s="34"/>
-      <c r="J82" s="36"/>
-      <c r="K82" s="36"/>
-      <c r="L82" s="36"/>
-      <c r="M82" s="35"/>
-    </row>
-    <row r="83" spans="1:13">
-      <c r="A83" s="51"/>
-      <c r="B83" s="46"/>
-      <c r="C83" s="40"/>
-      <c r="D83" s="40"/>
-      <c r="E83" s="41"/>
-      <c r="F83" s="68"/>
-      <c r="G83" s="68"/>
-      <c r="H83" s="68"/>
-      <c r="I83" s="34"/>
-      <c r="J83" s="36"/>
-      <c r="K83" s="36"/>
-      <c r="L83" s="36"/>
+      <c r="C83" s="42"/>
+      <c r="D83" s="42"/>
+      <c r="E83" s="82"/>
+      <c r="F83" s="67"/>
+      <c r="G83" s="67"/>
+      <c r="H83" s="67"/>
+      <c r="I83" s="67"/>
+      <c r="J83" s="44"/>
+      <c r="K83" s="45"/>
+      <c r="L83" s="45"/>
       <c r="M83" s="35"/>
     </row>
     <row r="84" spans="1:13">
-      <c r="A84" s="52"/>
-      <c r="B84" s="48"/>
-      <c r="C84" s="49"/>
-      <c r="D84" s="49"/>
-      <c r="E84" s="50"/>
+      <c r="A84" s="51"/>
+      <c r="B84" s="46"/>
+      <c r="C84" s="38"/>
+      <c r="D84" s="38"/>
+      <c r="E84" s="39"/>
       <c r="F84" s="68"/>
       <c r="G84" s="68"/>
       <c r="H84" s="68"/>
@@ -3815,151 +3867,131 @@
       <c r="M84" s="35"/>
     </row>
     <row r="85" spans="1:13">
-      <c r="A85" s="13"/>
-      <c r="B85" s="13"/>
-      <c r="C85" s="13"/>
-      <c r="D85" s="13"/>
-      <c r="E85" s="13"/>
-      <c r="F85" s="13"/>
-      <c r="G85" s="13"/>
-      <c r="H85" s="13"/>
-      <c r="I85" s="13"/>
-      <c r="J85" s="13"/>
+      <c r="A85" s="51"/>
+      <c r="B85" s="46"/>
+      <c r="C85" s="40"/>
+      <c r="D85" s="40"/>
+      <c r="E85" s="41"/>
+      <c r="F85" s="68"/>
+      <c r="G85" s="68"/>
+      <c r="H85" s="68"/>
+      <c r="I85" s="34"/>
+      <c r="J85" s="36"/>
+      <c r="K85" s="36"/>
+      <c r="L85" s="36"/>
+      <c r="M85" s="35"/>
     </row>
     <row r="86" spans="1:13">
-      <c r="A86" s="13"/>
-      <c r="B86" s="13" t="s">
+      <c r="A86" s="52"/>
+      <c r="B86" s="48"/>
+      <c r="C86" s="49"/>
+      <c r="D86" s="49"/>
+      <c r="E86" s="50"/>
+      <c r="F86" s="68"/>
+      <c r="G86" s="68"/>
+      <c r="H86" s="68"/>
+      <c r="I86" s="34"/>
+      <c r="J86" s="36"/>
+      <c r="K86" s="36"/>
+      <c r="L86" s="36"/>
+      <c r="M86" s="35"/>
+    </row>
+    <row r="87" spans="1:13">
+      <c r="A87" s="13"/>
+      <c r="B87" s="13"/>
+      <c r="C87" s="13"/>
+      <c r="D87" s="13"/>
+      <c r="E87" s="13"/>
+      <c r="F87" s="13"/>
+      <c r="G87" s="13"/>
+      <c r="H87" s="13"/>
+      <c r="I87" s="13"/>
+      <c r="J87" s="13"/>
+    </row>
+    <row r="88" spans="1:13">
+      <c r="A88" s="13"/>
+      <c r="B88" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="C86" s="13"/>
-      <c r="D86" s="13"/>
-      <c r="E86" s="13"/>
-      <c r="F86" s="13"/>
-      <c r="G86" s="13"/>
-      <c r="H86" s="13"/>
-      <c r="I86" s="13"/>
-      <c r="J86" s="13"/>
-    </row>
-    <row r="87" spans="1:13">
-      <c r="A87" s="3" t="s">
+      <c r="C88" s="13"/>
+      <c r="D88" s="13"/>
+      <c r="E88" s="13"/>
+      <c r="F88" s="13"/>
+      <c r="G88" s="13"/>
+      <c r="H88" s="13"/>
+      <c r="I88" s="13"/>
+      <c r="J88" s="13"/>
+    </row>
+    <row r="89" spans="1:13">
+      <c r="A89" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B87" s="14"/>
-      <c r="C87" s="14"/>
-      <c r="D87" s="14"/>
-      <c r="E87" s="14"/>
-      <c r="F87" s="14"/>
-      <c r="G87" s="14"/>
-      <c r="H87" s="14"/>
-      <c r="I87" s="14"/>
-      <c r="J87" s="14"/>
-      <c r="K87" s="14"/>
-      <c r="L87" s="6"/>
-      <c r="M87" s="15"/>
-    </row>
-    <row r="88" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A88" s="97" t="s">
+      <c r="B89" s="14"/>
+      <c r="C89" s="14"/>
+      <c r="D89" s="14"/>
+      <c r="E89" s="14"/>
+      <c r="F89" s="14"/>
+      <c r="G89" s="14"/>
+      <c r="H89" s="14"/>
+      <c r="I89" s="14"/>
+      <c r="J89" s="14"/>
+      <c r="K89" s="14"/>
+      <c r="L89" s="6"/>
+      <c r="M89" s="15"/>
+    </row>
+    <row r="90" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A90" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="B88" s="97" t="s">
+      <c r="B90" s="101" t="s">
         <v>93</v>
       </c>
-      <c r="C88" s="94" t="s">
+      <c r="C90" s="100" t="s">
         <v>95</v>
       </c>
-      <c r="D88" s="94" t="s">
+      <c r="D90" s="100" t="s">
         <v>96</v>
       </c>
-      <c r="E88" s="94" t="s">
+      <c r="E90" s="100" t="s">
         <v>86</v>
       </c>
-      <c r="F88" s="91"/>
-      <c r="G88" s="91"/>
-      <c r="H88" s="91"/>
-      <c r="I88" s="93"/>
-      <c r="J88" s="94"/>
-      <c r="K88" s="16"/>
-      <c r="L88" s="17"/>
-      <c r="M88" s="9"/>
-    </row>
-    <row r="89" spans="1:13">
-      <c r="A89" s="97"/>
-      <c r="B89" s="97"/>
-      <c r="C89" s="94"/>
-      <c r="D89" s="94"/>
-      <c r="E89" s="94"/>
-      <c r="F89" s="92"/>
-      <c r="G89" s="92"/>
-      <c r="H89" s="92"/>
-      <c r="I89" s="93"/>
-      <c r="J89" s="94"/>
-      <c r="K89" s="18"/>
-      <c r="L89" s="29"/>
-      <c r="M89" s="15"/>
-    </row>
-    <row r="90" spans="1:13">
-      <c r="A90" s="19">
-        <v>1</v>
-      </c>
-      <c r="B90" s="71" t="s">
-        <v>97</v>
-      </c>
-      <c r="C90" s="78" t="s">
-        <v>48</v>
-      </c>
-      <c r="D90" s="20"/>
-      <c r="E90" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="F90" s="87"/>
-      <c r="G90" s="89"/>
-      <c r="H90" s="89"/>
-      <c r="I90" s="87"/>
-      <c r="J90" s="21"/>
-      <c r="K90" s="21"/>
-      <c r="L90" s="28"/>
-      <c r="M90" s="15"/>
+      <c r="F90" s="111"/>
+      <c r="G90" s="111"/>
+      <c r="H90" s="111"/>
+      <c r="I90" s="113"/>
+      <c r="J90" s="100"/>
+      <c r="K90" s="16"/>
+      <c r="L90" s="17"/>
+      <c r="M90" s="9"/>
     </row>
     <row r="91" spans="1:13">
-      <c r="A91" s="19">
-        <f>A90+1</f>
-        <v>2</v>
-      </c>
-      <c r="B91" s="71" t="s">
-        <v>98</v>
-      </c>
-      <c r="C91" s="78" t="s">
-        <v>99</v>
-      </c>
-      <c r="D91" s="20"/>
-      <c r="E91" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="F91" s="87"/>
-      <c r="G91" s="89"/>
-      <c r="H91" s="89"/>
-      <c r="I91" s="87"/>
-      <c r="J91" s="21"/>
-      <c r="K91" s="21"/>
-      <c r="L91" s="28"/>
+      <c r="A91" s="101"/>
+      <c r="B91" s="101"/>
+      <c r="C91" s="100"/>
+      <c r="D91" s="100"/>
+      <c r="E91" s="100"/>
+      <c r="F91" s="112"/>
+      <c r="G91" s="112"/>
+      <c r="H91" s="112"/>
+      <c r="I91" s="113"/>
+      <c r="J91" s="100"/>
+      <c r="K91" s="18"/>
+      <c r="L91" s="29"/>
       <c r="M91" s="15"/>
     </row>
     <row r="92" spans="1:13">
       <c r="A92" s="19">
-        <f t="shared" ref="A92:A96" si="1">A91+1</f>
-        <v>3</v>
-      </c>
-      <c r="B92" s="72" t="s">
-        <v>110</v>
-      </c>
-      <c r="C92" s="79" t="s">
-        <v>54</v>
-      </c>
-      <c r="D92" s="20" t="s">
-        <v>55</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="B92" s="71" t="s">
+        <v>97</v>
+      </c>
+      <c r="C92" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="D92" s="20"/>
       <c r="E92" s="20" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F92" s="87"/>
       <c r="G92" s="89"/>
@@ -3967,36 +3999,50 @@
       <c r="I92" s="87"/>
       <c r="J92" s="21"/>
       <c r="K92" s="21"/>
-      <c r="L92" s="22"/>
+      <c r="L92" s="28"/>
       <c r="M92" s="15"/>
     </row>
     <row r="93" spans="1:13">
       <c r="A93" s="19">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="B93" s="73"/>
-      <c r="C93" s="80"/>
+        <f>A92+1</f>
+        <v>2</v>
+      </c>
+      <c r="B93" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="C93" s="78" t="s">
+        <v>99</v>
+      </c>
       <c r="D93" s="20"/>
-      <c r="E93" s="20"/>
+      <c r="E93" s="20" t="s">
+        <v>109</v>
+      </c>
       <c r="F93" s="87"/>
       <c r="G93" s="89"/>
       <c r="H93" s="89"/>
       <c r="I93" s="87"/>
       <c r="J93" s="21"/>
       <c r="K93" s="21"/>
-      <c r="L93" s="22"/>
+      <c r="L93" s="28"/>
       <c r="M93" s="15"/>
     </row>
     <row r="94" spans="1:13">
       <c r="A94" s="19">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="B94" s="73"/>
-      <c r="C94" s="80"/>
-      <c r="D94" s="20"/>
-      <c r="E94" s="20"/>
+        <f t="shared" ref="A94:A98" si="1">A93+1</f>
+        <v>3</v>
+      </c>
+      <c r="B94" s="72" t="s">
+        <v>110</v>
+      </c>
+      <c r="C94" s="79" t="s">
+        <v>54</v>
+      </c>
+      <c r="D94" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="E94" s="20" t="s">
+        <v>111</v>
+      </c>
       <c r="F94" s="87"/>
       <c r="G94" s="89"/>
       <c r="H94" s="89"/>
@@ -4009,25 +4055,25 @@
     <row r="95" spans="1:13">
       <c r="A95" s="19">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B95" s="73"/>
       <c r="C95" s="80"/>
-      <c r="D95" s="74"/>
-      <c r="E95" s="74"/>
-      <c r="F95" s="88"/>
-      <c r="G95" s="90"/>
-      <c r="H95" s="90"/>
-      <c r="I95" s="88"/>
-      <c r="J95" s="76"/>
-      <c r="K95" s="76"/>
-      <c r="L95" s="77"/>
+      <c r="D95" s="20"/>
+      <c r="E95" s="20"/>
+      <c r="F95" s="87"/>
+      <c r="G95" s="89"/>
+      <c r="H95" s="89"/>
+      <c r="I95" s="87"/>
+      <c r="J95" s="21"/>
+      <c r="K95" s="21"/>
+      <c r="L95" s="22"/>
       <c r="M95" s="15"/>
     </row>
     <row r="96" spans="1:13">
       <c r="A96" s="19">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B96" s="73"/>
       <c r="C96" s="80"/>
@@ -4042,54 +4088,91 @@
       <c r="L96" s="22"/>
       <c r="M96" s="15"/>
     </row>
+    <row r="97" spans="1:13">
+      <c r="A97" s="19">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B97" s="73"/>
+      <c r="C97" s="80"/>
+      <c r="D97" s="74"/>
+      <c r="E97" s="74"/>
+      <c r="F97" s="88"/>
+      <c r="G97" s="90"/>
+      <c r="H97" s="90"/>
+      <c r="I97" s="88"/>
+      <c r="J97" s="76"/>
+      <c r="K97" s="76"/>
+      <c r="L97" s="77"/>
+      <c r="M97" s="15"/>
+    </row>
+    <row r="98" spans="1:13">
+      <c r="A98" s="19">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B98" s="73"/>
+      <c r="C98" s="80"/>
+      <c r="D98" s="20"/>
+      <c r="E98" s="20"/>
+      <c r="F98" s="87"/>
+      <c r="G98" s="89"/>
+      <c r="H98" s="89"/>
+      <c r="I98" s="87"/>
+      <c r="J98" s="21"/>
+      <c r="K98" s="21"/>
+      <c r="L98" s="22"/>
+      <c r="M98" s="15"/>
+    </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="A24:B24"/>
+  <mergeCells count="27">
     <mergeCell ref="A22:B22"/>
-    <mergeCell ref="I59:J60"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="F90:F91"/>
+    <mergeCell ref="H90:H91"/>
+    <mergeCell ref="I90:J91"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="G90:G91"/>
+    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="B90:B91"/>
+    <mergeCell ref="C90:C91"/>
+    <mergeCell ref="D90:D91"/>
+    <mergeCell ref="E90:E91"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="C14:E14"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="B88:B89"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="D88:D89"/>
-    <mergeCell ref="E88:E89"/>
-    <mergeCell ref="F88:F89"/>
-    <mergeCell ref="H88:H89"/>
-    <mergeCell ref="I88:J89"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="G88:G89"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="I61:J62"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="E61:E62"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="H61:H62"/>
+    <mergeCell ref="F61:F62"/>
+    <mergeCell ref="A26:B26"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E100:H100" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E102:H102" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C24:C25" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25:C26" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
       <formula1>adjustFiledName</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
       <formula1>componentKind</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17:C22 F61:G78" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F63:G80 C17:C22" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>yesNo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C23" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C24" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">
       <formula1>adjustFieldName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C47:C49" xr:uid="{BDE40890-40F7-4E41-B7E1-478CEBD85557}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C49:C51" xr:uid="{BDE40890-40F7-4E41-B7E1-478CEBD85557}">
       <formula1>httpdMethod</formula1>
     </dataValidation>
   </dataValidations>
@@ -4173,7 +4256,7 @@
       <c r="D4" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="107"/>
+      <c r="F4" s="91"/>
       <c r="H4" s="58"/>
       <c r="J4" s="58"/>
       <c r="L4" s="58"/>
@@ -4183,7 +4266,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="60"/>
-      <c r="F5" s="108" t="s">
+      <c r="F5" s="92" t="s">
         <v>122</v>
       </c>
       <c r="H5" s="60" t="s">
@@ -4198,17 +4281,17 @@
     </row>
     <row r="6" spans="1:12">
       <c r="B6" s="61"/>
-      <c r="F6" s="108" t="s">
+      <c r="F6" s="92" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="F7" s="109" t="s">
+      <c r="F7" s="93" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="F8" s="110" t="s">
+      <c r="F8" s="94" t="s">
         <v>126</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1.0.6: Fix typo of BeforeRouterLeave to BeforeRouteLeave.
</commit_message>
<xml_diff>
--- a/meta/components/BoxSample.xlsx
+++ b/meta/components/BoxSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVueComponent/meta/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E968AE2-E77B-974B-A76F-B6CE299FDFEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260DDDC2-2B82-C443-BA31-5BB5AF54D38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1037,16 +1037,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>BeforeRouterLeave関数名</t>
-    <rPh sb="17" eb="19">
-      <t xml:space="preserve">カンスウ </t>
-    </rPh>
-    <rPh sb="19" eb="20">
-      <t xml:space="preserve">メイ </t>
-    </rPh>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>RouterHooks.beforeRouterLeave</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -1077,6 +1067,16 @@
       <t xml:space="preserve">テイギ </t>
     </rPh>
     <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>BeforeRouteLeave関数名</t>
+    <rPh sb="16" eb="18">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t xml:space="preserve">メイ </t>
+    </rPh>
+    <phoneticPr fontId="6"/>
   </si>
 </sst>
 </file>
@@ -2412,7 +2412,7 @@
   <dimension ref="A1:M98"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2747,14 +2747,14 @@
     </row>
     <row r="23" spans="1:13" s="32" customFormat="1">
       <c r="A23" s="98" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B23" s="99"/>
       <c r="C23" s="64" t="s">
+        <v>129</v>
+      </c>
+      <c r="D23" t="s">
         <v>130</v>
-      </c>
-      <c r="D23" t="s">
-        <v>131</v>
       </c>
       <c r="E23"/>
       <c r="F23"/>

</xml_diff>

<commit_message>
3.0.4: Implement layoutType property to RouteRecordRaw.meta.
</commit_message>
<xml_diff>
--- a/meta/components/BoxSample.xlsx
+++ b/meta/components/BoxSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVueComponent/meta/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260DDDC2-2B82-C443-BA31-5BB5AF54D38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15B9429-0BAE-DB42-AAC9-DFB86EC8E362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,6 +23,7 @@
     <definedName name="componentKind">config!$B$4:$B$5</definedName>
     <definedName name="createToString">config!$H$4:$H$5</definedName>
     <definedName name="httpdMethod">config!$F$4:$F$8</definedName>
+    <definedName name="layoutType">config!$N$3:$N$7</definedName>
     <definedName name="yesNo">config!$D$4:$D$5</definedName>
     <definedName name="チェック種別" localSheetId="1">#REF!</definedName>
     <definedName name="チェック種別">#REF!</definedName>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="138">
   <si>
     <t>パッケージ</t>
   </si>
@@ -1077,6 +1078,38 @@
       <t xml:space="preserve">メイ </t>
     </rPh>
     <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>レイアウト</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>/* 画面レイアウト識別子 */</t>
+    <rPh sb="3" eb="5">
+      <t xml:space="preserve">ガメンレイアウト </t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t xml:space="preserve">シキベツ </t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t xml:space="preserve">シ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>default</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>complex</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>simple</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>simple</t>
   </si>
 </sst>
 </file>
@@ -1773,27 +1806,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1802,38 +1834,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1845,8 +1870,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1879,18 +1904,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1900,12 +1923,12 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1919,16 +1942,16 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1947,33 +1970,39 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1989,14 +2018,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2409,10 +2435,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M98"/>
+  <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2454,9 +2480,6 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="3" t="s">
@@ -2468,12 +2491,9 @@
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="35"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="3" t="s">
@@ -2485,12 +2505,9 @@
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="34" t="s">
+      <c r="F7" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="35"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="3" t="s">
@@ -2502,12 +2519,9 @@
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="8"/>
-      <c r="F8" s="34" t="s">
+      <c r="F8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="35"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="3" t="s">
@@ -2517,99 +2531,81 @@
       <c r="C9" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="33"/>
+      <c r="D9" s="31"/>
       <c r="E9" s="11"/>
-      <c r="F9" s="34" t="s">
+      <c r="F9" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="35"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="106" t="s">
+      <c r="A10" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="107"/>
+      <c r="B10" s="99"/>
       <c r="C10" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="33"/>
+      <c r="D10" s="31"/>
       <c r="E10" s="11"/>
-      <c r="F10" s="34" t="s">
+      <c r="F10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="35"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="106" t="s">
+      <c r="A11" s="98" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="107"/>
+      <c r="B11" s="99"/>
       <c r="C11" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="33"/>
+      <c r="D11" s="31"/>
       <c r="E11" s="11"/>
-      <c r="F11" s="34" t="s">
+      <c r="F11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="35"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="106" t="s">
+      <c r="A12" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="107"/>
+      <c r="B12" s="99"/>
       <c r="C12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="33"/>
+      <c r="D12" s="31"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="34" t="s">
+      <c r="F12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="35"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="106" t="s">
+      <c r="A13" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="107"/>
-      <c r="C13" s="86" t="s">
+      <c r="B13" s="99"/>
+      <c r="C13" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="D13" s="33"/>
+      <c r="D13" s="31"/>
       <c r="E13" s="11"/>
-      <c r="F13" s="34" t="s">
+      <c r="F13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="35"/>
     </row>
     <row r="14" spans="1:11" ht="45" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="108" t="s">
+      <c r="C14" s="100" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="109"/>
-      <c r="E14" s="110"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
+      <c r="D14" s="101"/>
+      <c r="E14" s="102"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="3" t="s">
@@ -2621,19 +2617,13 @@
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="8"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-    </row>
-    <row r="16" spans="1:11" s="32" customFormat="1">
-      <c r="A16" s="62" t="s">
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="63"/>
-      <c r="C16" s="64" t="s">
+      <c r="B16" s="13"/>
+      <c r="C16" s="55" t="s">
         <v>27</v>
       </c>
       <c r="D16" t="s">
@@ -2641,16 +2631,16 @@
       </c>
       <c r="E16"/>
       <c r="F16"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="66"/>
+      <c r="G16"/>
+      <c r="H16"/>
       <c r="I16"/>
     </row>
-    <row r="17" spans="1:13" s="32" customFormat="1">
-      <c r="A17" s="62" t="s">
+    <row r="17" spans="1:12">
+      <c r="A17" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="63"/>
-      <c r="C17" s="64" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D17" t="s">
@@ -2658,1522 +2648,1436 @@
       </c>
       <c r="E17"/>
       <c r="F17"/>
-      <c r="G17" s="66"/>
-      <c r="H17" s="66"/>
+      <c r="G17"/>
+      <c r="H17"/>
       <c r="I17"/>
     </row>
-    <row r="18" spans="1:13" s="32" customFormat="1">
-      <c r="A18" s="62" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="63"/>
-      <c r="C18" s="64"/>
+    <row r="18" spans="1:12">
+      <c r="A18" s="54" t="s">
+        <v>132</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="55" t="s">
+        <v>137</v>
+      </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>133</v>
       </c>
       <c r="E18"/>
       <c r="F18"/>
-      <c r="G18" s="66"/>
-      <c r="H18" s="66"/>
+      <c r="G18"/>
+      <c r="H18"/>
       <c r="I18"/>
     </row>
-    <row r="19" spans="1:13" s="32" customFormat="1">
-      <c r="A19" s="62" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="63"/>
-      <c r="C19" s="64" t="s">
-        <v>14</v>
-      </c>
+    <row r="19" spans="1:12">
+      <c r="A19" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="55"/>
       <c r="D19" t="s">
-        <v>78</v>
+        <v>36</v>
       </c>
       <c r="E19"/>
       <c r="F19"/>
-      <c r="G19" s="66"/>
-      <c r="H19" s="66"/>
+      <c r="G19"/>
+      <c r="H19"/>
       <c r="I19"/>
     </row>
-    <row r="20" spans="1:13" s="32" customFormat="1">
-      <c r="A20" s="62" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="63"/>
-      <c r="C20" s="64" t="s">
+    <row r="20" spans="1:12">
+      <c r="A20" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="13"/>
+      <c r="C20" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="E20"/>
       <c r="F20"/>
-      <c r="G20" s="66"/>
-      <c r="H20" s="66"/>
+      <c r="G20"/>
+      <c r="H20"/>
       <c r="I20"/>
     </row>
-    <row r="21" spans="1:13" s="32" customFormat="1">
-      <c r="A21" s="62" t="s">
-        <v>81</v>
-      </c>
-      <c r="B21" s="63"/>
-      <c r="C21" s="64" t="s">
+    <row r="21" spans="1:12">
+      <c r="A21" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="13"/>
+      <c r="C21" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
       <c r="E21"/>
       <c r="F21"/>
-      <c r="G21" s="66"/>
-      <c r="H21" s="66"/>
+      <c r="G21"/>
+      <c r="H21"/>
       <c r="I21"/>
     </row>
-    <row r="22" spans="1:13" s="32" customFormat="1">
-      <c r="A22" s="98" t="s">
-        <v>82</v>
-      </c>
-      <c r="B22" s="99"/>
-      <c r="C22" s="64" t="s">
+    <row r="22" spans="1:12">
+      <c r="A22" s="54" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="13"/>
+      <c r="C22" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E22"/>
       <c r="F22"/>
-      <c r="G22" s="66"/>
-      <c r="H22" s="66"/>
+      <c r="G22"/>
+      <c r="H22"/>
       <c r="I22"/>
     </row>
-    <row r="23" spans="1:13" s="32" customFormat="1">
-      <c r="A23" s="98" t="s">
-        <v>131</v>
-      </c>
-      <c r="B23" s="99"/>
-      <c r="C23" s="64" t="s">
-        <v>129</v>
+    <row r="23" spans="1:12">
+      <c r="A23" s="89" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="90"/>
+      <c r="C23" s="55" t="s">
+        <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="E23"/>
       <c r="F23"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="66"/>
+      <c r="G23"/>
+      <c r="H23"/>
       <c r="I23"/>
     </row>
-    <row r="24" spans="1:13" s="32" customFormat="1">
-      <c r="A24" s="62" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="63"/>
-      <c r="C24" s="64" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24"/>
+    <row r="24" spans="1:12">
+      <c r="A24" s="89" t="s">
+        <v>131</v>
+      </c>
+      <c r="B24" s="90"/>
+      <c r="C24" s="55" t="s">
+        <v>129</v>
+      </c>
+      <c r="D24" t="s">
+        <v>130</v>
+      </c>
       <c r="E24"/>
       <c r="F24"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="66"/>
+      <c r="G24"/>
+      <c r="H24"/>
       <c r="I24"/>
     </row>
-    <row r="25" spans="1:13" s="32" customFormat="1">
-      <c r="A25" s="98" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="99"/>
-      <c r="C25" s="64" t="s">
+    <row r="25" spans="1:12">
+      <c r="A25" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="13"/>
+      <c r="C25" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="D25" t="s">
-        <v>19</v>
-      </c>
+      <c r="D25"/>
       <c r="E25"/>
       <c r="F25"/>
-      <c r="G25" s="66"/>
-      <c r="H25" s="66"/>
+      <c r="G25"/>
+      <c r="H25"/>
       <c r="I25"/>
     </row>
-    <row r="26" spans="1:13" s="32" customFormat="1">
-      <c r="A26" s="98" t="s">
-        <v>68</v>
-      </c>
-      <c r="B26" s="99"/>
-      <c r="C26" s="64" t="s">
+    <row r="26" spans="1:12">
+      <c r="A26" s="89" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="90"/>
+      <c r="C26" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="D26"/>
+      <c r="D26" t="s">
+        <v>19</v>
+      </c>
       <c r="E26"/>
       <c r="F26"/>
-      <c r="G26" s="66"/>
-      <c r="H26" s="66"/>
+      <c r="G26"/>
+      <c r="H26"/>
       <c r="I26"/>
     </row>
-    <row r="27" spans="1:13" s="37" customFormat="1">
-      <c r="A27" s="34"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="34"/>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28" s="30" t="s">
+    <row r="27" spans="1:12">
+      <c r="A27" s="89" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="90"/>
+      <c r="C27" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27"/>
+      <c r="I27"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="B28"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="81"/>
-      <c r="F28" s="44" t="s">
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="71"/>
+      <c r="F29" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="43"/>
-      <c r="K28" s="43"/>
-      <c r="L28" s="43"/>
-      <c r="M28" s="43"/>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="A29" s="47" t="s">
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="42" t="s">
+      <c r="B30" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="42"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="82"/>
-      <c r="F29" s="67"/>
-      <c r="G29" s="67"/>
-      <c r="H29" s="67"/>
-      <c r="I29" s="67"/>
-      <c r="J29" s="44"/>
-      <c r="K29" s="45"/>
-      <c r="L29" s="45"/>
-      <c r="M29" s="35"/>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="51">
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="72"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="57"/>
+      <c r="H30" s="57"/>
+      <c r="I30" s="57"/>
+      <c r="K30" s="37"/>
+      <c r="L30" s="37"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="43">
         <v>1</v>
       </c>
-      <c r="B30" s="46" t="s">
+      <c r="B31" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="68"/>
-      <c r="G30" s="68"/>
-      <c r="H30" s="68"/>
-      <c r="I30" s="34"/>
-      <c r="J30" s="36"/>
-      <c r="K30" s="36"/>
-      <c r="L30" s="36"/>
-      <c r="M30" s="35"/>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="51">
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="58"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="43">
         <v>2</v>
       </c>
-      <c r="B31" s="46" t="s">
+      <c r="B32" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="68"/>
-      <c r="G31" s="68"/>
-      <c r="H31" s="68"/>
-      <c r="I31" s="34"/>
-      <c r="J31" s="36"/>
-      <c r="K31" s="36"/>
-      <c r="L31" s="36"/>
-      <c r="M31" s="35"/>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="A32" s="51">
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="58"/>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="43">
         <v>3</v>
       </c>
-      <c r="B32" s="46" t="s">
+      <c r="B33" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="68"/>
-      <c r="G32" s="68"/>
-      <c r="H32" s="68"/>
-      <c r="I32" s="34"/>
-      <c r="J32" s="36"/>
-      <c r="K32" s="36"/>
-      <c r="L32" s="36"/>
-      <c r="M32" s="35"/>
-    </row>
-    <row r="33" spans="1:13">
-      <c r="A33" s="52"/>
-      <c r="B33" s="48"/>
-      <c r="C33" s="49"/>
-      <c r="D33" s="49"/>
-      <c r="E33" s="50"/>
-      <c r="F33" s="68"/>
-      <c r="G33" s="68"/>
-      <c r="H33" s="68"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="36"/>
-      <c r="K33" s="36"/>
-      <c r="L33" s="36"/>
-      <c r="M33" s="35"/>
-    </row>
-    <row r="34" spans="1:13">
-      <c r="A34" s="13"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
-    </row>
-    <row r="35" spans="1:13">
-      <c r="A35" s="30" t="s">
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="58"/>
+      <c r="H33" s="58"/>
+      <c r="J33"/>
+      <c r="K33"/>
+      <c r="L33"/>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="44"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="58"/>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34"/>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35"/>
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="81"/>
-      <c r="F35" s="44" t="s">
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="71"/>
+      <c r="F36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G35" s="44"/>
-      <c r="H35" s="44"/>
-      <c r="I35" s="44"/>
-      <c r="J35" s="43"/>
-      <c r="K35" s="43"/>
-      <c r="L35" s="43"/>
-      <c r="M35" s="43"/>
-    </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="47" t="s">
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="42" t="s">
+      <c r="B37" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="82"/>
-      <c r="F36" s="67"/>
-      <c r="G36" s="67"/>
-      <c r="H36" s="67"/>
-      <c r="I36" s="67"/>
-      <c r="J36" s="44"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
-      <c r="M36" s="35"/>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="A37" s="51">
+      <c r="C37" s="36"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="57"/>
+      <c r="H37" s="57"/>
+      <c r="I37" s="57"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="37"/>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="43">
         <v>1</v>
       </c>
-      <c r="B37" s="46" t="s">
+      <c r="B38" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="39"/>
-      <c r="F37" s="68"/>
-      <c r="G37" s="68"/>
-      <c r="H37" s="68"/>
-      <c r="I37" s="34"/>
-      <c r="J37" s="36"/>
-      <c r="K37" s="36"/>
-      <c r="L37" s="36"/>
-      <c r="M37" s="35"/>
-    </row>
-    <row r="38" spans="1:13">
-      <c r="A38" s="51">
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="58"/>
+      <c r="G38" s="58"/>
+      <c r="H38" s="58"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="43">
         <v>2</v>
       </c>
-      <c r="B38" s="46" t="s">
+      <c r="B39" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="40"/>
-      <c r="D38" s="40"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="68"/>
-      <c r="G38" s="68"/>
-      <c r="H38" s="68"/>
-      <c r="I38" s="34"/>
-      <c r="J38" s="36"/>
-      <c r="K38" s="36"/>
-      <c r="L38" s="36"/>
-      <c r="M38" s="35"/>
-    </row>
-    <row r="39" spans="1:13">
-      <c r="A39" s="52"/>
-      <c r="B39" s="48"/>
-      <c r="C39" s="49"/>
-      <c r="D39" s="49"/>
-      <c r="E39" s="50"/>
-      <c r="F39" s="68"/>
-      <c r="G39" s="68"/>
-      <c r="H39" s="68"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="36"/>
-      <c r="K39" s="36"/>
-      <c r="L39" s="36"/>
-      <c r="M39" s="35"/>
-    </row>
-    <row r="40" spans="1:13">
-      <c r="A40" s="83"/>
-      <c r="B40" s="84"/>
-      <c r="C40" s="85"/>
-      <c r="D40" s="85"/>
-      <c r="E40" s="85"/>
-      <c r="F40" s="68"/>
-      <c r="G40" s="68"/>
-      <c r="H40" s="68"/>
-      <c r="I40" s="34"/>
-      <c r="J40" s="36"/>
-      <c r="K40" s="36"/>
-      <c r="L40" s="36"/>
-      <c r="M40" s="35"/>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="A41" s="30" t="s">
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="58"/>
+      <c r="G39" s="58"/>
+      <c r="H39" s="58"/>
+      <c r="J39"/>
+      <c r="K39"/>
+      <c r="L39"/>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="44"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="41"/>
+      <c r="D40" s="41"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="58"/>
+      <c r="G40" s="58"/>
+      <c r="H40" s="58"/>
+      <c r="J40"/>
+      <c r="K40"/>
+      <c r="L40"/>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="73"/>
+      <c r="B41" s="74"/>
+      <c r="C41" s="75"/>
+      <c r="D41" s="75"/>
+      <c r="E41" s="75"/>
+      <c r="F41" s="58"/>
+      <c r="G41" s="58"/>
+      <c r="H41" s="58"/>
+      <c r="J41"/>
+      <c r="K41"/>
+      <c r="L41"/>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="B41" s="31"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="81"/>
-      <c r="F41" s="44" t="s">
+      <c r="B42" s="30"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="71"/>
+      <c r="F42" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G41" s="44"/>
-      <c r="H41" s="44"/>
-      <c r="I41" s="44"/>
-      <c r="J41" s="43"/>
-      <c r="K41" s="43"/>
-      <c r="L41" s="43"/>
-      <c r="M41" s="43"/>
-    </row>
-    <row r="42" spans="1:13">
-      <c r="A42" s="47" t="s">
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="42" t="s">
+      <c r="B43" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="82"/>
-      <c r="F42" s="67"/>
-      <c r="G42" s="67"/>
-      <c r="H42" s="67"/>
-      <c r="I42" s="67"/>
-      <c r="J42" s="44"/>
-      <c r="K42" s="45"/>
-      <c r="L42" s="45"/>
-      <c r="M42" s="35"/>
-    </row>
-    <row r="43" spans="1:13">
-      <c r="A43" s="51">
+      <c r="C43" s="36"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="72"/>
+      <c r="F43" s="57"/>
+      <c r="G43" s="57"/>
+      <c r="H43" s="57"/>
+      <c r="I43" s="57"/>
+      <c r="K43" s="37"/>
+      <c r="L43" s="37"/>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" s="43">
         <v>1</v>
       </c>
-      <c r="B43" s="46" t="s">
+      <c r="B44" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="39"/>
-      <c r="F43" s="68"/>
-      <c r="G43" s="68"/>
-      <c r="H43" s="68"/>
-      <c r="I43" s="34"/>
-      <c r="J43" s="36"/>
-      <c r="K43" s="36"/>
-      <c r="L43" s="36"/>
-      <c r="M43" s="35"/>
-    </row>
-    <row r="44" spans="1:13">
-      <c r="A44" s="51">
+      <c r="C44" s="32"/>
+      <c r="D44" s="32"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="58"/>
+      <c r="G44" s="58"/>
+      <c r="H44" s="58"/>
+      <c r="J44"/>
+      <c r="K44"/>
+      <c r="L44"/>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" s="43">
         <v>2</v>
       </c>
-      <c r="B44" s="46" t="s">
+      <c r="B45" s="38" t="s">
         <v>127</v>
       </c>
-      <c r="C44" s="40"/>
-      <c r="D44" s="40"/>
-      <c r="E44" s="41"/>
-      <c r="F44" s="68"/>
-      <c r="G44" s="68"/>
-      <c r="H44" s="68"/>
-      <c r="I44" s="34"/>
-      <c r="J44" s="36"/>
-      <c r="K44" s="36"/>
-      <c r="L44" s="36"/>
-      <c r="M44" s="35"/>
-    </row>
-    <row r="45" spans="1:13">
-      <c r="A45" s="52"/>
-      <c r="B45" s="48"/>
-      <c r="C45" s="49"/>
-      <c r="D45" s="49"/>
-      <c r="E45" s="50"/>
-      <c r="F45" s="68"/>
-      <c r="G45" s="68"/>
-      <c r="H45" s="68"/>
-      <c r="I45" s="34"/>
-      <c r="J45" s="36"/>
-      <c r="K45" s="36"/>
-      <c r="L45" s="36"/>
-      <c r="M45" s="35"/>
-    </row>
-    <row r="46" spans="1:13">
-      <c r="A46" s="13"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
-      <c r="J46" s="13"/>
-    </row>
-    <row r="47" spans="1:13">
-      <c r="A47" s="30" t="s">
+      <c r="C45" s="34"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="58"/>
+      <c r="G45" s="58"/>
+      <c r="H45" s="58"/>
+      <c r="J45"/>
+      <c r="K45"/>
+      <c r="L45"/>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" s="44"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="41"/>
+      <c r="E46" s="42"/>
+      <c r="F46" s="58"/>
+      <c r="G46" s="58"/>
+      <c r="H46" s="58"/>
+      <c r="J46"/>
+      <c r="K46"/>
+      <c r="L46"/>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47"/>
+      <c r="B47"/>
+      <c r="C47"/>
+      <c r="D47"/>
+      <c r="E47"/>
+      <c r="F47"/>
+      <c r="G47"/>
+      <c r="H47"/>
+      <c r="I47"/>
+      <c r="J47"/>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="B47" s="31"/>
-      <c r="C47" s="31"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="81"/>
-      <c r="F47" s="44" t="s">
+      <c r="B48" s="30"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="71"/>
+      <c r="F48" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G47" s="44"/>
-      <c r="H47" s="44"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="43"/>
-      <c r="K47" s="43"/>
-      <c r="L47" s="43"/>
-      <c r="M47" s="43"/>
-    </row>
-    <row r="48" spans="1:13">
-      <c r="A48" s="47" t="s">
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B48" s="42" t="s">
+      <c r="B49" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="C48" s="47" t="s">
+      <c r="C49" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="D48" s="42" t="s">
+      <c r="D49" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="E48" s="82"/>
-      <c r="F48" s="67"/>
-      <c r="G48" s="67"/>
-      <c r="H48" s="67"/>
-      <c r="I48" s="67"/>
-      <c r="J48" s="44"/>
-      <c r="K48" s="45"/>
-      <c r="L48" s="45"/>
-      <c r="M48" s="35"/>
-    </row>
-    <row r="49" spans="1:13">
-      <c r="A49" s="51">
+      <c r="E49" s="72"/>
+      <c r="F49" s="57"/>
+      <c r="G49" s="57"/>
+      <c r="H49" s="57"/>
+      <c r="I49" s="57"/>
+      <c r="K49" s="37"/>
+      <c r="L49" s="37"/>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" s="43">
         <v>1</v>
       </c>
-      <c r="B49" s="46" t="s">
+      <c r="B50" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="C49" s="95" t="s">
+      <c r="C50" s="85" t="s">
         <v>121</v>
       </c>
-      <c r="D49" s="38" t="s">
+      <c r="D50" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="E49" s="39"/>
-      <c r="F49" s="68"/>
-      <c r="G49" s="68"/>
-      <c r="H49" s="68"/>
-      <c r="I49" s="34"/>
-      <c r="J49" s="36"/>
-      <c r="K49" s="36"/>
-      <c r="L49" s="36"/>
-      <c r="M49" s="35"/>
-    </row>
-    <row r="50" spans="1:13">
-      <c r="A50" s="51">
+      <c r="E50" s="33"/>
+      <c r="F50" s="58"/>
+      <c r="G50" s="58"/>
+      <c r="H50" s="58"/>
+      <c r="J50"/>
+      <c r="K50"/>
+      <c r="L50"/>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" s="43">
         <v>2</v>
       </c>
-      <c r="B50" s="46" t="s">
+      <c r="B51" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="C50" s="96" t="s">
+      <c r="C51" s="86" t="s">
         <v>123</v>
       </c>
-      <c r="D50" s="40" t="s">
+      <c r="D51" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="E50" s="41"/>
-      <c r="F50" s="68"/>
-      <c r="G50" s="68"/>
-      <c r="H50" s="68"/>
-      <c r="I50" s="34"/>
-      <c r="J50" s="36"/>
-      <c r="K50" s="36"/>
-      <c r="L50" s="36"/>
-      <c r="M50" s="35"/>
-    </row>
-    <row r="51" spans="1:13">
-      <c r="A51" s="52"/>
-      <c r="B51" s="48"/>
-      <c r="C51" s="97"/>
-      <c r="D51" s="49"/>
-      <c r="E51" s="50"/>
-      <c r="F51" s="68"/>
-      <c r="G51" s="68"/>
-      <c r="H51" s="68"/>
-      <c r="I51" s="34"/>
-      <c r="J51" s="36"/>
-      <c r="K51" s="36"/>
-      <c r="L51" s="36"/>
-      <c r="M51" s="35"/>
+      <c r="E51" s="35"/>
+      <c r="F51" s="58"/>
+      <c r="G51" s="58"/>
+      <c r="H51" s="58"/>
+      <c r="J51"/>
+      <c r="K51"/>
+      <c r="L51"/>
     </row>
     <row r="52" spans="1:13">
-      <c r="A52" s="83"/>
-      <c r="B52" s="84"/>
-      <c r="C52" s="85"/>
-      <c r="D52" s="85"/>
-      <c r="E52" s="85"/>
-      <c r="F52" s="68"/>
-      <c r="G52" s="68"/>
-      <c r="H52" s="68"/>
-      <c r="I52" s="34"/>
-      <c r="J52" s="36"/>
-      <c r="K52" s="36"/>
-      <c r="L52" s="36"/>
-      <c r="M52" s="35"/>
+      <c r="A52" s="44"/>
+      <c r="B52" s="40"/>
+      <c r="C52" s="87"/>
+      <c r="D52" s="41"/>
+      <c r="E52" s="42"/>
+      <c r="F52" s="58"/>
+      <c r="G52" s="58"/>
+      <c r="H52" s="58"/>
+      <c r="J52"/>
+      <c r="K52"/>
+      <c r="L52"/>
     </row>
     <row r="53" spans="1:13">
-      <c r="A53" s="30" t="s">
+      <c r="A53" s="73"/>
+      <c r="B53" s="74"/>
+      <c r="C53" s="75"/>
+      <c r="D53" s="75"/>
+      <c r="E53" s="75"/>
+      <c r="F53" s="58"/>
+      <c r="G53" s="58"/>
+      <c r="H53" s="58"/>
+      <c r="J53"/>
+      <c r="K53"/>
+      <c r="L53"/>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="B53" s="31"/>
-      <c r="C53" s="31"/>
-      <c r="D53" s="31"/>
-      <c r="E53" s="81"/>
-      <c r="F53" s="44" t="s">
+      <c r="B54" s="30"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="71"/>
+      <c r="F54" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G53" s="44"/>
-      <c r="H53" s="44"/>
-      <c r="I53" s="44"/>
-      <c r="J53" s="43"/>
-      <c r="K53" s="43"/>
-      <c r="L53" s="43"/>
-      <c r="M53" s="43"/>
-    </row>
-    <row r="54" spans="1:13">
-      <c r="A54" s="47" t="s">
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B54" s="42" t="s">
+      <c r="B55" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C54" s="42"/>
-      <c r="D54" s="42"/>
-      <c r="E54" s="82"/>
-      <c r="F54" s="67" t="s">
+      <c r="C55" s="36"/>
+      <c r="D55" s="36"/>
+      <c r="E55" s="72"/>
+      <c r="F55" s="57" t="s">
         <v>112</v>
       </c>
-      <c r="G54" s="67"/>
-      <c r="H54" s="67"/>
-      <c r="I54" s="67"/>
-      <c r="J54" s="44"/>
-      <c r="K54" s="45"/>
-      <c r="L54" s="45"/>
-      <c r="M54" s="35"/>
-    </row>
-    <row r="55" spans="1:13">
-      <c r="A55" s="51"/>
-      <c r="B55" s="46"/>
-      <c r="C55" s="38"/>
-      <c r="D55" s="38"/>
-      <c r="E55" s="39"/>
-      <c r="F55" s="68"/>
-      <c r="G55" s="68"/>
-      <c r="H55" s="68"/>
-      <c r="I55" s="34"/>
-      <c r="J55" s="36"/>
-      <c r="K55" s="36"/>
-      <c r="L55" s="36"/>
-      <c r="M55" s="35"/>
+      <c r="G55" s="57"/>
+      <c r="H55" s="57"/>
+      <c r="I55" s="57"/>
+      <c r="K55" s="37"/>
+      <c r="L55" s="37"/>
     </row>
     <row r="56" spans="1:13">
-      <c r="A56" s="51"/>
-      <c r="B56" s="46"/>
-      <c r="C56" s="40"/>
-      <c r="D56" s="40"/>
-      <c r="E56" s="41"/>
-      <c r="F56" s="68"/>
-      <c r="G56" s="68"/>
-      <c r="H56" s="68"/>
-      <c r="I56" s="34"/>
-      <c r="J56" s="36"/>
-      <c r="K56" s="36"/>
-      <c r="L56" s="36"/>
-      <c r="M56" s="35"/>
+      <c r="A56" s="43"/>
+      <c r="B56" s="38"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="33"/>
+      <c r="F56" s="58"/>
+      <c r="G56" s="58"/>
+      <c r="H56" s="58"/>
+      <c r="J56"/>
+      <c r="K56"/>
+      <c r="L56"/>
     </row>
     <row r="57" spans="1:13">
-      <c r="A57" s="52"/>
-      <c r="B57" s="48"/>
-      <c r="C57" s="49"/>
-      <c r="D57" s="49"/>
-      <c r="E57" s="50"/>
-      <c r="F57" s="68"/>
-      <c r="G57" s="68"/>
-      <c r="H57" s="68"/>
-      <c r="I57" s="34"/>
-      <c r="J57" s="36"/>
-      <c r="K57" s="36"/>
-      <c r="L57" s="36"/>
-      <c r="M57" s="35"/>
+      <c r="A57" s="43"/>
+      <c r="B57" s="38"/>
+      <c r="C57" s="34"/>
+      <c r="D57" s="34"/>
+      <c r="E57" s="35"/>
+      <c r="F57" s="58"/>
+      <c r="G57" s="58"/>
+      <c r="H57" s="58"/>
+      <c r="J57"/>
+      <c r="K57"/>
+      <c r="L57"/>
     </row>
     <row r="58" spans="1:13">
-      <c r="A58" s="13"/>
-      <c r="B58" s="13"/>
-      <c r="C58" s="13"/>
-      <c r="D58" s="13"/>
-      <c r="E58" s="13"/>
-      <c r="F58" s="13"/>
-      <c r="G58" s="13"/>
-      <c r="H58" s="13"/>
-      <c r="I58" s="13"/>
-      <c r="J58" s="13"/>
+      <c r="A58" s="44"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="41"/>
+      <c r="D58" s="41"/>
+      <c r="E58" s="42"/>
+      <c r="F58" s="58"/>
+      <c r="G58" s="58"/>
+      <c r="H58" s="58"/>
+      <c r="J58"/>
+      <c r="K58"/>
+      <c r="L58"/>
     </row>
     <row r="59" spans="1:13">
-      <c r="A59" s="13"/>
-      <c r="B59" s="13" t="s">
+      <c r="A59"/>
+      <c r="B59"/>
+      <c r="C59"/>
+      <c r="D59"/>
+      <c r="E59"/>
+      <c r="F59"/>
+      <c r="G59"/>
+      <c r="H59"/>
+      <c r="I59"/>
+      <c r="J59"/>
+    </row>
+    <row r="60" spans="1:13">
+      <c r="A60"/>
+      <c r="B60" t="s">
         <v>83</v>
       </c>
-      <c r="C59" s="13"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="13"/>
-      <c r="G59" s="13"/>
-      <c r="H59" s="13"/>
-      <c r="I59" s="13"/>
-      <c r="J59" s="13"/>
-    </row>
-    <row r="60" spans="1:13">
-      <c r="A60" s="3" t="s">
+      <c r="C60"/>
+      <c r="D60"/>
+      <c r="E60"/>
+      <c r="F60"/>
+      <c r="G60"/>
+      <c r="H60"/>
+      <c r="I60"/>
+      <c r="J60"/>
+    </row>
+    <row r="61" spans="1:13">
+      <c r="A61" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B60" s="14"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="14"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="14"/>
-      <c r="I60" s="14"/>
-      <c r="J60" s="14"/>
-      <c r="K60" s="14"/>
-      <c r="L60" s="6"/>
-      <c r="M60" s="15"/>
-    </row>
-    <row r="61" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A61" s="101" t="s">
+      <c r="B61" s="13"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="13"/>
+      <c r="K61" s="13"/>
+      <c r="L61" s="6"/>
+      <c r="M61" s="14"/>
+    </row>
+    <row r="62" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A62" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="B61" s="101" t="s">
+      <c r="B62" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="C61" s="100" t="s">
+      <c r="C62" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="D61" s="100" t="s">
+      <c r="D62" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="E61" s="100" t="s">
+      <c r="E62" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="F61" s="104" t="s">
+      <c r="F62" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="G61" s="104" t="s">
+      <c r="G62" s="95" t="s">
         <v>16</v>
       </c>
-      <c r="H61" s="102" t="s">
+      <c r="H62" s="103" t="s">
         <v>115</v>
       </c>
-      <c r="I61" s="100" t="s">
+      <c r="I62" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="J61" s="100"/>
-      <c r="K61" s="16"/>
-      <c r="L61" s="17"/>
-      <c r="M61" s="9"/>
-    </row>
-    <row r="62" spans="1:13">
-      <c r="A62" s="101"/>
-      <c r="B62" s="101"/>
-      <c r="C62" s="100"/>
-      <c r="D62" s="100"/>
-      <c r="E62" s="100"/>
-      <c r="F62" s="105"/>
-      <c r="G62" s="105"/>
-      <c r="H62" s="103"/>
-      <c r="I62" s="100"/>
-      <c r="J62" s="100"/>
-      <c r="K62" s="18"/>
-      <c r="L62" s="29"/>
-      <c r="M62" s="15"/>
+      <c r="J62" s="94"/>
+      <c r="K62" s="15"/>
+      <c r="L62" s="16"/>
+      <c r="M62" s="9"/>
     </row>
     <row r="63" spans="1:13">
-      <c r="A63" s="19">
+      <c r="A63" s="97"/>
+      <c r="B63" s="97"/>
+      <c r="C63" s="94"/>
+      <c r="D63" s="94"/>
+      <c r="E63" s="94"/>
+      <c r="F63" s="96"/>
+      <c r="G63" s="96"/>
+      <c r="H63" s="104"/>
+      <c r="I63" s="94"/>
+      <c r="J63" s="94"/>
+      <c r="K63" s="17"/>
+      <c r="L63" s="28"/>
+      <c r="M63" s="14"/>
+    </row>
+    <row r="64" spans="1:13">
+      <c r="A64" s="18">
         <v>1</v>
       </c>
-      <c r="B63" s="71" t="s">
+      <c r="B64" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="C63" s="78" t="s">
+      <c r="C64" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="D63" s="20"/>
-      <c r="E63" s="20" t="s">
+      <c r="D64" s="19"/>
+      <c r="E64" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F63" s="20" t="s">
+      <c r="F64" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G63" s="69"/>
-      <c r="H63" s="69"/>
-      <c r="I63" s="20" t="s">
+      <c r="G64" s="59"/>
+      <c r="H64" s="59"/>
+      <c r="I64" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="J63" s="21"/>
-      <c r="K63" s="21"/>
-      <c r="L63" s="28"/>
-      <c r="M63" s="15"/>
-    </row>
-    <row r="64" spans="1:13">
-      <c r="A64" s="19">
-        <f>A63+1</f>
+      <c r="J64" s="20"/>
+      <c r="K64" s="20"/>
+      <c r="L64" s="27"/>
+      <c r="M64" s="14"/>
+    </row>
+    <row r="65" spans="1:13">
+      <c r="A65" s="18">
+        <f>A64+1</f>
         <v>2</v>
       </c>
-      <c r="B64" s="71" t="s">
+      <c r="B65" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="C64" s="78" t="s">
+      <c r="C65" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="D64" s="20"/>
-      <c r="E64" s="20" t="b">
+      <c r="D65" s="19"/>
+      <c r="E65" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="F64" s="20"/>
-      <c r="G64" s="69"/>
-      <c r="H64" s="69"/>
-      <c r="I64" s="20" t="s">
+      <c r="F65" s="19"/>
+      <c r="G65" s="59"/>
+      <c r="H65" s="59"/>
+      <c r="I65" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="J64" s="21"/>
-      <c r="K64" s="21"/>
-      <c r="L64" s="28"/>
-      <c r="M64" s="15"/>
-    </row>
-    <row r="65" spans="1:13">
-      <c r="A65" s="19">
-        <f t="shared" ref="A65:A79" si="0">A64+1</f>
+      <c r="J65" s="20"/>
+      <c r="K65" s="20"/>
+      <c r="L65" s="27"/>
+      <c r="M65" s="14"/>
+    </row>
+    <row r="66" spans="1:13">
+      <c r="A66" s="18">
+        <f t="shared" ref="A66:A80" si="0">A65+1</f>
         <v>3</v>
       </c>
-      <c r="B65" s="72" t="s">
+      <c r="B66" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="C65" s="79" t="s">
+      <c r="C66" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="D65" s="20" t="s">
+      <c r="D66" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="E65" s="20"/>
-      <c r="F65" s="20"/>
-      <c r="G65" s="69" t="s">
+      <c r="E66" s="19"/>
+      <c r="F66" s="19"/>
+      <c r="G66" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="H65" s="69"/>
-      <c r="I65" s="20" t="s">
+      <c r="H66" s="59"/>
+      <c r="I66" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="J65" s="21"/>
-      <c r="K65" s="21"/>
-      <c r="L65" s="22"/>
-      <c r="M65" s="15"/>
-    </row>
-    <row r="66" spans="1:13">
-      <c r="A66" s="19">
+      <c r="J66" s="20"/>
+      <c r="K66" s="20"/>
+      <c r="L66" s="21"/>
+      <c r="M66" s="14"/>
+    </row>
+    <row r="67" spans="1:13">
+      <c r="A67" s="18">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B66" s="73" t="s">
+      <c r="B67" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="C66" s="80" t="s">
+      <c r="C67" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="D66" s="20"/>
-      <c r="E66" s="20"/>
-      <c r="F66" s="20"/>
-      <c r="G66" s="69" t="s">
+      <c r="D67" s="19"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="19"/>
+      <c r="G67" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="H66" s="69"/>
-      <c r="I66" s="20" t="s">
+      <c r="H67" s="59"/>
+      <c r="I67" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="J66" s="21"/>
-      <c r="K66" s="21"/>
-      <c r="L66" s="22"/>
-      <c r="M66" s="15"/>
-    </row>
-    <row r="67" spans="1:13">
-      <c r="A67" s="19">
+      <c r="J67" s="20"/>
+      <c r="K67" s="20"/>
+      <c r="L67" s="21"/>
+      <c r="M67" s="14"/>
+    </row>
+    <row r="68" spans="1:13">
+      <c r="A68" s="18">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B67" s="73" t="s">
+      <c r="B68" s="63" t="s">
         <v>116</v>
       </c>
-      <c r="C67" s="80" t="s">
+      <c r="C68" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="D67" s="20"/>
-      <c r="E67" s="20"/>
-      <c r="F67" s="20"/>
-      <c r="G67" s="69" t="s">
+      <c r="D68" s="19"/>
+      <c r="E68" s="19"/>
+      <c r="F68" s="19"/>
+      <c r="G68" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="H67" s="69" t="s">
+      <c r="H68" s="59" t="s">
         <v>116</v>
       </c>
-      <c r="I67" s="20" t="s">
+      <c r="I68" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="J67" s="21"/>
-      <c r="K67" s="21"/>
-      <c r="L67" s="22"/>
-      <c r="M67" s="15"/>
-    </row>
-    <row r="68" spans="1:13">
-      <c r="A68" s="19">
+      <c r="J68" s="20"/>
+      <c r="K68" s="20"/>
+      <c r="L68" s="21"/>
+      <c r="M68" s="14"/>
+    </row>
+    <row r="69" spans="1:13">
+      <c r="A69" s="18">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B68" s="73"/>
-      <c r="C68" s="80"/>
-      <c r="D68" s="74"/>
-      <c r="E68" s="74"/>
-      <c r="F68" s="74"/>
-      <c r="G68" s="75"/>
-      <c r="H68" s="75"/>
-      <c r="I68" s="74"/>
-      <c r="J68" s="76"/>
-      <c r="K68" s="76"/>
-      <c r="L68" s="77"/>
-      <c r="M68" s="15"/>
-    </row>
-    <row r="69" spans="1:13">
-      <c r="A69" s="19">
+      <c r="B69" s="63"/>
+      <c r="C69" s="70"/>
+      <c r="D69" s="64"/>
+      <c r="E69" s="64"/>
+      <c r="F69" s="64"/>
+      <c r="G69" s="65"/>
+      <c r="H69" s="65"/>
+      <c r="I69" s="64"/>
+      <c r="J69" s="66"/>
+      <c r="K69" s="66"/>
+      <c r="L69" s="67"/>
+      <c r="M69" s="14"/>
+    </row>
+    <row r="70" spans="1:13">
+      <c r="A70" s="18">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B69" s="73"/>
-      <c r="C69" s="80"/>
-      <c r="D69" s="20"/>
-      <c r="E69" s="20"/>
-      <c r="F69" s="20"/>
-      <c r="G69" s="69"/>
-      <c r="H69" s="69"/>
-      <c r="I69" s="20"/>
-      <c r="J69" s="21"/>
-      <c r="K69" s="21"/>
-      <c r="L69" s="22"/>
-      <c r="M69" s="15"/>
-    </row>
-    <row r="70" spans="1:13">
-      <c r="A70" s="19">
+      <c r="B70" s="63"/>
+      <c r="C70" s="70"/>
+      <c r="D70" s="19"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="19"/>
+      <c r="G70" s="59"/>
+      <c r="H70" s="59"/>
+      <c r="I70" s="19"/>
+      <c r="J70" s="20"/>
+      <c r="K70" s="20"/>
+      <c r="L70" s="21"/>
+      <c r="M70" s="14"/>
+    </row>
+    <row r="71" spans="1:13">
+      <c r="A71" s="18">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B70" s="73"/>
-      <c r="C70" s="80"/>
-      <c r="D70" s="74"/>
-      <c r="E70" s="74"/>
-      <c r="F70" s="74"/>
-      <c r="G70" s="75"/>
-      <c r="H70" s="75"/>
-      <c r="I70" s="74"/>
-      <c r="J70" s="76"/>
-      <c r="K70" s="76"/>
-      <c r="L70" s="77"/>
-      <c r="M70" s="15"/>
-    </row>
-    <row r="71" spans="1:13">
-      <c r="A71" s="19">
+      <c r="B71" s="63"/>
+      <c r="C71" s="70"/>
+      <c r="D71" s="64"/>
+      <c r="E71" s="64"/>
+      <c r="F71" s="64"/>
+      <c r="G71" s="65"/>
+      <c r="H71" s="65"/>
+      <c r="I71" s="64"/>
+      <c r="J71" s="66"/>
+      <c r="K71" s="66"/>
+      <c r="L71" s="67"/>
+      <c r="M71" s="14"/>
+    </row>
+    <row r="72" spans="1:13">
+      <c r="A72" s="18">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B71" s="73"/>
-      <c r="C71" s="80"/>
-      <c r="D71" s="74"/>
-      <c r="E71" s="74"/>
-      <c r="F71" s="74"/>
-      <c r="G71" s="75"/>
-      <c r="H71" s="75"/>
-      <c r="I71" s="74"/>
-      <c r="J71" s="76"/>
-      <c r="K71" s="76"/>
-      <c r="L71" s="77"/>
-      <c r="M71" s="15"/>
-    </row>
-    <row r="72" spans="1:13">
-      <c r="A72" s="19">
+      <c r="B72" s="63"/>
+      <c r="C72" s="70"/>
+      <c r="D72" s="64"/>
+      <c r="E72" s="64"/>
+      <c r="F72" s="64"/>
+      <c r="G72" s="65"/>
+      <c r="H72" s="65"/>
+      <c r="I72" s="64"/>
+      <c r="J72" s="66"/>
+      <c r="K72" s="66"/>
+      <c r="L72" s="67"/>
+      <c r="M72" s="14"/>
+    </row>
+    <row r="73" spans="1:13">
+      <c r="A73" s="18">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B72" s="73"/>
-      <c r="C72" s="80"/>
-      <c r="D72" s="20"/>
-      <c r="E72" s="20"/>
-      <c r="F72" s="20"/>
-      <c r="G72" s="69"/>
-      <c r="H72" s="69"/>
-      <c r="I72" s="20"/>
-      <c r="J72" s="21"/>
-      <c r="K72" s="21"/>
-      <c r="L72" s="22"/>
-      <c r="M72" s="15"/>
-    </row>
-    <row r="73" spans="1:13">
-      <c r="A73" s="19">
+      <c r="B73" s="63"/>
+      <c r="C73" s="70"/>
+      <c r="D73" s="19"/>
+      <c r="E73" s="19"/>
+      <c r="F73" s="19"/>
+      <c r="G73" s="59"/>
+      <c r="H73" s="59"/>
+      <c r="I73" s="19"/>
+      <c r="J73" s="20"/>
+      <c r="K73" s="20"/>
+      <c r="L73" s="21"/>
+      <c r="M73" s="14"/>
+    </row>
+    <row r="74" spans="1:13">
+      <c r="A74" s="18">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B73" s="73"/>
-      <c r="C73" s="80"/>
-      <c r="D73" s="74"/>
-      <c r="E73" s="74"/>
-      <c r="F73" s="74"/>
-      <c r="G73" s="75"/>
-      <c r="H73" s="75"/>
-      <c r="I73" s="74"/>
-      <c r="J73" s="76"/>
-      <c r="K73" s="76"/>
-      <c r="L73" s="77"/>
-      <c r="M73" s="15"/>
-    </row>
-    <row r="74" spans="1:13">
-      <c r="A74" s="19">
+      <c r="B74" s="63"/>
+      <c r="C74" s="70"/>
+      <c r="D74" s="64"/>
+      <c r="E74" s="64"/>
+      <c r="F74" s="64"/>
+      <c r="G74" s="65"/>
+      <c r="H74" s="65"/>
+      <c r="I74" s="64"/>
+      <c r="J74" s="66"/>
+      <c r="K74" s="66"/>
+      <c r="L74" s="67"/>
+      <c r="M74" s="14"/>
+    </row>
+    <row r="75" spans="1:13">
+      <c r="A75" s="18">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B74" s="73"/>
-      <c r="C74" s="80"/>
-      <c r="D74" s="74"/>
-      <c r="E74" s="74"/>
-      <c r="F74" s="74"/>
-      <c r="G74" s="75"/>
-      <c r="H74" s="75"/>
-      <c r="I74" s="74"/>
-      <c r="J74" s="76"/>
-      <c r="K74" s="76"/>
-      <c r="L74" s="77"/>
-      <c r="M74" s="15"/>
-    </row>
-    <row r="75" spans="1:13">
-      <c r="A75" s="19">
+      <c r="B75" s="63"/>
+      <c r="C75" s="70"/>
+      <c r="D75" s="64"/>
+      <c r="E75" s="64"/>
+      <c r="F75" s="64"/>
+      <c r="G75" s="65"/>
+      <c r="H75" s="65"/>
+      <c r="I75" s="64"/>
+      <c r="J75" s="66"/>
+      <c r="K75" s="66"/>
+      <c r="L75" s="67"/>
+      <c r="M75" s="14"/>
+    </row>
+    <row r="76" spans="1:13">
+      <c r="A76" s="18">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B75" s="73"/>
-      <c r="C75" s="80"/>
-      <c r="D75" s="20"/>
-      <c r="E75" s="20"/>
-      <c r="F75" s="20"/>
-      <c r="G75" s="69"/>
-      <c r="H75" s="69"/>
-      <c r="I75" s="20"/>
-      <c r="J75" s="21"/>
-      <c r="K75" s="21"/>
-      <c r="L75" s="22"/>
-      <c r="M75" s="15"/>
-    </row>
-    <row r="76" spans="1:13">
-      <c r="A76" s="19">
+      <c r="B76" s="63"/>
+      <c r="C76" s="70"/>
+      <c r="D76" s="19"/>
+      <c r="E76" s="19"/>
+      <c r="F76" s="19"/>
+      <c r="G76" s="59"/>
+      <c r="H76" s="59"/>
+      <c r="I76" s="19"/>
+      <c r="J76" s="20"/>
+      <c r="K76" s="20"/>
+      <c r="L76" s="21"/>
+      <c r="M76" s="14"/>
+    </row>
+    <row r="77" spans="1:13">
+      <c r="A77" s="18">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B76" s="73"/>
-      <c r="C76" s="80"/>
-      <c r="D76" s="74"/>
-      <c r="E76" s="74"/>
-      <c r="F76" s="74"/>
-      <c r="G76" s="75"/>
-      <c r="H76" s="75"/>
-      <c r="I76" s="74"/>
-      <c r="J76" s="76"/>
-      <c r="K76" s="76"/>
-      <c r="L76" s="77"/>
-      <c r="M76" s="15"/>
-    </row>
-    <row r="77" spans="1:13">
-      <c r="A77" s="19">
+      <c r="B77" s="63"/>
+      <c r="C77" s="70"/>
+      <c r="D77" s="64"/>
+      <c r="E77" s="64"/>
+      <c r="F77" s="64"/>
+      <c r="G77" s="65"/>
+      <c r="H77" s="65"/>
+      <c r="I77" s="64"/>
+      <c r="J77" s="66"/>
+      <c r="K77" s="66"/>
+      <c r="L77" s="67"/>
+      <c r="M77" s="14"/>
+    </row>
+    <row r="78" spans="1:13">
+      <c r="A78" s="18">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B77" s="73"/>
-      <c r="C77" s="80"/>
-      <c r="D77" s="74"/>
-      <c r="E77" s="74"/>
-      <c r="F77" s="74"/>
-      <c r="G77" s="75"/>
-      <c r="H77" s="75"/>
-      <c r="I77" s="74"/>
-      <c r="J77" s="76"/>
-      <c r="K77" s="76"/>
-      <c r="L77" s="77"/>
-      <c r="M77" s="15"/>
-    </row>
-    <row r="78" spans="1:13">
-      <c r="A78" s="19">
+      <c r="B78" s="63"/>
+      <c r="C78" s="70"/>
+      <c r="D78" s="64"/>
+      <c r="E78" s="64"/>
+      <c r="F78" s="64"/>
+      <c r="G78" s="65"/>
+      <c r="H78" s="65"/>
+      <c r="I78" s="64"/>
+      <c r="J78" s="66"/>
+      <c r="K78" s="66"/>
+      <c r="L78" s="67"/>
+      <c r="M78" s="14"/>
+    </row>
+    <row r="79" spans="1:13">
+      <c r="A79" s="18">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B78" s="73"/>
-      <c r="C78" s="80"/>
-      <c r="D78" s="20"/>
-      <c r="E78" s="20"/>
-      <c r="F78" s="20"/>
-      <c r="G78" s="69"/>
-      <c r="H78" s="69"/>
-      <c r="I78" s="20"/>
-      <c r="J78" s="21"/>
-      <c r="K78" s="21"/>
-      <c r="L78" s="22"/>
-      <c r="M78" s="15"/>
-    </row>
-    <row r="79" spans="1:13">
-      <c r="A79" s="19">
+      <c r="B79" s="63"/>
+      <c r="C79" s="70"/>
+      <c r="D79" s="19"/>
+      <c r="E79" s="19"/>
+      <c r="F79" s="19"/>
+      <c r="G79" s="59"/>
+      <c r="H79" s="59"/>
+      <c r="I79" s="19"/>
+      <c r="J79" s="20"/>
+      <c r="K79" s="20"/>
+      <c r="L79" s="21"/>
+      <c r="M79" s="14"/>
+    </row>
+    <row r="80" spans="1:13">
+      <c r="A80" s="18">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B79" s="73"/>
-      <c r="C79" s="80"/>
-      <c r="D79" s="74"/>
-      <c r="E79" s="74"/>
-      <c r="F79" s="74"/>
-      <c r="G79" s="75"/>
-      <c r="H79" s="75"/>
-      <c r="I79" s="74"/>
-      <c r="J79" s="76"/>
-      <c r="K79" s="76"/>
-      <c r="L79" s="77"/>
-      <c r="M79" s="15"/>
-    </row>
-    <row r="80" spans="1:13">
-      <c r="A80" s="23"/>
-      <c r="B80" s="24"/>
-      <c r="C80" s="25"/>
-      <c r="D80" s="25"/>
-      <c r="E80" s="25"/>
-      <c r="F80" s="25"/>
-      <c r="G80" s="70"/>
-      <c r="H80" s="70"/>
-      <c r="I80" s="25"/>
-      <c r="J80" s="26"/>
-      <c r="K80" s="26"/>
-      <c r="L80" s="27"/>
-      <c r="M80" s="15"/>
-    </row>
-    <row r="82" spans="1:13">
-      <c r="A82" s="30" t="s">
+      <c r="B80" s="63"/>
+      <c r="C80" s="70"/>
+      <c r="D80" s="64"/>
+      <c r="E80" s="64"/>
+      <c r="F80" s="64"/>
+      <c r="G80" s="65"/>
+      <c r="H80" s="65"/>
+      <c r="I80" s="64"/>
+      <c r="J80" s="66"/>
+      <c r="K80" s="66"/>
+      <c r="L80" s="67"/>
+      <c r="M80" s="14"/>
+    </row>
+    <row r="81" spans="1:13">
+      <c r="A81" s="22"/>
+      <c r="B81" s="23"/>
+      <c r="C81" s="24"/>
+      <c r="D81" s="24"/>
+      <c r="E81" s="24"/>
+      <c r="F81" s="24"/>
+      <c r="G81" s="60"/>
+      <c r="H81" s="60"/>
+      <c r="I81" s="24"/>
+      <c r="J81" s="25"/>
+      <c r="K81" s="25"/>
+      <c r="L81" s="26"/>
+      <c r="M81" s="14"/>
+    </row>
+    <row r="83" spans="1:13">
+      <c r="A83" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="B82" s="31"/>
-      <c r="C82" s="31"/>
-      <c r="D82" s="31"/>
-      <c r="E82" s="81"/>
-      <c r="F82" s="44" t="s">
+      <c r="B83" s="30"/>
+      <c r="C83" s="30"/>
+      <c r="D83" s="30"/>
+      <c r="E83" s="71"/>
+      <c r="F83" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G82" s="44"/>
-      <c r="H82" s="44"/>
-      <c r="I82" s="44"/>
-      <c r="J82" s="43"/>
-      <c r="K82" s="43"/>
-      <c r="L82" s="43"/>
-      <c r="M82" s="43"/>
-    </row>
-    <row r="83" spans="1:13">
-      <c r="A83" s="47" t="s">
+    </row>
+    <row r="84" spans="1:13">
+      <c r="A84" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B83" s="42" t="s">
+      <c r="B84" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C83" s="42"/>
-      <c r="D83" s="42"/>
-      <c r="E83" s="82"/>
-      <c r="F83" s="67"/>
-      <c r="G83" s="67"/>
-      <c r="H83" s="67"/>
-      <c r="I83" s="67"/>
-      <c r="J83" s="44"/>
-      <c r="K83" s="45"/>
-      <c r="L83" s="45"/>
-      <c r="M83" s="35"/>
-    </row>
-    <row r="84" spans="1:13">
-      <c r="A84" s="51"/>
-      <c r="B84" s="46"/>
-      <c r="C84" s="38"/>
-      <c r="D84" s="38"/>
-      <c r="E84" s="39"/>
-      <c r="F84" s="68"/>
-      <c r="G84" s="68"/>
-      <c r="H84" s="68"/>
-      <c r="I84" s="34"/>
-      <c r="J84" s="36"/>
-      <c r="K84" s="36"/>
-      <c r="L84" s="36"/>
-      <c r="M84" s="35"/>
+      <c r="C84" s="36"/>
+      <c r="D84" s="36"/>
+      <c r="E84" s="72"/>
+      <c r="F84" s="57"/>
+      <c r="G84" s="57"/>
+      <c r="H84" s="57"/>
+      <c r="I84" s="57"/>
+      <c r="K84" s="37"/>
+      <c r="L84" s="37"/>
     </row>
     <row r="85" spans="1:13">
-      <c r="A85" s="51"/>
-      <c r="B85" s="46"/>
-      <c r="C85" s="40"/>
-      <c r="D85" s="40"/>
-      <c r="E85" s="41"/>
-      <c r="F85" s="68"/>
-      <c r="G85" s="68"/>
-      <c r="H85" s="68"/>
-      <c r="I85" s="34"/>
-      <c r="J85" s="36"/>
-      <c r="K85" s="36"/>
-      <c r="L85" s="36"/>
-      <c r="M85" s="35"/>
+      <c r="A85" s="43"/>
+      <c r="B85" s="38"/>
+      <c r="C85" s="32"/>
+      <c r="D85" s="32"/>
+      <c r="E85" s="33"/>
+      <c r="F85" s="58"/>
+      <c r="G85" s="58"/>
+      <c r="H85" s="58"/>
+      <c r="J85"/>
+      <c r="K85"/>
+      <c r="L85"/>
     </row>
     <row r="86" spans="1:13">
-      <c r="A86" s="52"/>
-      <c r="B86" s="48"/>
-      <c r="C86" s="49"/>
-      <c r="D86" s="49"/>
-      <c r="E86" s="50"/>
-      <c r="F86" s="68"/>
-      <c r="G86" s="68"/>
-      <c r="H86" s="68"/>
-      <c r="I86" s="34"/>
-      <c r="J86" s="36"/>
-      <c r="K86" s="36"/>
-      <c r="L86" s="36"/>
-      <c r="M86" s="35"/>
+      <c r="A86" s="43"/>
+      <c r="B86" s="38"/>
+      <c r="C86" s="34"/>
+      <c r="D86" s="34"/>
+      <c r="E86" s="35"/>
+      <c r="F86" s="58"/>
+      <c r="G86" s="58"/>
+      <c r="H86" s="58"/>
+      <c r="J86"/>
+      <c r="K86"/>
+      <c r="L86"/>
     </row>
     <row r="87" spans="1:13">
-      <c r="A87" s="13"/>
-      <c r="B87" s="13"/>
-      <c r="C87" s="13"/>
-      <c r="D87" s="13"/>
-      <c r="E87" s="13"/>
-      <c r="F87" s="13"/>
-      <c r="G87" s="13"/>
-      <c r="H87" s="13"/>
-      <c r="I87" s="13"/>
-      <c r="J87" s="13"/>
+      <c r="A87" s="44"/>
+      <c r="B87" s="40"/>
+      <c r="C87" s="41"/>
+      <c r="D87" s="41"/>
+      <c r="E87" s="42"/>
+      <c r="F87" s="58"/>
+      <c r="G87" s="58"/>
+      <c r="H87" s="58"/>
+      <c r="J87"/>
+      <c r="K87"/>
+      <c r="L87"/>
     </row>
     <row r="88" spans="1:13">
-      <c r="A88" s="13"/>
-      <c r="B88" s="13" t="s">
+      <c r="A88"/>
+      <c r="B88"/>
+      <c r="C88"/>
+      <c r="D88"/>
+      <c r="E88"/>
+      <c r="F88"/>
+      <c r="G88"/>
+      <c r="H88"/>
+      <c r="I88"/>
+      <c r="J88"/>
+    </row>
+    <row r="89" spans="1:13">
+      <c r="A89"/>
+      <c r="B89" t="s">
         <v>94</v>
       </c>
-      <c r="C88" s="13"/>
-      <c r="D88" s="13"/>
-      <c r="E88" s="13"/>
-      <c r="F88" s="13"/>
-      <c r="G88" s="13"/>
-      <c r="H88" s="13"/>
-      <c r="I88" s="13"/>
-      <c r="J88" s="13"/>
-    </row>
-    <row r="89" spans="1:13">
-      <c r="A89" s="3" t="s">
+      <c r="C89"/>
+      <c r="D89"/>
+      <c r="E89"/>
+      <c r="F89"/>
+      <c r="G89"/>
+      <c r="H89"/>
+      <c r="I89"/>
+      <c r="J89"/>
+    </row>
+    <row r="90" spans="1:13">
+      <c r="A90" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B89" s="14"/>
-      <c r="C89" s="14"/>
-      <c r="D89" s="14"/>
-      <c r="E89" s="14"/>
-      <c r="F89" s="14"/>
-      <c r="G89" s="14"/>
-      <c r="H89" s="14"/>
-      <c r="I89" s="14"/>
-      <c r="J89" s="14"/>
-      <c r="K89" s="14"/>
-      <c r="L89" s="6"/>
-      <c r="M89" s="15"/>
-    </row>
-    <row r="90" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A90" s="101" t="s">
+      <c r="B90" s="13"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="13"/>
+      <c r="E90" s="13"/>
+      <c r="F90" s="13"/>
+      <c r="G90" s="13"/>
+      <c r="H90" s="13"/>
+      <c r="I90" s="13"/>
+      <c r="J90" s="13"/>
+      <c r="K90" s="13"/>
+      <c r="L90" s="6"/>
+      <c r="M90" s="14"/>
+    </row>
+    <row r="91" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A91" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="B90" s="101" t="s">
+      <c r="B91" s="97" t="s">
         <v>93</v>
       </c>
-      <c r="C90" s="100" t="s">
+      <c r="C91" s="94" t="s">
         <v>95</v>
       </c>
-      <c r="D90" s="100" t="s">
+      <c r="D91" s="94" t="s">
         <v>96</v>
       </c>
-      <c r="E90" s="100" t="s">
+      <c r="E91" s="94" t="s">
         <v>86</v>
       </c>
-      <c r="F90" s="111"/>
-      <c r="G90" s="111"/>
-      <c r="H90" s="111"/>
-      <c r="I90" s="113"/>
-      <c r="J90" s="100"/>
-      <c r="K90" s="16"/>
-      <c r="L90" s="17"/>
-      <c r="M90" s="9"/>
-    </row>
-    <row r="91" spans="1:13">
-      <c r="A91" s="101"/>
-      <c r="B91" s="101"/>
-      <c r="C91" s="100"/>
-      <c r="D91" s="100"/>
-      <c r="E91" s="100"/>
-      <c r="F91" s="112"/>
-      <c r="G91" s="112"/>
-      <c r="H91" s="112"/>
-      <c r="I91" s="113"/>
-      <c r="J91" s="100"/>
-      <c r="K91" s="18"/>
-      <c r="L91" s="29"/>
-      <c r="M91" s="15"/>
+      <c r="F91" s="91"/>
+      <c r="G91" s="91"/>
+      <c r="H91" s="91"/>
+      <c r="I91" s="93"/>
+      <c r="J91" s="94"/>
+      <c r="K91" s="15"/>
+      <c r="L91" s="16"/>
+      <c r="M91" s="9"/>
     </row>
     <row r="92" spans="1:13">
-      <c r="A92" s="19">
+      <c r="A92" s="97"/>
+      <c r="B92" s="97"/>
+      <c r="C92" s="94"/>
+      <c r="D92" s="94"/>
+      <c r="E92" s="94"/>
+      <c r="F92" s="92"/>
+      <c r="G92" s="92"/>
+      <c r="H92" s="92"/>
+      <c r="I92" s="93"/>
+      <c r="J92" s="94"/>
+      <c r="K92" s="17"/>
+      <c r="L92" s="28"/>
+      <c r="M92" s="14"/>
+    </row>
+    <row r="93" spans="1:13">
+      <c r="A93" s="18">
         <v>1</v>
       </c>
-      <c r="B92" s="71" t="s">
+      <c r="B93" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="C92" s="78" t="s">
+      <c r="C93" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="D92" s="20"/>
-      <c r="E92" s="20" t="s">
+      <c r="D93" s="19"/>
+      <c r="E93" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="F92" s="87"/>
-      <c r="G92" s="89"/>
-      <c r="H92" s="89"/>
-      <c r="I92" s="87"/>
-      <c r="J92" s="21"/>
-      <c r="K92" s="21"/>
-      <c r="L92" s="28"/>
-      <c r="M92" s="15"/>
-    </row>
-    <row r="93" spans="1:13">
-      <c r="A93" s="19">
-        <f>A92+1</f>
+      <c r="F93" s="77"/>
+      <c r="G93" s="79"/>
+      <c r="H93" s="79"/>
+      <c r="I93" s="77"/>
+      <c r="J93" s="20"/>
+      <c r="K93" s="20"/>
+      <c r="L93" s="27"/>
+      <c r="M93" s="14"/>
+    </row>
+    <row r="94" spans="1:13">
+      <c r="A94" s="18">
+        <f>A93+1</f>
         <v>2</v>
       </c>
-      <c r="B93" s="71" t="s">
+      <c r="B94" s="61" t="s">
         <v>98</v>
       </c>
-      <c r="C93" s="78" t="s">
+      <c r="C94" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="D93" s="20"/>
-      <c r="E93" s="20" t="s">
+      <c r="D94" s="19"/>
+      <c r="E94" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="F93" s="87"/>
-      <c r="G93" s="89"/>
-      <c r="H93" s="89"/>
-      <c r="I93" s="87"/>
-      <c r="J93" s="21"/>
-      <c r="K93" s="21"/>
-      <c r="L93" s="28"/>
-      <c r="M93" s="15"/>
-    </row>
-    <row r="94" spans="1:13">
-      <c r="A94" s="19">
-        <f t="shared" ref="A94:A98" si="1">A93+1</f>
+      <c r="F94" s="77"/>
+      <c r="G94" s="79"/>
+      <c r="H94" s="79"/>
+      <c r="I94" s="77"/>
+      <c r="J94" s="20"/>
+      <c r="K94" s="20"/>
+      <c r="L94" s="27"/>
+      <c r="M94" s="14"/>
+    </row>
+    <row r="95" spans="1:13">
+      <c r="A95" s="18">
+        <f t="shared" ref="A95:A99" si="1">A94+1</f>
         <v>3</v>
       </c>
-      <c r="B94" s="72" t="s">
+      <c r="B95" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="C94" s="79" t="s">
+      <c r="C95" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="D94" s="20" t="s">
+      <c r="D95" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="E94" s="20" t="s">
+      <c r="E95" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="F94" s="87"/>
-      <c r="G94" s="89"/>
-      <c r="H94" s="89"/>
-      <c r="I94" s="87"/>
-      <c r="J94" s="21"/>
-      <c r="K94" s="21"/>
-      <c r="L94" s="22"/>
-      <c r="M94" s="15"/>
-    </row>
-    <row r="95" spans="1:13">
-      <c r="A95" s="19">
+      <c r="F95" s="77"/>
+      <c r="G95" s="79"/>
+      <c r="H95" s="79"/>
+      <c r="I95" s="77"/>
+      <c r="J95" s="20"/>
+      <c r="K95" s="20"/>
+      <c r="L95" s="21"/>
+      <c r="M95" s="14"/>
+    </row>
+    <row r="96" spans="1:13">
+      <c r="A96" s="18">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B95" s="73"/>
-      <c r="C95" s="80"/>
-      <c r="D95" s="20"/>
-      <c r="E95" s="20"/>
-      <c r="F95" s="87"/>
-      <c r="G95" s="89"/>
-      <c r="H95" s="89"/>
-      <c r="I95" s="87"/>
-      <c r="J95" s="21"/>
-      <c r="K95" s="21"/>
-      <c r="L95" s="22"/>
-      <c r="M95" s="15"/>
-    </row>
-    <row r="96" spans="1:13">
-      <c r="A96" s="19">
+      <c r="B96" s="63"/>
+      <c r="C96" s="70"/>
+      <c r="D96" s="19"/>
+      <c r="E96" s="19"/>
+      <c r="F96" s="77"/>
+      <c r="G96" s="79"/>
+      <c r="H96" s="79"/>
+      <c r="I96" s="77"/>
+      <c r="J96" s="20"/>
+      <c r="K96" s="20"/>
+      <c r="L96" s="21"/>
+      <c r="M96" s="14"/>
+    </row>
+    <row r="97" spans="1:13">
+      <c r="A97" s="18">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B96" s="73"/>
-      <c r="C96" s="80"/>
-      <c r="D96" s="20"/>
-      <c r="E96" s="20"/>
-      <c r="F96" s="87"/>
-      <c r="G96" s="89"/>
-      <c r="H96" s="89"/>
-      <c r="I96" s="87"/>
-      <c r="J96" s="21"/>
-      <c r="K96" s="21"/>
-      <c r="L96" s="22"/>
-      <c r="M96" s="15"/>
-    </row>
-    <row r="97" spans="1:13">
-      <c r="A97" s="19">
+      <c r="B97" s="63"/>
+      <c r="C97" s="70"/>
+      <c r="D97" s="19"/>
+      <c r="E97" s="19"/>
+      <c r="F97" s="77"/>
+      <c r="G97" s="79"/>
+      <c r="H97" s="79"/>
+      <c r="I97" s="77"/>
+      <c r="J97" s="20"/>
+      <c r="K97" s="20"/>
+      <c r="L97" s="21"/>
+      <c r="M97" s="14"/>
+    </row>
+    <row r="98" spans="1:13">
+      <c r="A98" s="18">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B97" s="73"/>
-      <c r="C97" s="80"/>
-      <c r="D97" s="74"/>
-      <c r="E97" s="74"/>
-      <c r="F97" s="88"/>
-      <c r="G97" s="90"/>
-      <c r="H97" s="90"/>
-      <c r="I97" s="88"/>
-      <c r="J97" s="76"/>
-      <c r="K97" s="76"/>
-      <c r="L97" s="77"/>
-      <c r="M97" s="15"/>
-    </row>
-    <row r="98" spans="1:13">
-      <c r="A98" s="19">
+      <c r="B98" s="63"/>
+      <c r="C98" s="70"/>
+      <c r="D98" s="64"/>
+      <c r="E98" s="64"/>
+      <c r="F98" s="78"/>
+      <c r="G98" s="80"/>
+      <c r="H98" s="80"/>
+      <c r="I98" s="78"/>
+      <c r="J98" s="66"/>
+      <c r="K98" s="66"/>
+      <c r="L98" s="67"/>
+      <c r="M98" s="14"/>
+    </row>
+    <row r="99" spans="1:13">
+      <c r="A99" s="18">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B98" s="73"/>
-      <c r="C98" s="80"/>
-      <c r="D98" s="20"/>
-      <c r="E98" s="20"/>
-      <c r="F98" s="87"/>
-      <c r="G98" s="89"/>
-      <c r="H98" s="89"/>
-      <c r="I98" s="87"/>
-      <c r="J98" s="21"/>
-      <c r="K98" s="21"/>
-      <c r="L98" s="22"/>
-      <c r="M98" s="15"/>
+      <c r="B99" s="63"/>
+      <c r="C99" s="70"/>
+      <c r="D99" s="19"/>
+      <c r="E99" s="19"/>
+      <c r="F99" s="77"/>
+      <c r="G99" s="79"/>
+      <c r="H99" s="79"/>
+      <c r="I99" s="77"/>
+      <c r="J99" s="20"/>
+      <c r="K99" s="20"/>
+      <c r="L99" s="21"/>
+      <c r="M99" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="F90:F91"/>
-    <mergeCell ref="H90:H91"/>
-    <mergeCell ref="I90:J91"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="G90:G91"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="B90:B91"/>
-    <mergeCell ref="C90:C91"/>
-    <mergeCell ref="D90:D91"/>
-    <mergeCell ref="E90:E91"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="H62:H63"/>
+    <mergeCell ref="F62:F63"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="C14:E14"/>
-    <mergeCell ref="A25:B25"/>
     <mergeCell ref="A23:B23"/>
-    <mergeCell ref="I61:J62"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="E61:E62"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="H61:H62"/>
-    <mergeCell ref="F61:F62"/>
+    <mergeCell ref="F91:F92"/>
+    <mergeCell ref="H91:H92"/>
+    <mergeCell ref="I91:J92"/>
+    <mergeCell ref="G62:G63"/>
+    <mergeCell ref="G91:G92"/>
+    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="B91:B92"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="D91:D92"/>
+    <mergeCell ref="E91:E92"/>
     <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="I62:J63"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:B63"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E102:H102" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E103:H103" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25:C26" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C26:C27" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
       <formula1>adjustFiledName</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
       <formula1>componentKind</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F63:G80 C17:C22" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F64:G81 C17 C19:C23" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>yesNo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C24" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">
       <formula1>adjustFieldName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C49:C51" xr:uid="{BDE40890-40F7-4E41-B7E1-478CEBD85557}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C50:C52" xr:uid="{BDE40890-40F7-4E41-B7E1-478CEBD85557}">
       <formula1>httpdMethod</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18" xr:uid="{4BE0588A-3B8A-7B4F-B1CE-EF62180DE29A}">
+      <formula1>layoutType</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.59027777777777779" right="0.59027777777777779" top="0.59027777777777779" bottom="0.59027777777777779" header="0.51180555555555562" footer="0.11805555555555557"/>
@@ -4189,109 +4093,125 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="55" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" style="55" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="55" customWidth="1"/>
-    <col min="6" max="6" width="18.5" style="55" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="55" customWidth="1"/>
-    <col min="8" max="8" width="18.5" style="55" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="55" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" style="55" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.83203125" style="55" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" style="55" bestFit="1" customWidth="1"/>
-    <col min="13" max="253" width="8.83203125" style="55" customWidth="1"/>
-    <col min="254" max="16384" width="10.83203125" style="55"/>
+    <col min="1" max="3" width="8.83203125" style="47" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" style="47" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="47" customWidth="1"/>
+    <col min="6" max="6" width="18.5" style="47" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="47" customWidth="1"/>
+    <col min="8" max="8" width="18.5" style="47" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="47" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="47" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.83203125" style="47" customWidth="1"/>
+    <col min="14" max="14" width="14" style="47" customWidth="1"/>
+    <col min="15" max="253" width="8.83203125" style="47" customWidth="1"/>
+    <col min="254" max="16384" width="10.83203125" style="47"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="19">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:14" ht="19">
+      <c r="A1" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="54" t="s">
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="46" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="B3" s="56" t="s">
+      <c r="N1" s="45"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="B3" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="56" t="s">
+      <c r="F3" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="H3" s="56" t="s">
+      <c r="H3" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="56" t="s">
+      <c r="J3" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="56" t="s">
+      <c r="L3" s="48" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="B4" s="57" t="s">
+      <c r="N3" s="48" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="B4" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="91"/>
-      <c r="H4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="L4" s="58"/>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="B5" s="59" t="s">
+      <c r="F4" s="81"/>
+      <c r="H4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="N4" s="49"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="B5" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="60"/>
-      <c r="F5" s="92" t="s">
+      <c r="D5" s="52"/>
+      <c r="F5" s="82" t="s">
         <v>122</v>
       </c>
-      <c r="H5" s="60" t="s">
+      <c r="H5" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="60" t="s">
+      <c r="J5" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="60" t="s">
+      <c r="L5" s="52" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="B6" s="61"/>
-      <c r="F6" s="92" t="s">
+      <c r="N5" s="49" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="B6" s="53"/>
+      <c r="F6" s="82" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="F7" s="93" t="s">
+      <c r="N6" s="51" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="F7" s="83" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="F8" s="94" t="s">
+      <c r="N7" s="88" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="F8" s="84" t="s">
         <v>126</v>
       </c>
     </row>

</xml_diff>